<commit_message>
add classifiers and pretrained document_type_model
</commit_message>
<xml_diff>
--- a/tests/test.xlsx
+++ b/tests/test.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E39"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -464,16 +464,17 @@
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr">
         <is>
-          <t xml:space="preserve">EX-10.6 4 d826673dex106.htm EX-10.6
-Exhibit 10.6
-AMENDED AND RESTATED SHAREHOLDERS' AGREEMENT
-This Amended and Restated Shareholders' Agreement (this "Agreement"), among The Goldman Sachs Group, Inc., a Delaware corporation ("GS Inc."), and the Covered Persons (hereinafter defined) listed on Appendix A hereto, as such Appendix A may be amended from time to time pursuant to the provisions hereof.
+          <t xml:space="preserve">EX-10.14 4 orctf-ex1014_70.htm EX-10.14
+Exhibit 10.14
+COLLATERAL MANAGEMENT AGREEMENT
+This Agreement, dated as of December 16, 2020 (this "Agreement"), is entered into by and between Owl Rock Technology Financing 2020-1, an exempted company incorporated with limited liability under the laws of the Cayman Islands, with its registered office at the offices of Walkers Fiduciary Limited, Cayman Corporate Centre, 27 Hospital Road, George Town, Grand Cayman, KY1-9008, Cayman Islands (together with successors and assigns permitted hereunder, the "Issuer"), and Owl Rock Technology Advisors LLC ("Owl Rock Technology Advisors"), a Delaware limited liability company, with its principal offices located at 399 Park Avenue, 38th Floor, New York, NY 10022, as collateral manager (in such capacity, the "Collateral Manager"). Capitalized terms used and not otherwise defined herein have the meanings assigned to them in the Indenture.
 WITNESSETH:
-WHEREAS, the Covered Persons are beneficial owners of shares of Common Stock, par value $0.01 per share, of GS Inc. (the "Common Stock").
-WHEREAS, GS Inc. entered into the Shareholders' Agreement (hereinafter defined) in connection with the initial public offering of GS Inc. to address certain relationships among the parties thereto with respect to the voting and disposition of shares of Common Stock and various other matters, and to give to the Shareholders' Committee (hereinafter defined) the power to enforce their agreements with respect thereto.
-WHEREAS, the GS Inc. Board of Directors has determined that it is in the best interests of GS Inc. to maintain the firm's retention requirement applicable to Management Committee Members through a Board-level policy rather than through this Agreement.
-WHEREAS, the Shareholders' Committee and GS Inc. accordingly desire to amend the Shareholders' Agreement to remove the transfer restrictions previously set forth in Section 2.1 thereof and to amend other provisions of the Shareholders' Agreement to reflect such removal, in accordance with Section 7.2(h) thereof.
-NOW, THEREFORE, in consideration of the premises and of the mutual agreements, covenants and provisions herein contained, the parties hereto agree to amend and restate the Shareholders' Agreement in its entirety as follows:
+WHEREAS, the Issuer intends to issue Notes pursuant to an indenture dated as of December 16, 2020 (the "Indenture"), among the Issuer, Owl Rock Technology Financing 2020-1 LLC, as co-issuer of the Co-Issued Notes (the "Co-Issuer" and, together with the Issuer, the "Issuers"), and State Street Bank and Trust Company, as trustee (together with any successor trustee permitted under the Indenture, the "Trustee");
+WHEREAS, the Issuer intends to issue Preferred Shares pursuant to the Issuer's memorandum and articles of association and subject to the Fiscal Agency Agreement, dated as of the Closing Date (the "Fiscal Agency Agreement"), among the Fiscal Agent, the Share Registrar and the Issuer, as amended from time to time in accordance with the terms thereof; 
+WHEREAS, the Issuer intends to pledge certain Collateral Obligations, Eligible Investments and Cash (all as defined in the Indenture) and certain other assets (all as set forth in the Indenture) (collectively, the "Assets") to the Trustee as security for its obligations under the Indenture;
+WHEREAS, the Issuer wishes to enter into this Agreement, pursuant to which the Collateral Manager agrees to perform, on behalf of the Issuer, certain duties with respect to the Assets in the manner and on the terms set forth herein and to perform such additional duties as are consistent with the terms of this Agreement, the Indenture and the Collateral Administration Agreement; and
+WHEREAS, the Collateral Manager has the capacity to provide the services required hereby and is prepared to perform such services upon the terms and conditions set forth herein.
+NOW, THEREFORE, in consideration of the mutual agreements herein set forth, the parties hereto agree as follows:
 </t>
         </is>
       </c>
@@ -482,10 +483,33 @@
       <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B3" t="inlineStr"/>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
       <c r="C3" t="inlineStr"/>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr"/>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Definitions</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Terms used herein and not defined below or elsewhere herein shall have the meanings set forth in the Indenture.
+"Agreement" shall mean this Agreement, as amended from time to time.
+"Cause" shall have the meaning set forth in Section 14.
+"Collateral Manager Information" shall have the meaning ascribed to such term in the Offering Circular.
+"Collateral Manager Securities" shall mean any Securities owned by the Collateral Manager, an Affiliate thereof, or any account, fund, client or portfolio established and controlled by the Collateral Manager or an Affiliate thereof or for which the Collateral Manager or an Affiliate thereof acts as the investment adviser or with respect to which the Collateral Manager or an Affiliate thereof exercises discretionary control thereover.
+"Governing Instruments" shall mean the memorandum of association, articles of association and by-laws, if applicable, in the case of a corporation, the partnership agreement, in the case of a partnership, the limited liability company agreement and certificate of formation, in the case of a limited liability company or the trust agreement and (if applicable) certificate of trust, in the case of a trust.
+"Notice of Removal" shall have the meaning set forth in Section 14.
+"Offering Circular" shall mean the final Offering Circular with respect to the Notes.
+"Related Person" shall mean with respect to any Person, the owners of the equity interests therein, directors, officers, employees, managers, agents and professional advisors thereof.
+"Responsible Officer" shall mean, with respect to any Person, any duly authorized director, officer or manager of such Person with direct responsibility for the administration of the applicable agreement and also, with respect to a particular matter, any other duly authorized director, officer or manager of such Person to whom such matter is referred because of such director's, officer's or manager's knowledge of and familiarity with the particular subject. Each party may receive and accept a certification of the authority of any other party as conclusive evidence of the authority of any Person to act, and such certification may be considered as in full force and effect until receipt by such other party of written notice to the contrary.
+"Termination Notice" shall have the meaning set forth in Section 14.
+</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -493,15 +517,32 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>I</t>
+          <t>2</t>
         </is>
       </c>
       <c r="C4" t="inlineStr"/>
-      <c r="D4" t="inlineStr"/>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>General Duties and Authorization of the Collateral Manager</t>
+        </is>
+      </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t xml:space="preserve">ARTICLE I
-DEFINITIONS AND OTHER MATTERS
+          <t xml:space="preserve">The Collateral Manager shall provide services to the Issuer as follows:
+(a)Subject to and in accordance with the applicable terms of the Indenture and the terms of this Agreement, the Collateral Manager agrees to, and is appointed and authorized by
+the Issuer to (i) select the Assets to be acquired, sold, terminated, tendered or otherwise disposed of by the Issuer, (ii) invest and reinvest the Assets subject to the Investment Criteria and other conditions and restrictions set forth in the Indenture, (iii) instruct the Trustee with respect to any acquisition, disposition or tender of, or Offer with respect to, any Assets received in respect thereof in the open market or otherwise by the Issuer, and (iv) perform all other tasks and take all other actions that any of the Indenture, the Collateral Administration Agreement or this Agreement specify are to be taken by the Collateral Manager (provided that the Collateral Manager will not be bound to follow any amendment or supplement to the Indenture unless it has consented thereto in accordance with the Indenture); and the Collateral Manager may, in its sole discretion, take any other action not inconsistent with an action that such agreements specify may be taken by the Collateral Manager.
+(b)The Collateral Manager shall monitor the Assets on behalf of the Issuer on an ongoing basis and will further agree to provide or cause to be provided to the Issuer all reports, schedules and other data reasonably available to the Collateral Manager that the Issuer is required to prepare and deliver or cause to be prepared and delivered under the Indenture, in such forms and containing such information required thereby, in reasonably sufficient time for such required reports, schedules and data to be reviewed and delivered by or on behalf of the Issuer to the parties entitled thereto under the Indenture. The obligation of the Collateral Manager to furnish such reports, schedules and other data is subject to the Collateral Manager's timely receipt of necessary information, reports, schedules and other data from the Person responsible for the delivery or preparation thereof (including without limitation, Obligors of the Collateral Obligations, the Rating Agency, the Trustee and the Collateral Administrator) and to any confidentiality restrictions with respect thereto. 
+(c)Without limiting the foregoing, the Issuer authorizes the Collateral Manager to, at any time and subject to and in accordance with this Agreement, the Indenture and the Loan Sale Agreement: (i) direct the Trustee to dispose of any or all Assets in the open market or otherwise, (ii) direct the Trustee to acquire or retain, as security for the Secured Notes in substitution for or in addition to any Collateral Obligations, Eligible Investments or other Assets, one or more Collateral Obligations, Eligible Investments or other Assets, and (iii) as agent of the Issuer, direct the Trustee to take the following actions with respect to any Asset:
+(A)tender such Assets pursuant to an Offer;
+(B)consent or object to any proposed amendment, modification or waiver with respect to such Asset, including pursuant to an Offer;
+(C)retain or dispose of any securities or other property (if other than Cash) received pursuant to an Offer or with respect to any Asset;
+(D)waive any default with respect to any Asset;
+(E)vote to accelerate, or to rescind the acceleration of, the maturity of any Asset; or
+(F)exercise any other rights or remedies with respect to such Asset as provided in the related Underlying Document or take any other
+action consistent with the terms of the Indenture and the standard of care set forth in Section 2(f).
+(d)The Issuer hereby irrevocably (except as provided below) appoints the Collateral Manager as its true and lawful agent and attorney-in-fact (with full power of substitution) in its name, place and stead and at its expense, in connection with the performance of its duties provided for in this Agreement or in the Indenture. The Issuer hereby ratifies and confirms all that such attorney-in-fact (or any substitute) shall lawfully do hereunder and pursuant hereto and authorizes such attorney-in-fact to exercise full discretion and act for the Issuer in the same manner and with the same force and effect as the managers or officers of the Issuer might or could do in respect of the performance of such services, as well as in respect of all other things the Collateral Manager deems necessary or incidental to the furtherance or conduct of such services, subject in each case to the other terms of this Agreement. The Issuer hereby authorizes such attorney-in-fact, in its sole discretion (but subject to applicable law and the provisions of this Agreement and the Indenture), to take all actions that it considers reasonably necessary and appropriate in respect of the Assets, this Agreement, the Indenture and the other Transaction Documents. This grant of power of attorney is coupled with an interest, and it shall survive and not be affected by the subsequent dissolution or bankruptcy of the Issuer, except that, notwithstanding anything herein to the contrary, the appointment herein of the Collateral Manager as the Issuer's agent and attorney-in-fact shall automatically cease and terminate upon the effective date of any termination of this Agreement, the resignation of the Collateral Manager pursuant to Section 12 or any removal of the Collateral Manager pursuant to Section 14.
+(e)The Collateral Manager and the Issuer shall take such other action, and furnish such certificates, opinions and other documents, as may be reasonably requested by the other party hereto in order to effectuate the purposes of this Agreement and to facilitate compliance with applicable laws and regulations and the terms of this Agreement.
+(f)The Collateral Manager will perform its obligations under this Agreement, the Indenture and the Fiscal Agency Agreement with reasonable care and in good faith using a degree of skill and attention no less than that which the Collateral Manager exercises with respect to comparable assets that it may manage for itself and its other clients and which is consistent with what the Collateral Manager reasonably believes to be the customary and usual collateral management practices that a prudent collateral manager of national recognition in the United States would use to manage comparable assets for its own account and for the account of others, except as expressly provided otherwise in this Agreement, the Indenture and the Fiscal Agency Agreement or under applicable law; provided that the Collateral Manager shall not be liable for any losses or damages resulting from any failure to satisfy the foregoing standard of care except to the extent that such failure would result in liability pursuant to Section 10. Without prejudicing the preceding, the Collateral Manager shall follow its customary standards, policies and procedures in performing its duties under this Agreement, the Indenture and the Fiscal Agency Agreement.
 </t>
         </is>
       </c>
@@ -512,53 +553,19 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr"/>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Definitions</t>
+          <t>Brokerage</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t xml:space="preserve"> The following words and phrases as used herein shall have the following meanings, except as otherwise expressly provided or unless the context otherwise requires:
-(a) This "Agreement" shall have the meaning ascribed to such term in the Recitals.
-(b) A "beneficial owner" of a security includes any person who, directly or indirectly, through any contract, arrangement, understanding, relationship or otherwise has or shares: (i) voting power, which includes the power to vote, or to direct the voting of, such security and/or (ii) investment power, which includes the power to dispose, or to direct the disposition, of such security, but for purposes of this Agreement a person shall not be deemed a beneficial owner of Common Stock (A)
-solely by virtue of the application of Exchange Act Rule 13d-3(d) or Exchange Act Rule 13d-5, (B) solely by virtue of the possession of the legal right to vote securities under applicable state or other law (such as by proxy or power of attorney) or (C) held of record by a "private foundation" subject to the requirements of Section 509 of the Code. "Beneficially own" and "beneficial ownership" shall have correlative meanings.
-(c) "Code" shall mean the United States Internal Revenue Code of 1986, as amended from time to time, and the applicable rulings and regulations thereunder.
-(d) "Common Stock" shall have the meaning ascribed to such term in the Recitals.
-(e) "Company" shall mean GS Inc., together with its Subsidiaries.
-(f) "Continuing Provisions" shall have the meaning ascribed to such term in Section 7.1(b).
-(g) "Covered Persons" shall mean the Participating Managing Directors, whose names are listed on Appendix A hereto, and all persons who may become Participating Managing Directors, whose names will be added to Appendix A hereto.
-(h) "Covered Shares" shall mean the aggregate of any shares of Common Stock, including any shares underlying restricted or performance-based stock units, granted under a Goldman Sachs Compensation Plan as compensation for each year for which they were Covered Persons that are delivered to Covered Persons from time to time, calculated on an after-tax basis using the Specified Tax Rate.
-(i) "Effective Date" shall mean the close of business on December 31, 2019.
-(j) "Exchange Act" shall mean the United States Securities Exchange Act of 1934, as amended from time to time.
-(k) A reference to an "Exchange Act Rule" shall mean such rule or regulation of the SEC under the Exchange Act, as in effect from time to time or as replaced by a successor rule thereto.
-(l) "Goldman Sachs 401(k) Plan" shall mean The Goldman Sachs 401(k) Plan, as amended or supplemented from time to time, and any successors to such Plan (previously known as The Goldman Sachs Employees' Profit Sharing Retirement Income Plan). The Plan is intended to be a profit sharing plan for purposes of the qualification requirements for Section 401(a) of the Code.
-(m) "Goldman Sachs Compensation Plan" shall mean the Stock Incentive Plan or any other deferred compensation or employee benefit plan of GS Inc. adopted by the Board of Directors of GS Inc. and specified by the Shareholders' Committee as a Goldman Sachs Compensation Plan (other than the Goldman Sachs 401(k) Plan).
-(n) "GS Inc." shall have the meaning ascribed to such term in the Recitals.
-(o) "Management Committee Members" shall mean the members of the Management Committee of GS Inc.
-(p) "Participating Managing Director" shall mean a Managing Director of the Company who at the time in question participates in the Partner Compensation Plan or any other compensation or benefit plan specified by the Shareholders' Committee.
-(q) "Partner Compensation Plan" shall mean The Goldman Sachs Partner Compensation Plan adopted by the Board of Directors of GS Inc., and approved by the stockholders of GS Inc., on May 7, 1999, as amended or supplemented from time to time, and any successors to such Plan.
-(r) A "person" shall include, as applicable, any individual, estate, trust, corporation, partnership, limited liability company, unlimited liability company, foundation, association or other entity.
-(s) "Preliminary Vote" shall have the meaning ascribed to such term in Section 4.1(a) hereof.
-(t) "Restricted Person" shall mean any person who is not (i) a Covered Person or (ii) a director, officer or employee of the Company acting in such person's capacity as a director, officer or employee.
-(u) "SEC" shall mean the United States Securities and Exchange Commission.
-(v) "Shareholders' Agreement" shall mean the Shareholders' Agreement adopted by the Board of Directors of GS Inc. on May 7, 1999, as amended or supplemented from time to time up to but excluding the Effective Date.
-(w) "Shareholders' Committee" shall mean the body constituted to administer the terms and provisions of this Agreement pursuant to Article V hereof.
-(x) "SIP Committee" shall mean the committee authorized to administer the Stock Incentive Plan.
-(y) "Sole Beneficial Owner" shall mean a person who is the beneficial owner of shares of Common Stock, who does not share beneficial ownership of such shares of Common Stock with any other person (other than pursuant to this Agreement or applicable community property laws) and who is the only person (other than pursuant to applicable community property laws) with a direct economic interest in such shares of Common Stock. The interest of a spouse or a domestic partner in a joint account, and an economic interest of the Company as pledgee, shall be disregarded for this purpose.
-(z) "Specified Tax Rate" shall mean the rate determined from time to time by the SIP Committee (or any person authorized thereby), in its sole discretion, to be applicable to the calculation of Covered Shares.
-(aa) "Stock Incentive Plan" shall mean The Goldman Sachs Amended and Restated Stock Incentive Plan adopted by the Board of Directors of GS Inc. on January 16, 2003 and approved by the stockholders of GS Inc. on April 1, 2003, as amended or supplemented from time to time, and any predecessors or successors to such Plan.
-(bb) "Subsidiary" shall mean any person in which GS Inc. owns, directly or indirectly, a majority of the equity economic or voting ownership interest.
-(cc) "vote" shall include actions taken or proposed to be taken by written consent.
-(dd) "Voting Shares" shall have the meaning ascribed to such term in Section 4.1(a).
+          <t xml:space="preserve">If the Collateral Manager chooses to effect a transaction for the purchase or sale of an Asset through a broker-dealer, the Collateral Manager shall use commercially reasonable efforts to obtain the best execution for all orders placed with respect to the Assets, considering all
+circumstances (but, for the avoidance of doubt and without limiting the foregoing, with no obligation to obtain the lowest price) and in a manner permitted by law. Subject to the preceding sentence, the Collateral Manager may, in the allocation of business, take into consideration research and other brokerage services furnished to the Collateral Manager or its Affiliates by brokers and dealers which are not Affiliates of the Collateral Manager. Such services may be furnished to the Collateral Manager or its Affiliates in connection with its other advisory activities or investment operations. Transactions may be executed as part of concurrent authorizations to purchase or sell the same investment for other accounts served by the Collateral Manager or its Affiliates. When these concurrent transactions occur, the objective of the Collateral Manager (and any of its Affiliates involved in such transactions) shall be to allocate the executions among the accounts in an equitable manner. A more complete description of the Collateral Manager's policies with respect to the placement of orders is set forth in the Collateral Manager's most recent Form ADV, a copy of which has been made available to the Issuer and to the Trustee.
 </t>
         </is>
       </c>
@@ -569,22 +576,28 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr"/>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Gender</t>
+          <t>Additional Activities of the Collateral Manager</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t xml:space="preserve"> For the purposes of this Agreement, the words "he," "his" or "himself" shall be interpreted to include the masculine, feminine and corporate, other entity or trust form.
+          <t xml:space="preserve">Nothing herein shall prevent the Collateral Manager or any of its Affiliates from engaging in its customary businesses, or from rendering services of any kind to the Issuer and its Affiliates, the Trustee, the Holders or beneficial owners of the Securities or any other Person or entity to the extent permitted by applicable law and not expressly prohibited under the Indenture. Without prejudice to the generality of the foregoing, the Collateral Manager or any of its Affiliates and any directors, officers, partners, employees and agents of the Collateral Manager or its Affiliates may, among other things, and subject to any limits specified in the Indenture:
+(a)serve as directors (whether supervisory or managing), partners, officers, employees, agents, nominees or signatories for the Issuer, its Affiliates or any issuer of any obligations included in the Assets, to the extent permitted by their Governing Instruments, as from time to time amended, or by any resolutions duly adopted by the Issuer, its Affiliates or any issuer of any obligations included in the Assets, pursuant to their respective Governing Instruments;
+(b)receive fees for services of any nature rendered to the issuer of any obligations included in the Assets;
+(c)be retained to provide services to the Issuer or its Affiliates that are unrelated to this Agreement, and be paid therefor;
+(d)be a secured or unsecured creditor of, or hold an equity interest in, the Issuer, its Affiliates or any issuer of any obligation included in the Assets;
+(e)make a market in any Collateral Obligations or in any Notes; and
+(f)serve as a member of any "creditors' committee" or informal workout group with respect to any obligation included in the Assets which is, has become, or, in the Collateral Manager's opinion, may become a Defaulted Obligation.
+It is understood that the Collateral Manager and any of its Affiliates have engaged (and expect to continue to engage) in other business and have furnished (and expect to continue to furnish) investment management and advisory services to others, including Persons which may
+have investment policies similar to those followed by the Collateral Manager with respect to the Assets and which may own obligations or securities of the same class, or which are of the same type, as the Collateral Obligations or the Eligible Investments or other obligations or securities of the Obligors or issuers of the Collateral Obligations or the Eligible Investments. The Collateral Manager will be free, in its sole discretion, to make recommendations to others, or effect transactions on behalf of itself or for others, which may be the same as or different from those effected with respect to the Assets and the Issuer. Nothing in the Indenture or this Agreement shall prevent the Collateral Manager or any of its Affiliates, acting either as principal or agent on behalf of others, from buying or selling, or from recommending to or directing any other account to buy or sell, at any time, obligations or securities of the same kind or class, or obligations or securities of a different kind or class of the same Obligor or issuer, as those directed by the Collateral Manager to be purchased or sold on behalf of the Issuer.
+It is understood that, to the extent permitted by applicable law, the Collateral Manager, its Affiliates or their respective Related Persons or any member of their families or a Person advised by the Collateral Manager or its Affiliates may have an interest in a particular transaction or in obligations or securities of the same kind or class, or obligations or securities of a different kind or class of the same Obligor or issuer, as those whose purchase or sale the Collateral Manager may direct under this Agreement. If, in light of market conditions and investment objectives, the Collateral Manager determines that it would be advisable to purchase or sell the same Collateral Obligation both for the Issuer, and either the proprietary account of the Collateral Manager or any Affiliate of the Collateral Manager or another client of the Collateral Manager or any Affiliate, the Collateral Manager will allocate such investment opportunities across such Persons for which such opportunities are appropriate in a manner it deems fair and equitable over time in accordance with (i) its internal conflicts of interest and allocation policies (as such policies and procedures may change from time to time in the sole discretion of the Collateral Manager) and (ii) any applicable requirements of the Advisers Act. The Issuer agrees that, in the course of managing the Collateral Obligations held by the Issuer, the Collateral Manager may consider its relationships with other clients (including Obligors and issuers) and its Affiliates. The Collateral Manager may decline to make a particular investment for the Issuer in view of such relationships.
+Unless the Collateral Manager determines in its sole discretion that such purchase or sale may be appropriate, the Collateral Manager may refrain from directing the purchase or sale hereunder of securities or obligations of (i) Persons of which the Collateral Manager, its Affiliates or any of its or their officers, directors, partners or employees are directors or officers, (ii) Persons for which the Collateral Manager or any of its Affiliates acts as financial adviser or underwriter or (iii) Persons about which the Collateral Manager or any of its Affiliates has information which the Collateral Manager deems confidential or non-public or otherwise might prohibit it from trading such securities or obligations in accordance with applicable law. The Collateral Manager shall not be obligated to utilize with respect to the Assets any particular investment opportunity of which it becomes aware or to pursue any particular investment strategy.
 </t>
         </is>
       </c>
@@ -593,10 +606,24 @@
       <c r="A7" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B7" t="inlineStr"/>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
       <c r="C7" t="inlineStr"/>
-      <c r="D7" t="inlineStr"/>
-      <c r="E7" t="inlineStr"/>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Acquisitions from or Dispositions to the Collateral Manager and Related Parties</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Subject to compliance with applicable laws and regulations and subject to this Agreement and the applicable provisions of the Loan Sale Agreement and the Indenture, the Collateral Manager may direct the Trustee to acquire a Collateral Obligation from, or sell a Collateral
+Obligation, Eligible Investment or Equity Security to, the Collateral Manager, any of its Affiliates or any client for whom the Collateral Manager or any of its Affiliates serve as investment advisor. Any such acquisition by the Issuer shall be for Fair Market Value or as otherwise specified in the Indenture.
+</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -604,19 +631,20 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>II</t>
+          <t>6</t>
         </is>
       </c>
       <c r="C8" t="inlineStr"/>
-      <c r="D8" t="inlineStr"/>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Records; Confidentiality</t>
+        </is>
+      </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t xml:space="preserve">ARTICLE II
-LIMITATIONS ON TRANSFER OF SHARES
-Section 2.1 Holding of Common Stock in GS Inc. Brokerage Accounts or in Custody and in Nominee Name.
-(a) Each Covered Person understands and agrees that all shares of Common Stock beneficially owned by him (other than shares of Common Stock held of record by a trustee in the Goldman Sachs 401(k) Plan or in any plan designated as a Goldman Sachs Compensation Plan) shall, as determined by the Shareholders' Committee from time to time, be held either in a brokerage account with a Subsidiary in his name or in the custody of a custodian (and registered in the name of a nominee for such Covered Person). If shares of Common Stock are required to be held in the custody of a custodian as provided in this Section 2.1(a), each Covered Person agrees (i) to assign, endorse and register for transfer into such nominee name or deliver to such custodian any such shares of Common Stock which are not so registered or so held, as the case may be, and (ii) that the form of the custody agreement and the identity of the custodian and nominee must be satisfactory in form and substance to the Shareholders' Committee and GS Inc.
-(b) For such time as shares of Common Stock are required to be held in the custody of a custodian in accordance with Section 2.1(a), whenever the nominee holder shall receive any dividend or other distribution upon any shares of Common Stock other than in shares of Common Stock, the Shareholders' Committee will give
-or cause to be given notice or direction to the applicable nominee and/or custodian referred to in paragraph (a) to permit the prompt distribution of such dividend or distribution to the beneficial owner of such shares of Common Stock, net of any tax withholding amounts required to be withheld by the nominee, unless the distribution of such dividend or distribution is restricted by the terms of another agreement between the Covered Person and the Company known to the Shareholders' Committee.
+          <t xml:space="preserve">(a)The Collateral Manager shall maintain appropriate books of account and records relating to services performed hereunder, and such books of account and records shall be accessible for inspection by a representative of the Issuer, the Trustee and the Independent accountants appointed by the Collateral Manager on behalf of the Issuer pursuant to Article X of the Indenture at any time during normal business hours and upon not less than three Business Days' prior notice. The Collateral Manager shall provide the Issuer with sufficient information and reports to maintain the books and records of the Issuer.
+(b)The Collateral Manager shall keep confidential any and all information obtained in connection with the services rendered hereunder and shall not disclose any such information to non-affiliated third parties except (i) with the prior written consent of the Issuer, (ii) such information as any Rating Agency shall reasonably request in connection with its rating of the Notes, (iii) in connection with establishing trading or investment accounts or otherwise in connection with effecting transactions on behalf of the Issuer, (iv) as required by law, regulation, court order or the rules or regulations of any self-regulating organization, regulatory authority, body or official having jurisdiction over the Collateral Manager, (v) to its professional advisers or (vi) such information as shall have been publicly disclosed other than in violation of this Agreement. Notwithstanding the foregoing, the Collateral Manager (a) may present summary data with respect to the performance of the Assets in conjunction with presentation of performance statistics of other funds managed or to be managed by the Collateral Manager or its Affiliates, and may aggregate data with respect to the performance of one or more categories of Assets with similar data of such other funds and (b) may disclose such other information about the Issuer, the Assets and the Securities as is customarily disclosed by managers of collateralized loan obligations. For purposes of this Section 6, the Holders and beneficial owners of the Securities shall in no event be considered "non-affiliated third parties."
+(c)Notwithstanding anything in this Agreement or any other Transaction Document to the contrary, the Collateral Manager, the Issuers, the Trustee and the Holders and beneficial owners of the Securities (and each of their respective employees, representatives or other agents) may disclose to any and all Persons, without limitation of any kind, the U.S. tax treatment and U.S. tax structure (in each case, under applicable federal, state or local law) of the transactions contemplated by this Agreement and all materials of any kind (including opinions or other tax analyses) that are provided to them relating to such U.S. tax treatment and U.S. tax structure; provided that such U.S. tax treatment and U.S. tax structure shall be kept confidential to the extent reasonably necessary to comply with applicable U.S. federal or state laws.
 </t>
         </is>
       </c>
@@ -625,10 +653,24 @@
       <c r="A9" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="B9" t="inlineStr"/>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
       <c r="C9" t="inlineStr"/>
-      <c r="D9" t="inlineStr"/>
-      <c r="E9" t="inlineStr"/>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Obligations of the Collateral Manager</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Unless otherwise specifically required by any provision of this Agreement, any other Transaction Document or applicable law, the Collateral Manager shall use commercially
+reasonable efforts to ensure that no action is taken by it, and shall not intentionally or with reckless disregard take any action, which would (a) materially adversely affect the Issuer for purposes of Cayman Islands law, United States federal or state law or any other law known to the Collateral Manager to be applicable to the Issuer, (b) not be permitted under the Issuers' Governing Instruments, (c) violate in any material respect any law, rule or regulation of any governmental body or agency having jurisdiction over the Issuer, including, without limitation, any Cayman Islands or United States federal, state or other applicable securities law, (d) require registration of the Issuer or the pool of Assets as an "investment company" under the Investment Company Act or (e) result in the Issuer or the Co-Issuer violating the terms of the Indenture. In connection with the foregoing, but without prejudice to Section 2 hereof, the Collateral Manager will not be required to make any independent investigation of any facts or laws in connection with its obligations under this Agreement or the conduct of its business generally. If the Collateral Manager is ordered to take any such action by the Issuer, the Collateral Manager shall promptly notify the Issuer, the Trustee and the Rating Agency of the Collateral Manager's judgment that such action would, or would reasonably be expected to, have one or more of the consequences set forth above and need not take such action unless (i) the action would not have the consequences set forth in clause (c) above and (ii) the Issuer again requests the Collateral Manager to do so and a Majority of each Class of Notes have consented thereto in writing. Notwithstanding any such request, the Collateral Manager need not take such action unless arrangements satisfactory to it are made to insure or indemnify the Collateral Manager from any liability it may incur as a result of such action. The Collateral Manager, its partners, their respective partners, and the Collateral Manager's directors, officers, stockholders and employees shall not be liable to the Issuer, the Trustee, the Holders or any other Person, except as provided in Section 10 of this Agreement. Any indemnification or insurance pursuant to this Section 7 that is payable out of the Assets shall be payable only in accordance with the priorities set forth in Article XI of the Indenture.
+</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
@@ -636,39 +678,23 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>III</t>
+          <t>8</t>
         </is>
       </c>
       <c r="C10" t="inlineStr"/>
-      <c r="D10" t="inlineStr"/>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Compensation</t>
+        </is>
+      </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t xml:space="preserve">ARTICLE III
-REPRESENTATIONS AND WARRANTIES OF THE PARTIES
-Section 3.1 Each Covered Person severally represents and warrants for himself that:
-(a) Such Covered Person has (and, with respect to shares of Common Stock to be acquired, will have) the right to vote pursuant to Section 4.1 of this Agreement all shares of Common Stock of which the Covered Person is the Sole Beneficial Owner; and
-(b) (if the Covered Person is other than a natural person, with respect to subsections (i) through (x), and if the Covered Person is a natural person, with respect to subsections (iv) through (x) only):
-(i) 
-such Covered Person is duly organized and validly existing in good standing under the laws of the jurisdiction of such Covered Person's formation;
-(ii) 
-such Covered Person has full right, power and authority to enter into and perform this Agreement;
-(iii) 
-the execution and delivery of this Agreement and the performance of the transactions contemplated herein have been duly authorized, and no further proceedings on the part of such Covered Person are necessary to authorize the execution, delivery and performance of this Agreement; and this Agreement has been duly executed by such Covered Person;
-(iv) 
-the person signing this Agreement on behalf of such Covered Person has been duly authorized by such Covered Person to do so;
-(v) 
-this Agreement constitutes the legal, valid and binding obligation of such Covered Person, enforceable against such Covered Person in accordance with its terms (subject to bankruptcy, insolvency, fraudulent transfer, reorganization, moratorium and similar laws of general applicability relating to or affecting creditors' rights and to general equity principles);
-(vi) 
-neither the execution and delivery of this Agreement by such Covered Person nor the consummation of the transactions contemplated herein conflicts with or results in a breach of any of the terms, conditions or provisions of any agreement or instrument to which such Covered Person is a party or by which the assets of such Covered Person are bound (including without limitation the organizational documents of such Covered Person, if such Covered Person is other than a natural person), or constitutes a default under any of the foregoing, or violates any law or regulation;
-(vii) 
-such Covered Person has obtained all authorizations, consents, approvals and clearances of all courts, governmental agencies and authorities, and any other person, if any (including the spouse of such Covered Person with respect to the interest of such spouse in the shares of Common Stock of such Covered Person if the consent of such spouse is required), required to permit such Covered Person to enter into this Agreement and to consummate the transactions contemplated herein;
-(viii) 
-there are no actions, suits or proceedings pending, or, to the knowledge of such Covered Person, threatened against or affecting such Covered Person or such Covered Person's assets in any court or before or by any federal, state, municipal or other governmental department, commission, board, bureau, agency or instrumentality which, if adversely determined, would impair the ability of such Covered Person to perform this Agreement;
-(ix) 
-the performance of this Agreement will not violate any order, writ, injunction, decree or demand of any court or federal, state, municipal or other governmental department, commission, board, bureau, agency or instrumentality to which such Covered Person is subject; and
-(x) 
-no statement, representation or warranty made by such Covered Person in this Agreement, nor any information provided by such Covered Person for inclusion in a report filed pursuant to Section 6.3 hereof or in a registration statement filed by GS Inc. contains or will contain any untrue statement of a material fact or omits or will omit to state a material fact necessary in order to make the statements, representations or warranties contained herein or information provided therein not misleading.
-Each Covered Person severally agrees for himself that the foregoing provision of this Article III shall be a continuing representation and covenant by him during the period that he shall be a Covered Person, and he shall take all actions as shall from time to time be necessary to cure any breach or violation and to obtain any authorizations, consents, approvals and clearances in order that such representations shall be true and correct during that period.
+          <t xml:space="preserve">(a)The Issuer shall pay to the Collateral Manager, for services rendered and performance of its obligations under this Agreement, a fee, payable in arrears on each Payment Date (including any Redemption Date, other than a Redemption Date in connection with a redemption of Secured Notes in part by Class not occurring on a regularly scheduled Payment Date) in accordance with the Priority of Payments that consists of (i) an amount equal to 0.15% per annum (calculated on the basis of a 360 day year and the actual number of days elapsed during the related Interest Accrual Period) of the Fee Basis Amount measured as of the first day of the Collection Period relating to such Payment Date (the "Base Management Fee") and (ii) an amount equal to 0.20% per annum (calculated on the basis of a 360 day year and the actual number of days elapsed during the related Interest Accrual Period) of the Fee Basis Amount measured as of the first day of the Collection Period relating to such Payment Date (the "Subordinated Management Fee" and, together with the Base Management Fee, the "Management Fees"). If any portion of any Management Fee payable on any Payment Date in accordance with the Priority of Payments is not paid in full for any reason, such portion shall be deferred and remain due and payable on subsequent Payment Dates.
+(b)The Collateral Manager may, in its sole discretion, waive its rights to receive any portion of the Management Fees payable on any Payment Date. The Collateral
+Manager hereby waives its rights to receive all Management Fees until such date as the Collateral Manager notifies the Issuer and the Trustee that it is revoking such waiver.
+(c)If this Agreement is terminated for any reason, or if the Collateral Manager resigns or is removed, the Base Management Fee and the Subordinated Management Fee will each be prorated for any partial period elapsing from the last Payment Date on which such Collateral Manager was entitled to receive the Base Management Fee and the Subordinated Management Fee to the effective date of such termination, resignation or removal and shall be immediately due and payable on each Payment Date following the effective date of such termination, resignation or removal in accordance with the Priority of Payments until paid in full. Otherwise, such Collateral Manager shall not be entitled to any further compensation for further services but shall be entitled to receive any expense reimbursement accrued to the effective date of termination, resignation or removal and any indemnity amounts owing (or that may become owing) under this Agreement. Any Management Fee, expense reimbursement and indemnities owed to such Collateral Manager or owed to any successor Collateral Manager on any Payment Date shall be paid pro rata based on the amount thereof then owing to each such Person, subject to the Priority of Payments.
+(d)The Collateral Manager shall be responsible for expenses incurred in the performance of its obligations under this Agreement; provided, however, the Issuer will pay or reimburse the Collateral Manager for expenses including fees and out-of-pocket expenses reasonably incurred by the Collateral Manager in connection with the services provided under this Agreement with respect to (i) the costs and expenses of the Collateral Manager incurred in connection with the negotiation, preparation and execution of this Agreement and all other agreements and matters related to the issuance of any Securities; (ii) any transfer fees necessary to register any Collateral Obligation in accordance with the Indenture; (iii) any fees and expenses in connection with the acquisition, management or disposition of Assets or otherwise in connection with the Securities or the Issuer (including (a) investment related travel, communications and related expenses, (b) loan processing fees, accounting and legal fees and expenses (including internally allocated expenses) and other expenses of professionals retained by the Collateral Manager on behalf of the Issuer and (c) amounts in connection with the termination, cancellation or abandonment of a potential acquisition or disposition of any Assets that is not consummated); (iv) any and all taxes, regulatory and governmental charges that may be incurred or payable by the Issuer; (v) any and all insurance premiums or expenses incurred in connection with the activities of the Issuer by the Collateral Manager; (vi) any and all costs, fees and expenses incurred in connection with the rating of the Secured Notes or obtaining ratings or credit estimates on Collateral Obligations, and communications with the Rating Agency; (vii) any and all costs, fees and expenses incurred in connection with the Collateral Manager's communications with the Holders (including charges related to annual meetings and for preparation of reports); (viii) costs, fees and expenses of one or more firms that provide software databases and applications for the purpose of modeling, evaluating and monitoring the Assets and the Securities pursuant to a licensing or other agreement; (ix) fees and expenses for services to the Issuer in respect of the Assets relating to asset pricing and rating services; (x) any and all expenses incurred to comply with any law or regulation related to the activities of the Issuer and, to the extent relating to the Issuer and the Assets, the Collateral Manager; (xi) the fees and expenses of any independent advisor employed to value or consider Collateral Obligations; (xii) any and all costs, fees and expenses incurred in connection with any amendment or supplemental indenture effected (or proposed to be effected) pursuant to the Indenture; (xiii) in the event the Issuer is included in the
+consolidated financial statements of the Collateral Manager or its Affiliates, costs and expenses associated with the preparation of such financial statements and other information by the Collateral Manager or its Affiliates to the extent related to the inclusion of the Issuer in such financial statements; (xiv) any and all costs, fees and expenses incurred in connection with the preparation and audit of the Issuer's financial statements; (xv) any out-of-pocket costs or expenses incurred by the Collateral Manager in connection with complying with applicable law; and (xvi) as otherwise agreed upon by the Issuer and the Collateral Manager, to be paid in accordance with the Indenture. In addition, the Issuer will pay or reimburse the costs and expenses (including fees and disbursements of counsel and accountants) of the Collateral Manager and the Issuer incurred in connection with or incidental to the entering into of this Agreement or any amendment hereto.
 </t>
         </is>
       </c>
@@ -677,10 +703,23 @@
       <c r="A11" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="B11" t="inlineStr"/>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
       <c r="C11" t="inlineStr"/>
-      <c r="D11" t="inlineStr"/>
-      <c r="E11" t="inlineStr"/>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Benefit of the Agreement</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">The Collateral Manager shall perform its obligations hereunder in accordance with the terms of this Agreement and the terms of the Indenture applicable to it and shall use all reasonable endeavors, in the course of carrying out such obligations, to protect the interests of the Holders as a group. The Collateral Manager agrees that such obligations shall be enforceable at the instance of the Issuer, the Trustee, on behalf of the Holders, or the requisite percentage of Holders as provided in the Indenture.
+</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
@@ -688,19 +727,36 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>IV</t>
+          <t>10</t>
         </is>
       </c>
       <c r="C12" t="inlineStr"/>
-      <c r="D12" t="inlineStr"/>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Limits of Collateral Manager Responsibility</t>
+        </is>
+      </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t xml:space="preserve">ARTICLE IV
-VOTING AGREEMENT
-Section 4.1 Preliminary Vote of Covered Persons; Voting Procedures.
-(a) Prior to any vote of the stockholders of GS Inc., there shall be a separate, preliminary vote, on each matter upon which a stockholder vote is proposed to be taken (each, a "Preliminary Vote"), of all of the shares of Common Stock of which a Covered Person is the Sole Beneficial Owner (excluding shares of Common Stock held by the trust underlying the Goldman Sachs 401(k) Plan) and any shares of Common Stock held by the trust underlying any plan designated as a Goldman Sachs Compensation Plan and allocated to a Covered Person (collectively, the "Voting Shares").
-(b) Other than in elections of directors, every Voting Share shall be voted in accordance with the vote of the majority of the votes cast on the matter in question by the Voting Shares in the Preliminary Vote.
-(c) In elections of directors, every Voting Share shall be voted in favor of the election of those persons, equal in number to the number of such positions to be filled, receiving the highest numbers of votes cast by the Voting Shares in the Preliminary Vote.
+          <t xml:space="preserve">(a)The Collateral Manager assumes no responsibility under this Agreement other than to render the services called for hereunder and under the terms of the Indenture applicable to it in good faith and shall not be responsible for any action or inaction of the Issuer or the Trustee in following or declining to follow any advice, recommendation or direction of the Collateral Manager. The Collateral Manager, its Affiliates, and their respective Related Persons shall not be liable to the Issuers, the Trustee, any Holder of Securities, any holder of the Issuer's ordinary shares, the Initial Purchaser, any of their respective Affiliates or Related Persons or any other Person for any act, omission, error of judgment, mistake of law, or for any claim, loss, liability, damage, judgements, assessments, settlement cost, or other expense (including attorneys' fees and expenses and court costs) arising out of any investment, or for any other act or omission in the performance of the Collateral Manager's obligations under or in connection with this Agreement or the terms of any other Transaction Document applicable to the Collateral Manager, incurred as a result of actions taken or recommended or for any omissions of the Collateral Manager, or for any decrease in the value of the Assets, except the Collateral Manager will be liable (i) by reason of acts or omissions constituting bad faith, willful misconduct or gross negligence in the performance of its duties under this Agreement and under the terms of the Indenture or (ii) with respect to the Collateral Manager Information, as of the date made, containing any untrue statement of a material fact or omitting to state a material fact necessary in order to make the statements in the Offering Circular, in light of the circumstances under which they were made, not misleading (the preceding clauses (i) and (ii) collectively referred to as "Collateral Manager Breaches").
+(b)The Collateral Manager shall not be liable for any consequential, punitive, exemplary or special damages or lost profits under this Agreement or under the Indenture. Nothing
+contained in this Agreement shall be deemed to waive any liability which cannot be waived under applicable state or federal law or any rules or regulations thereunder.
+(c)Indemnity by the Issuer. The Issuer shall indemnify and hold harmless (the Issuer in such case, the "Indemnifying Party") the Collateral Manager, its Affiliates, and their respective Related Persons (such parties collectively in such case, the "Indemnified Parties") from and against any and all losses, claims, damages, judgments, assessments, costs or other liabilities (collectively, "Losses") (as Administrative Expenses) and will promptly reimburse each such Indemnified Party for all reasonable fees and expenses incurred by an Indemnified Party with respect thereto (including, without limitation, reasonable fees and expenses of counsel and costs of collection) (collectively, "Expenses") (as Administrative Expenses) arising out of or in connection with the issuance of the Securities (including, without limitation, any untrue statement of material fact or alleged untrue statement of material fact contained in the Offering Circular, or any omission or alleged omission to state in the Offering Circular a material fact necessary in order to make the statements therein, in the light of the circumstances under which they were made, not misleading, other than Collateral Manager Information), the transactions contemplated by the Offering Circular, the Indenture or this Agreement and any acts or omissions of any such Indemnified Party; provided that such Indemnified Party shall not be indemnified for any Losses or Expenses incurred as a result of any Collateral Manager Breach or any information contained under the headings "U.S. Credit Risk Retention" and "EU Risk Retention Requirements--The Retention Holder" in the Offering Circular as of the date made containing any untrue statement of a material fact or omitting to state a material fact necessary in order to make the statements in the Offering Circular, in light of the circumstances under which they were made, not misleading.
+(d)Notwithstanding anything contained herein to the contrary, the obligations of the Issuer under this Section 10 shall be limited-recourse obligations of the Issuer, payable solely out of the Assets in accordance with the priorities set forth in Article XI of the Indenture and shall be subject to the terms of Section 22 hereof. 
+(e)Notwithstanding anything to the contrary contained in this Agreement, the provisions of this Agreement shall not be construed so as to provide for the exculpation of the Collateral Manager or the indemnification of the Issuer or the Collateral Manager for any liability (including liability under U.S. federal securities laws), to the extent (but only to the extent) that such liability may not be waived, modified or limited under applicable law or such indemnification may not be demanded under applicable law, but shall otherwise be construed so as to effectuate the provisions of this Agreement to the fullest extent permitted by applicable law.
+(f)In providing services under this Agreement, the Collateral Manager may rely in good faith upon and will be fully protected and incur no liability for acting at the direction of the Issuer (where such direction has been given without direct advice from the Collateral Manager) or for relying upon advice of nationally recognized counsel, accountants or other advisers as the Collateral Manager determines, in its sole discretion, is reasonably appropriate in connection with the services provided by the Collateral Manager under this Agreement.
+(g)An Indemnified Party shall (or with respect to an Indemnified Party other than the Collateral Manager, the Collateral Manager shall cause such Indemnified Party to) promptly notify the Indemnifying Party if the Indemnified Party receives a complaint, claim,
+compulsory process or other notice of any loss, claim, damage or liability giving rise to a claim for indemnification under this Section 10 and give written notice to the Indemnifying Party of such claim within ten (10) days after such claim is made or threatened, which notice shall specify in reasonable detail the nature of the claim and the amount (or an estimate of the amount) of the claim but failure so to notify the Indemnifying Party (i) shall not relieve such Indemnifying Party from its obligations under paragraph (a) above unless and to the extent that it did not otherwise learn of such action or proceeding and to the extent such failure results in the forfeiture by the Indemnifying Party of substantial rights and defenses and (ii) shall not, in any event, relieve the Indemnifying Party for any obligations to any Person entitled to indemnity pursuant to paragraph (a) above other than the indemnification obligations provided for in paragraph (a) above.
+(h)With respect to any claim made or threatened against an Indemnified Party, or compulsory process or request served upon such Indemnified Party for which such Indemnified Party is or may be entitled to indemnification under this Section 10, such Indemnified Party shall (or with respect to an Indemnified Party other than the Collateral Manager, the Collateral Manager shall cause such Indemnified Party to), at the Indemnifying Party's expense:
+(i)provide the Indemnifying Party such information and cooperation with respect to such claim as the Indemnifying Party may reasonably require, including, but not limited to, making appropriate personnel available to the Indemnifying Party at such reasonable times as the Indemnifying Party may request;
+(ii)cooperate and take all such steps as the Indemnifying Party may reasonably request to preserve and protect any defense to such claim;
+(iii)in the event suit is brought with respect to such claim, upon reasonable prior notice, afford to the Indemnifying Party the right, which the Indemnifying Party may exercise in its sole discretion and at its expense, to participate in the investigation, defense and settlement of such claim;
+(iv)neither incur any material expense to defend against nor release or settle any such claim or make any admission with respect thereto (other than routine or incontestable admissions or factual admissions the failure to make which would expose such Indemnified Party to unindemnified liability) without the prior written consent of the Indemnifying Party; provided, that the Indemnifying Party shall have advised such Indemnified Party that such Indemnified Party is entitled to be indemnified hereunder with respect to such claim; and
+(v)upon reasonable prior notice, afford to the Indemnifying Party the right, in its sole discretion and at its sole expense, to assume the defense of such claim, including, but not limited to, the right to designate counsel and to control all negotiations, litigation, arbitration, settlements, compromises and appeals of such claim; provided, that if the Indemnifying Party assumes the defense of such claim, it shall not be liable for any fees and expenses of counsel for any Indemnified Party incurred thereafter in connection with such claim except that if such Indemnified Party reasonably determines that counsel designated by the Indemnifying Party has a conflict of interest, such Indemnifying Party shall pay the reasonable fees and disbursements of one counsel (in addition to any local
+counsel) separate from its own counsel for all Indemnified Parties in connection with any one action or separate but similar or related actions in the same jurisdiction arising out of the same general allegations or circumstances; and provided further, that prior to entering into any final settlement or compromise, such Indemnifying Party shall seek the consent of the Indemnified Party and use its best efforts in the light of the then prevailing circumstances (including, without limitation, any express or implied time constraint on any pending settlement offer) to obtain the consent of such Indemnified Party as to the terms of settlement or compromise. If an Indemnified Party does not consent to the settlement or compromise within a reasonable time under the circumstances, the Indemnifying Party shall not thereafter be obligated to indemnify the Indemnified Party for any amount in excess of such proposed settlement or compromise.
+(i)No Indemnified Party shall, without the prior written consent of the Indemnifying Party, which consent shall not be unreasonably withheld or delayed, settle or compromise any claim giving rise to a claim for indemnity hereunder, or permit a default or consent to the entry of any judgment in respect thereof, unless such settlement, compromise or consent includes, as an unconditional term thereof, the giving by the claimant to the Indemnifying Party of a release from liability substantially equivalent to the release given by the claimant to such Indemnified Party in respect of such claim.
+(j)In the event that any Indemnified Party waives its right to indemnification hereunder, the Indemnifying Party shall not be entitled to appoint counsel to represent such Indemnified Party nor shall the Indemnifying Party reimburse such Indemnified Party for any costs of counsel to such Indemnified Party.
+(k)Indemnity by Collateral Manager. The Collateral Manager shall indemnify, defend and hold harmless the Issuer and its Related Persons from and against any and all Losses and shall reimburse each such Person for all Expenses in investigating, preparing, pursuing or defending any claim, action, proceeding or investigation with respect to any pending or threatened litigation against the Issuer or any such Related Person (collectively, "Actions"), to the extent that such Action is caused by, or is a direct consequence of, any Collateral Manager Breach; provided that no such indemnity shall be paid to the extent that such Action was caused by, or arose out of or in connection with, bad faith, willful misconduct, gross negligence or reckless disregard of the Issuer or any Related Person.
 </t>
         </is>
       </c>
@@ -711,31 +767,31 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr"/>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Irrevocable Proxy and Power of Attorney</t>
+          <t>No Partnership or Joint Venture</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t xml:space="preserve">(a) By his signature hereto, each Covered Person hereby gives the Shareholders' Committee, with full power of substitution and resubstitution, an irrevocable proxy to vote or otherwise act with respect to all of the Covered Person's Voting Shares as of the relevant record date or other date used for purposes of determining holders of Common Stock entitled to vote or take any action, as fully, to the same extent and with the same effect as such Covered Person might or could do under any applicable laws or regulations governing the rights and powers of stockholders of a Delaware corporation, as follows:
-(i) 
-such proxy shall be voted in connection with such matters as are the subject of a Preliminary Vote as provided in this Agreement in accordance with such Preliminary Vote;
-(ii) 
-the holder of such proxy shall be authorized to vote on such other matters as may come before a meeting of stockholders of GS Inc. or any adjournment thereof and as are related, directly or indirectly, to the matter which was the subject of the Preliminary Vote as the holder of such proxy sees fit in his discretion but in a manner consistent with the Preliminary Vote; and
-(iii) 
-the holder of such proxy shall be authorized to vote on such other matters as may come before a meeting of stockholders of GS Inc. or any adjournment thereof (including matters related to adjournment thereof) as the holder of such proxy sees fit in his discretion but not
-to cast any vote under this clause (iii) which is inconsistent with the Preliminary Vote or which would achieve an outcome that would frustrate the intent of the Preliminary Vote. Each Covered Person hereby affirms that this proxy is given as a term of this Agreement and as such is coupled with an interest and is irrevocable.
-It is further understood and agreed by each Covered Person that this proxy may be exercised by the holder of such proxy with respect to all Voting Shares of such Covered Person for the period beginning on the Effective Date and ending on the earlier of (a) the date this Agreement shall have been terminated pursuant to Section 7.1(a) hereof or, (b) in the case of a Covered Person, Section 7.1(b) hereof.
-(b) By his signature hereto, each Covered Person appoints the Shareholders' Committee, with full power of substitution and resubstitution, his true and lawful attorney-in-fact to direct, in accordance with the provisions of this Article IV, the voting of any Voting Shares held of record by any other person but beneficially owned by such Covered Person (including any Voting Shares held by the trust underlying any plan designated as a Goldman Sachs Compensation Plan and allocated to such Covered Person), granting to such attorneys, and each of them, full power and authority to do and perform each and every act and thing whatsoever that such attorney or attorneys may deem necessary, advisable or appropriate to carry out fully the intent of Section 4.1 and Section 4.2(a) as such Covered Person might or could do personally, hereby ratifying and confirming all acts and things that such attorney or attorneys may do or cause to be done by virtue of this power of attorney. It is understood and agreed by each Covered Person that this appointment, empowerment and authorization may be exercised by the aforementioned persons with respect to all Voting Shares of such Covered Person, and held of record by another person, for the period beginning on the Effective Date and ending on (a) the earlier of the date this Agreement shall have been terminated pursuant to Section 7.1(a) hereof or, (b) in the case of a Covered Person, Section 7.1(b) hereof.
+          <t xml:space="preserve">The Issuer and the Collateral Manager are not partners or joint venturers with each other and nothing herein shall be construed to make them such partners or joint venturers or impose any liability as such on either of them. The Collateral Manager's relation to the Issuer shall be deemed to be solely that of an independent contractor.
+12.Term; Termination.
+(a)This Agreement shall commence as of the date first set forth above and shall continue in force until the first of the following occurs: (i) the payment in full of the Notes and the termination of the Indenture in accordance with its terms; (ii) the liquidation of the Assets and the
+final distribution of the proceeds of such liquidation pursuant to the terms of the Indenture; or (iii) the termination of this Agreement in accordance with clause (b) or (c) of this Section 12 or Section 14 of this Agreement.
+(b)This Agreement may be terminated without cause by the Collateral Manager, and the Collateral Manager may resign upon 90 days' prior written notice (or such shorter notice as is acceptable to the Issuer) to the Issuer, the Trustee (who will forward such notice to each Holder), and the Rating Agency; provided, however, that the Collateral Manager shall have the right to resign immediately upon the effectiveness of any material change in applicable law or regulations which renders the performance by the Collateral Manager of its duties under the Collateral Management Agreement or under the Indenture to be a violation of such law or regulation. No such termination or resignation shall be effective until the date as of which a successor collateral manager shall have been appointed in accordance with this Agreement and delivered an instrument of acceptance to the Issuer and the resigned Collateral Manager and the successor collateral manager has effectively assumed all of the Collateral Manager's duties and obligations pursuant to this Agreement.
+(c)If this Agreement is terminated pursuant to this Section 12, such termination shall be without any further liability or obligation of either party to the other, except as provided in Sections 8(c), 10, 15 and 22 of this Agreement, which provisions shall survive the termination of this Agreement.
+(d)Promptly after notice of any removal for Cause pursuant to Section 14 hereof or resignation of the Collateral Manager pursuant to this Section 12 while any Securities are Outstanding, the Issuer shall:
+(i)transmit copies of such notice to the Trustee (who shall forward a copy of such notice to the Holders), the Fiscal Agent and the Rating Agency; and
+(ii)at the direction of a Majority of the Preferred Shares appoint as a successor collateral manager any institution that (A) has demonstrated an ability to professionally and competently perform duties similar to those imposed upon the Collateral Manager hereunder, (B) is legally qualified and has the capacity to assume all of the duties, responsibilities and obligations of the Collateral Manager hereunder and under the applicable terms of the Indenture, (C) does not cause the Issuer or the Co-Issuer or the pool of Assets to become required to register under the Investment Company Act, (D) has been approved by a Majority of the Controlling Class and a Majority of the Preferred Shares (provided, for the avoidance of doubt, that if a Majority of the Controlling Class or a Majority of the Preferred Shares has nominated such successor, it shall be deemed to have approved of such successor) and (E) does not by its appointment cause the Issuer or the Co-Issuer to be treated as a publicly traded partnership taxable as a corporation for U.S. federal income tax purposes or subject to U.S. federal, state or local income tax on a net income basis (including any tax liability imposed under Section 1446 of the Code).
+(e)If (i) a Majority of the Preferred Shares fails to nominate a successor within 30 days of initial notice of the resignation or removal of the Collateral Manager or (ii) a Majority of the Controlling Class does not approve the proposed successor nominated by the holders of the
+Preferred Shares within 10 days of the date of the notice of such nomination, then a Majority of the Controlling Class shall, within 60 days of the failure described in clause (i) or (ii) of this sentence, as the case may be, nominate a successor Collateral Manager that meets the criteria set forth in clause (d)(ii) above. If a Majority of the Preferred Shares approves such proposed successor nominated pursuant to the preceding sentence, such nominee shall become the Collateral Manager. If no successor Collateral Manager is appointed within 90 days (or, in the event of a change in applicable law or regulation which renders the performance by the resigning Collateral Manager of its duties under this Agreement or the Indenture to be a violation of such law or regulation, within 30 days) following the termination or resignation of the Collateral Manager, any of the Collateral Manager, a Majority of the Preferred Shares and the Majority of the Controlling Class shall have the right to petition a court of competent jurisdiction to appoint a successor Collateral Manager, in either such case whose appointment shall become effective after such successor has accepted its appointment and without the consent of any Holder of any Securities.
+(f)Any successor Collateral Manager shall be entitled to the Base Management Fee and the Subordinated Management Fee accruing from the effective date of its appointment. No compensation payable to such successor Collateral Manager shall be greater than such components of the Management Fee without the prior written consent of 100% of the Holders of each Class of Securities, including Collateral Manager Securities.
+(g)The Issuer, the Trustee and the successor collateral manager shall take such action (or cause the outgoing Collateral Manager to take such action) consistent with this Agreement and the terms of the Indenture applicable to the Collateral Manager, as shall be necessary to effectuate any such succession. Promptly following the appointment of a successor collateral manager in accordance with the foregoing, the Issuer shall provide written notice thereof to the Rating Agency.
+(h)In the event of removal of the Collateral Manager pursuant to this Agreement by the Issuer, the Issuer shall have all of the rights and remedies available with respect thereto at law or equity, and, without limiting the foregoing, the Issuer may by notice in writing to the Collateral Manager as provided under this Agreement terminate all the rights and obligations of the Collateral Manager under this Agreement (except those that survive termination pursuant to Section 12(c) above). Upon expiration of the applicable notice period with respect to termination specified in this Section 12 or Section 14 of this Agreement, as applicable, all authority and power of the Collateral Manager under this Agreement, whether with respect to the Assets or otherwise, shall automatically and without further action by any person or entity pass to and be vested in the successor collateral manager upon the appointment thereof. Nevertheless, the Collateral Manager shall take such steps as may be reasonably necessary to transfer such authority and power.
 </t>
         </is>
       </c>
@@ -744,10 +800,48 @@
       <c r="A14" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="B14" t="inlineStr"/>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
       <c r="C14" t="inlineStr"/>
-      <c r="D14" t="inlineStr"/>
-      <c r="E14" t="inlineStr"/>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Delegation; Assignments; Succession</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t xml:space="preserve">(a)Except as provided in this Agreement, the Collateral Manager may not assign or delegate its rights or responsibilities under this Agreement without obtaining the consent of the Issuer and the consent of a Majority of the Controlling Class and a Majority of the Preferred Shares (voting separately).
+(b)The Collateral Manager may, without obtaining the consent of any Holder of Securities, but subject to any consent of the Issuer required for an assignment under the Advisers Act, assign any of its rights or obligations under this Agreement to an Affiliate of the Collateral Manager, to the surviving entity of a merger, consolidation or restructuring of the Collateral Manager, or to any other entity to which all or substantially all of the assets, or at the time of such transfer, the collateral management business, of the Collateral Manager has been transferred; provided that such Affiliate, successor or transferee (i) has demonstrated an ability to professionally and competently perform duties similar to those imposed upon the Collateral Manager pursuant to this Agreement, (ii) has the legal right and capacity to act as Collateral Manager under this Agreement, (iii) shall not cause any of the Issuer, the Co-Issuer or the pool of Assets to become required to register under the provisions of the 1940 Act and (iv) by its appointment will not cause the Issuer or Co-Issuer to be treated as a publicly traded partnership taxable as a corporation for U.S. federal income tax purposes or subject to U.S. federal, state or local income tax on a net income basis (including any tax liability imposed under Section 1446 of the Code). The Collateral Manager shall deliver prior notice to the Rating Agency of any such assignment or combination.
+(c)In addition, the Collateral Manager may, without the consent of any Person, delegate to third parties (including without limitation its Affiliates) the duties assigned to the Collateral Manager under this Agreement, and employ third parties (including without limitation its Affiliates) to render advice (including investment advice), to provide services to arrange for trade execution and otherwise provide assistance to the Issuer, and to perform any of the Collateral Manager's duties under this Agreement; provided that the Collateral Manager shall not (i) delegate investment advice responsibilities, including (without limitation) asset selection, credit review and the negotiation and determination of the acquisition price of a Collateral Obligation to non-affiliates; (ii) be relieved of any of its duties under this Agreement regardless of the performance of any services by third parties; or (iii) by its appointment cause the Issuer or the Co-Issuer to be treated as a publicly traded partnership taxable as a corporation for U.S. federal income tax purposes or subject to U.S. federal, state or local income tax on a net income basis (including any tax liability imposed under Section 1446 of the Code).
+(d)Any assignment by the Collateral Manager consented to by the Issuer and the required Holders shall bind the assignee hereunder in the same manner as the Collateral Manager is bound. In addition, the assignee shall execute and deliver to the Issuer and the Trustee an appropriate agreement naming such assignee as a Collateral Manager. Upon the execution and delivery of such a counterpart by the assignee, the Collateral Manager shall be released from further obligations pursuant to this Agreement, except with respect to its obligations under Section 10 of this Agreement arising prior to such assignment and except with respect to its obligations under Sections 15 and 22 hereof. 
+(e)This Agreement shall not be assigned by the Issuer without the prior written consent of the Collateral Manager, except that the Collateral Manager agrees and consents to the assignment by the Issuer of this Agreement pursuant to Section 15.1(f) of the Indenture.
+(f)In the event of any assignment by the Issuer, the Issuer shall (x) use its best efforts to cause its successor to execute and deliver to the Collateral Manager such documents as
+the Collateral Manager shall consider reasonably necessary to effect fully such assignment and (y) provide written notice thereof to the Issuer, each Holder, the Trustee and the Rating Agency.
+14.Termination by the Issuer for Cause.
+This Agreement may be terminated, and the Collateral Manager may be removed for Cause (as defined below) upon 30 Business Days' prior written notice by the Issuer (a "Termination Notice") at the direction of either (i) a Majority of the Controlling Class or (ii) a Majority of the Preferred Shares; provided that Collateral Manager Securities shall be disregarded and have no voting rights with respect to any vote in respect of removal of the Collateral Manager for Cause. Simultaneous with its direction to the Issuer to so remove the Collateral Manager, either (i) a Majority of the Controlling Class or (ii) a Majority of the Preferred Shares (as applicable) shall give to the Issuer a written statement setting forth the reason for such removal (a "Notice of Removal") and the Issuer shall deliver a copy of the Termination Notice and the Notice of Removal to the Trustee (who shall deliver a copy of such notice to the Holders) within five Business Days of receipt of such written notice. No such termination or removal pursuant to this Section 14 shall be effective (A) until the date as of which a successor collateral manager shall have been appointed in accordance with Section 12 and have delivered an instrument of acceptance to the Issuer and the removed Collateral Manager and the successor collateral manager has effectively assumed all of the Collateral Manager's duties and obligations under this Agreement and the Indenture and (B) unless the Notice of Removal shall have been delivered to the Issuer as set forth above.
+For purposes of determining "Cause" with respect to termination of this Agreement pursuant to this Section 14, such term shall mean any one of the following events:
+(a)the Collateral Manager willfully and intentionally violated or breached any material provision of this Agreement or the Indenture applicable to it (not including a willful and intentional breach that results from a good faith dispute regarding reasonable alternative courses of action or reasonable interpretation of instructions);
+(b)the Collateral Manager breached any provision of this Agreement or any terms of the Indenture applicable to it (other than as covered by clause (a) above and it being understood that failure to meet any Concentration Limitation, Collateral Quality Test or Coverage Test is not a breach for purposes of this clause (b)), which breach would reasonably be expected to have a material adverse effect on any Class of Secured Notes and shall not cure such breach (if capable of being cured) within 60 days after the earlier to occur of a Responsible Officer of the Collateral Manager receiving notice or having actual knowledge of such breach, unless, if such breach is remediable, the Collateral Manager has taken action commencing the cure thereof within such 60 day period that the Collateral Manager believes in good faith will remedy such breach within 90 days after the earlier to occur of a Responsible Officer receiving notice or having actual knowledge thereof;
+(c)the failure of any representation or warranty of the Collateral Manager in Section 16 hereof to be correct in any material respect when such representation or warranty is made, which failure (i) would reasonably be expected to have a material adverse effect on any Class of Secured Notes and (ii) if capable of being corrected, is not corrected by the Collateral Manager within 45 days of a Responsible Officer of the Collateral Manager receiving notice of
+such failure, unless if such failure is remediable, the Collateral Manager has taken action commencing the cure thereof within such 45-day period that the Collateral Manager believes in good faith will remedy such failure within 90 days after the earlier to occur of a Responsible Officer receiving notice thereof or having actual knowledge thereof;
+(d)(A) the Collateral Manager is wound up or dissolved; (B) there is appointed over the Collateral Manager or a substantial portion of its assets a receiver, administrator, administrative receiver, trustee or similar officer; or (C) the Collateral Manager (i) ceases to be able to, or admits in writing its inability to, pay its debts as they become due and payable, or makes a general assignment for the benefit of, or enters into any composition or arrangement with, its creditors generally; (ii) applies for or consents (by admission of material allegations of a petition or otherwise) to the appointment of a receiver, trustee, assignee, custodian, liquidator or sequestrator (or other similar official) of the Collateral Manager or of any substantial part of its properties or assets, or authorizes such an application or consent, or proceedings seeking such appointment are commenced without such authorization, consent or application against the Collateral Manager and continue undismissed for 60 days; (iii) authorizes or files a voluntary petition in bankruptcy, or applies for or consents (by admission of material allegations of a petition or otherwise) to the application of any bankruptcy, reorganization, arrangement, readjustment of debt, insolvency or dissolution, or authorizes such application or consent, or proceedings to such end are instituted against the Collateral Manager without such authorization, application or consent and are approved as properly instituted and remain undismissed for 60 days or result in adjudication of bankruptcy or insolvency; or (iv) permits or suffers all or any substantial part of its properties or assets to be sequestered or attached by court order and the order remains undismissed for 60 days;
+(e)the occurrence and continuation of an Event of Default specified under clause (a), (b) or (c) of the definition of such term that results primarily from any material breach by the Collateral Manager of its duties under this Agreement or under the Indenture which breach or default is not cured within any applicable cure period (excluding any such Event of Default relating to a good faith dispute with respect to reasonable alternative courses of action or the meaning of any relevant provision under the Transaction Documents or any matter that is in the process of being reconciled in accordance with the applicable Transaction Documents); or
+(f)(i) the occurrence of an act by the Collateral Manager that constitutes fraud or felony criminal activity in the performance of its obligations under this Agreement (as determined pursuant to a final adjudication by a court of competent jurisdiction) or the Collateral Manager being indicted for a felony criminal offense materially related to its business of providing asset management services or (ii) any Responsible Officer of the Collateral Manager primarily responsible for the performance by the Collateral Manager of its obligations under this Agreement (in the performance of his or her investment management duties) is indicted for a felony criminal offense materially related to the business of the Collateral Manager providing asset management services and continues to have responsibility for the performance by the Collateral Manager under this Agreement for a period of thirty (30) days after such indictment.
+Prior to the effective appointment of any successor collateral manager in accordance with this Agreement, the event or circumstance giving rise to the removal of the Collateral Manager for Cause described above (other than pursuant to clause (d) of the definition thereof) may be waived
+by a written approval of both a Majority of the Controlling Class and a Majority of the Preferred Shares (voting separately) as a basis for termination of this Agreement and removal of the Collateral Manager hereunder; provided that Collateral Manager Securities shall be disregarded and have no voting rights for purposes of this waiver, it being understood that if all of the Securities of either such Class are Collateral Manager Securities, the approval of a Majority of such Class shall not be required for such waiver.
+If any of the events specified in clauses (a) through (f) of this Section 14 shall occur, the Collateral Manager shall give prompt written notice thereof to the Issuer, the Trustee (who shall forward such notice to the Holders) and the Rating Agency; provided that if the events specified in clause (d) above shall occur, the Collateral Manager shall give written notice thereof to the Issuer, the Trustee (who will forward such notice to the holders of the Securities) and the Rating Agency immediately upon the Collateral Manager's becoming aware of the occurrence of such event. In no event will the Trustee be required to determine whether or not Cause exists to remove the Collateral Manager.
+15.Action Upon Termination.
+(a)From and after the effective date of termination of this Agreement, the Collateral Manager shall not be entitled to compensation for further services hereunder, but shall be paid all compensation to which it is entitled, and shall receive all other amounts for which it is entitled to reimbursement, all as provided in and subject to Section 8 hereof, and shall be entitled to receive any amounts owing under Sections 7 and 10 hereof. Upon such termination, the Collateral Manager shall as soon as practicable:
+(i)deliver to and at the direction of the Issuer all property and documents of the Trustee or the Issuer or otherwise relating to the Assets then in the custody of the Collateral Manager; and
+(ii)deliver to the Trustee an accounting with respect to the books and records delivered to the Trustee or the successor collateral manager appointed pursuant to Section 12(d) hereof.
+Notwithstanding such termination, the Collateral Manager shall remain liable for its acts or omissions hereunder as described in Section 10 arising prior to termination and for any expenses, losses, damages, liabilities, demands, charges and claims of any nature whatsoever (including reasonable attorneys' fees) in respect of or arising out of a breach of the representations and warranties made by the Collateral Manager in Section 16(b) hereof or from any failure of the Collateral Manager to comply in all material respects with the provisions of this Section 15.
+(b)The Collateral Manager agrees that, notwithstanding any termination, it shall reasonably cooperate in any Proceeding arising in connection with this Agreement, the Indenture or any of the Assets (excluding any such Proceeding in which claims are asserted against the Collateral Manager or any Affiliate of the Collateral Manager) upon receipt of appropriate indemnification and expense reimbursement.
+</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
@@ -755,15 +849,34 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>16</t>
         </is>
       </c>
       <c r="C15" t="inlineStr"/>
-      <c r="D15" t="inlineStr"/>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Representations and Warranties</t>
+        </is>
+      </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t xml:space="preserve">ARTICLE V
-SHAREHOLDERS' COMMITTEE
+          <t xml:space="preserve">(a)The Issuer hereby represents and warrants to the Collateral Manager as follows:
+(i)The Issuer has been duly incorporated and is validly existing under the laws of the Cayman Islands, has all requisite corporate power and authority to own its assets and the securities proposed to be owned by it and included in the Assets and to transact the business in which it is presently engaged and is duly qualified under the laws of each jurisdiction where its ownership or lease of property or the conduct of its business requires, or the performance of its obligations under this Agreement, the Indenture or the Securities would require, such qualification, except for failures to be so qualified, authorized or licensed that would not in the aggregate have a material adverse effect on the business, operations, assets or financial condition of the Issuer.
+(ii)The Issuer has all requisite corporate power and authority to execute, deliver and perform this Agreement, the Indenture and the Securities and all obligations required hereunder, under the Indenture and the Securities and has taken all necessary action to authorize the execution, delivery and performance of this Agreement, the Indenture and the Securities and the performance of all obligations imposed upon it hereunder and thereunder. No consent of any other Person including, without limitation, shareholders and creditors of the Issuer, and no license, permit, approval or authorization of, exemption by, notice or report to, or registration, filing or declaration with, any governmental authority, other than those that may be required under state securities or "blue sky" laws and those that have been or shall be obtained in connection with the Indenture and the issuance of the Securities, is required by the Issuer in connection with this Agreement, the Indenture or the Securities or the execution, delivery, performance, validity or enforceability of this Agreement, the Indenture or the Securities or the obligations imposed upon it hereunder or thereunder. This Agreement constitutes, and each instrument or document required hereunder, when executed and delivered hereunder, shall constitute, the legally valid and binding obligations of the Issuer enforceable against the Issuer in accordance with its terms, subject, as to enforcement, to (a) the effect of bankruptcy, insolvency or similar laws affecting generally the enforcement of creditors' rights, as such laws would apply in the event of any bankruptcy, receivership, insolvency or similar event applicable to the Issuer and (b) general equitable principles (whether enforceability of such principles is considered in a proceeding at law or in equity).
+(iii)The execution, delivery and performance of this Agreement and the documents and instruments required hereunder shall not violate any provision of any existing law or regulation binding on the Issuer, or any order, judgment, award or decree of any court, arbitrator or governmental authority binding on or applicable to the Issuer, or the Governing Instruments of, or any securities issued by, the Issuer or of any mortgage, indenture, lease, contract or other agreement, instrument or undertaking to which the Issuer is a party or by which the Issuer or any of its assets is or may be bound, the violation of which would have a material adverse effect on the business, operations, assets or financial condition of the Issuer, and shall not result in or require the creation or imposition of any lien on any of its property, assets or revenues pursuant to the provisions of any such mortgage, indenture, lease, contract or other agreement, instrument or undertaking (other than the lien of the Indenture).
+(iv)The Issuer is not in violation of its Governing Instruments or in breach or violation of or in default under the Indenture or any contract or agreement to which it is a party or by which it or any of its assets may be bound, or any applicable statute or any rule, regulation or order of any court, government agency or body having jurisdiction over the Issuer or its properties, the breach or violation of which or default under which would have a material adverse effect on the validity or enforceability of this Agreement or the performance by the Issuer of its duties hereunder.
+(v)True and complete copies of the Indenture and the Issuer's Governing Instruments have been or, no later than the Closing Date, will be delivered to the Collateral Manager. In addition, the Issuer acknowledges that it has received Part 2 of the Collateral Manager's Form ADV filed with the Securities and Exchange Commission, as required by Rule 204-3 under the Advisers Act, prior to or concurrently with the date of execution of this Agreement.
+The Issuer agrees to deliver a true and complete copy of each and every amendment to the documents referred to in Section 16(a)(v) above to the Collateral Manager as promptly as practicable after its adoption or execution.
+(b)The Collateral Manager hereby represents and warrants to the Issuer as follows:
+(i)The Collateral Manager is a limited liability company duly organized and validly existing and in good standing under the law of the State of Delaware and has full power and authority to own its assets and to transact the business in which it is currently engaged and is duly qualified as a limited liability company and is in good standing under the laws of each jurisdiction where its ownership or lease of property or the conduct of its business requires, or the performance of this Agreement would require such qualification, except for those jurisdictions in which the failure to be so qualified, authorized or licensed would not have a material adverse effect on the business, operations, assets or financial condition of the Collateral Manager or on the ability of the Collateral Manager to perform its obligations under, or on the validity or enforceability of, this Agreement and the provisions of the Indenture which are applicable to the Collateral Manager; the Collateral Manager is a registered investment adviser under the United States Investment Advisers Act of 1940, as amended (the "Advisers Act").
+(ii)The Collateral Manager has full power and authority to execute and deliver this Agreement and perform all obligations required hereunder and under the provisions of the Indenture which are applicable to the Collateral Manager, and the Collateral Manager has taken all necessary action to authorize this Agreement on the terms and conditions hereof and the execution, delivery and performance of this Agreement and all obligations required hereunder and under the terms of the Indenture which are applicable to the Collateral Manager. No consent of any other person, including, without limitation, creditors of the Collateral Manager, and no license, permit, approval or authorization of, exemption by, notice or report to, or registration, filing or declaration with, any governmental authority (other than those already obtained) is required by the Collateral Manager in connection with this Agreement or the execution, delivery,
+performance, validity or enforceability of this Agreement or the obligations required hereunder or under the terms of the Indenture which are applicable to the Collateral Manager. This Agreement has been, and each instrument and document required hereunder or under the terms of the Indenture shall be, executed and delivered by a duly authorized officer of the Collateral Manager, and this Agreement constitutes, and each instrument and document required hereunder or under the terms of the Indenture when executed and delivered by the Collateral Manager hereunder or under the terms of the Indenture shall constitute, the legally valid and binding obligations of the Collateral Manager enforceable against the Collateral Manager in accordance with their terms, subject, as to enforcement, to (a) the effect of bankruptcy, insolvency or similar laws affecting generally the enforcement of creditors' rights and (b) general equitable principles (whether considered in a proceeding at law or in equity).
+(iii)The execution, delivery and performance of this Agreement and the terms of the Indenture applicable to the Collateral Manager and the documents and instruments required hereunder or under the terms of the Indenture shall not violate any provision of any existing law or regulation binding on or applicable to the Collateral Manager, or any order, judgment, award or decree of any court, arbitrator or governmental authority binding on the Collateral Manager, or the Governing Instruments of, or any securities issued by the Collateral Manager or of any mortgage, indenture, lease, contract or other agreement, instrument or undertaking to which the Collateral Manager is a party or by which the Collateral Manager or any of its assets is or may be bound, the violation of which would have a material adverse effect on the business operations, assets or financial condition of the Collateral Manager or its ability to perform its obligations under this Agreement, and shall not result in or require the creation or imposition of any lien on any of its property, assets or revenues pursuant to the provisions of any such mortgage, indenture, lease, contract or other agreement, instrument or undertaking.
+(iv)There is no charge, investigation, action, suit or proceeding before or by any court pending or, to the knowledge of the Collateral Manager, threatened that, if determined adversely to the Collateral Manager, would have a material adverse effect upon the performance by the Collateral Manager of its duties under, or on the validity or enforceability of, this Agreement or the provisions of the Indenture applicable to the Collateral Manager hereunder.
+(v)The Collateral Manager is authorized to carry on its business in the United States.
+(vi)The Collateral Manager is not in violation of its Governing Instruments or in breach or violation of or in default under any contract or agreement to which it is a party or by which it or any of its property may be bound, or any applicable statute or any rule, regulation or order of any court, government agency or body having jurisdiction over the Collateral Manager or its properties, the breach or violation of which or default under which would have a material adverse effect on the validity or enforceability of this Agreement or the provisions of the Indenture applicable to the Collateral Manager hereunder, or the performance by the Collateral Manager of its duties hereunder or under the Indenture.
+(vii)The Collateral Manager Information contained in the Offering Circular, as the same may be thereafter amended or supplemented, as of the date thereof, as of the date of any such amendment or supplement, and as of the Closing Date, is true and correct in all material respects and does not omit to state any material fact necessary in order to make the statements therein, in the light of the circumstances under which they were made, not misleading.
+The Collateral Manager makes no representation, express or implied, with respect to the Issuer or the disclosure with respect to the Issuer.
 </t>
         </is>
       </c>
@@ -774,22 +887,18 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
+          <t>17</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr"/>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Membership</t>
+          <t>Observation Rights</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t xml:space="preserve"> The Shareholders' Committee shall at all times consist of all of those individuals who are both Covered Persons and members of the Board of Directors of GS Inc. and who agree to serve as members of the Shareholders' Committee.
+          <t xml:space="preserve">The Issuer covenants and agrees, if requested in writing by the Collateral Manager and to the extent practicable under the circumstances, to notify the Collateral Manager of each meeting of the Board of Directors of the Issuer following the receipt of such request by the Issuer and to use commercially reasonable efforts to provide any materials distributed to the Board of Directors in connection with any such meeting and to afford a representative of the Collateral Manager the opportunity to be present at each such meeting, in person or by telephone at the option of the Collateral Manager.
 </t>
         </is>
       </c>
@@ -800,22 +909,56 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
+          <t>18</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr"/>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Additional Members</t>
+          <t>Notices</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t xml:space="preserve"> If there are less than three individuals who are both Covered Persons and members of the Board of Directors of GS Inc. and who agree to serve as members of the Shareholders' Committee, the Shareholders' Committee shall consist of each such individual plus such additional individuals who are Covered Persons and who are selected pursuant to procedures established by the Shareholders' Committee as shall assure a Shareholders' Committee of not less than three members who are Covered Persons.
+          <t xml:space="preserve">Unless expressly provided otherwise herein, all notices, requests, demands and other communications required or permitted under this Agreement shall be in writing (including by telecopy) and shall be deemed to have been duly given, made and received when delivered against receipt or upon actual receipt, by registered or certified mail, postage prepaid, return receipt requested, by hand delivery, or by courier service or, in the case of telecopy or email notice, when received in legible form, addressed as set forth below:
+(a)
+If to the Issuer:
+Owl Rock Technology Financing 2020-1
+c/o Walkers Fiduciary Limited
+Cayman Corporate Centre
+27 Hospital Road,
+George Town, Grand Cayman
+Attention: The Directors
+KY1-9008, Cayman Islands
+Telephone no. +1 (345) 814-7600
+Email: fiduciary@walkersglobal.com
+(b)
+If to the Collateral Manager:
+Owl Rock Technology Advisors LLC
+399 Park Avenue, Floor 38
+New York, NY 10022
+Attention: Alan Kirshenbaum
+E-mail Address: alan@owlrock.com with a copy to legal@owlrock.com
+(c)
+If to the Trustee:
+State Street Bank and Trust Company
+1776 Heritage Drive
+Mail Code: JAB0250
+North Quincy, Massachusetts 02171
+Attention: Structured Trust and Analytics
+Ref: Owl Rock Technology Financing 2020-1
+Facsimile: (617) 937-4358
+Telephone: (617) 662-9839
+(d)
+If to the Rating Agency:
+S&amp;P Global Rating
+55 Water Street, 41st Floor
+New York, New York 10041
+Attention: Structured Credit-CDO Surveillance
+(e)
+If to the Holders:
+At their respective addresses set forth on the Register.
+Any party may alter the address, email address or telecopy number to which communications or copies are to be sent by giving notice of such change of address in conformity with the provisions of this Section 18 for the giving of notice.
 </t>
         </is>
       </c>
@@ -826,25 +969,18 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
+          <t>19</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr"/>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Determinations of and Actions by the Shareholders' Committee</t>
+          <t>Binding Nature of Agreement; Successors and Assigns</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t xml:space="preserve">(a) All determinations necessary or advisable under this Agreement (including determinations of beneficial ownership) shall be made by the Shareholders' Committee, whose determinations shall be final and binding. The Shareholders' Committee's determinations under this Agreement and actions (including waivers) hereunder need not be uniform and may be made selectively among Covered Persons (whether or not such Covered Persons are similarly situated).
-(b) Each Covered Person recognizes and agrees that the members of the
-Shareholders' Committee in acting hereunder shall at all times be acting in their capacities as members of the Shareholders' Committee and not as directors or officers of the Company and in so acting or failing to act shall not have any fiduciary duties to the Covered Persons as a member of the Shareholders' Committee by virtue of the fact that one or more of such members may also be serving as a director or officer of the Company or otherwise.
-(c) The Shareholders' Committee shall act through a majority vote of its members and such actions may be taken in person at a meeting (in person or telephonically) or by a written instrument signed by all of the members.
+          <t xml:space="preserve">This Agreement shall be binding upon and inure to the benefit of the parties hereto and their respective heirs, personal representatives, successors and assigns as provided herein. The Collateral Manager agrees that its obligations hereunder shall be enforceable, at the instance of the Issuer, on behalf of the Issuer by the Trustee under the Indenture, as provided in the Indenture (subject to the rights and defenses of the Collateral Manager and the provisions of Sections 10 and 15 hereunder). The Collateral Manager agrees and consents to the provisions contained in Article XV of the Indenture.
 </t>
         </is>
       </c>
@@ -855,22 +991,20 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr"/>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Certain Obligations of the Shareholders' Committee</t>
+          <t>Entire Agreement; Amendments</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t xml:space="preserve"> The Shareholders' Committee shall be obligated (a) to attend as proxy, or cause a person designated by it and acting as lawful proxy to attend as proxy, each meeting of the stockholders of GS Inc. and to vote or to cause such designee to vote the Voting Shares over which it has the power to vote in accordance with the results of the Preliminary Vote as set forth in Section 4.1, and (b) to develop procedures governing Preliminary Votes and other votes and actions to be taken pursuant to this Agreement.
+          <t xml:space="preserve">This Agreement contains the entire agreement and understanding among the parties hereto with respect to the subject matter hereof and supersedes all prior and contemporaneous agreements, understandings, inducements and conditions, express or implied, oral or written, of any nature whatsoever with respect to the subject matter hereof. The parties hereto hereby acknowledge that any prior agreement concerning the subject matter hereof has been terminated as of the date hereof and is of no further force or effect (except for provisions in such agreement designated to survive termination). (For the avoidance of doubt, the parties acknowledge that this Agreement does not govern the relationship of Owl Rock Technology Advisors in its capacity as a Holder.) The express terms hereof control and supersede any course of performance and/or usage of the trade inconsistent with any of the terms hereof.
+This Agreement may be amended by the parties thereto to (i) correct inconsistencies, typographical or other errors, defects or ambiguities or (ii) conform the Collateral Management Agreement to the Offering Circular, the Collateral Administration Agreement or the Indenture (as it may be amended from time to time in accordance with the terms thereof), in each case without the consent of the holders of any Securities and without satisfaction of the S&amp;P Rating Condition. The Collateral Manager will provide notice to the Rating Agency of any such amendment.
+Any other amendment to this Agreement requires the consent of the parties hereto and the approval of a Majority of the Preferred Shares, with at least ten (10) days' prior written notice to the Trustee (who shall forward such notice to the Controlling Class), the Fiscal Agent and the Rating Agency; provided that any such amendment to this Agreement that would (i) modify the definition of the term Cause, (ii) modify the Base Management Fee, including any component of the Base Management Fee, the method for calculating any component of the Base Management Fee or any definition used in any component of the Base Management Fee or (iii) modify the Class or Classes or the percentage of the Aggregate Outstanding Amount of any Class that has the right to remove the Collateral Manager, consent to any assignment of this Agreement or nominate or approve any successor Collateral Manager shall, in each case, also require the approval of a Majority of the Controlling Class and satisfaction of the S&amp;P Rating Condition.
 </t>
         </is>
       </c>
@@ -879,10 +1013,23 @@
       <c r="A20" s="1" t="n">
         <v>18</v>
       </c>
-      <c r="B20" t="inlineStr"/>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
       <c r="C20" t="inlineStr"/>
-      <c r="D20" t="inlineStr"/>
-      <c r="E20" t="inlineStr"/>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Conflict with the Indenture</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t xml:space="preserve">In the event that this Agreement requires any action to be taken with respect to any matter and the Indenture requires that a different action be taken with respect to such matter, and such actions are mutually exclusive, the provisions of the Indenture in respect thereof shall control.
+</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
@@ -890,26 +1037,20 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>VI</t>
+          <t>22</t>
         </is>
       </c>
       <c r="C21" t="inlineStr"/>
-      <c r="D21" t="inlineStr"/>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Subordination; Limited Recourse; Non-Petition</t>
+        </is>
+      </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t xml:space="preserve">ARTICLE VI
-OTHER AGREEMENTS OF THE PARTIES
-Section 6.1 Standstill Provisions. Each Covered Person agrees that such Covered Person shall not, directly or indirectly, alone or in concert with any other person:
-(a) make, or in any way participate in, any "solicitation" of "proxies" (as such terms are defined in Exchange Act Rule 14a-1) relating to any securities of the Company to or with any Restricted Person;
-(b) deposit any shares of Common Stock in a voting trust or subject any shares of Common Stock to any voting agreement or arrangement that includes as a party any Restricted Person;
-(c) form, join or in any way participate in a group (as contemplated by Exchange Act Rule 13d-5(b)) with respect to any securities of the Company (or any securities the ownership of which would make the owner thereof a beneficial owner of securities of the Company (for this purpose as determined by Exchange Act Rule 13d-3 and Exchange Act Rule 13d-5)) that includes as a party any Restricted Person;
-(d) make any announcement subject to Exchange Act Rule 14a-1(l)(2)(iv) to any Restricted Person;
-(e) initiate or propose any "shareholder proposal" subject to Exchange Act
-Rule 14a-8;
-(f) together with any Restricted Person, make any offer or proposal to acquire any securities or assets of GS Inc. or any of its Subsidiaries or solicit or propose to effect or negotiate any form of business combination, restructuring, recapitalization or other extraordinary transaction involving, or any change in control of, GS Inc., its Subsidiaries or any of their respective securities or assets;
-(g) together with any Restricted Person, seek the removal of any directors or a change in the composition or size of the board of directors of GS Inc.;
-(h) together with any Restricted Person, in any way participate in a call for any special meeting of the stockholders of GS Inc.; or
-(i) assist, advise or encourage any person with respect to, or seek to do, any of the foregoing.
+          <t xml:space="preserve">(a)The Collateral Manager agrees that the payment of all amounts to which it is entitled pursuant to this Agreement shall be subordinated to the extent set forth in the Indenture, including Article XI thereof.
+(b)Notwithstanding any other provision of this Agreement, the obligations of the Issuer hereunder are, from time to time and at any time, limited recourse obligations of the Issuer, payable solely from the Assets and only to the extent of funds available from time to time and in accordance with the Priority of Payments, and following exhaustion of the Assets, any claims of the Collateral Manager hereunder shall be extinguished and shall not thereafter revive. The Collateral Manager further agrees (i) not to take any action in respect of any claims hereunder against any officer, director, employee, shareholder, noteholder or administrator of the Issuer and (ii) not to cause the filing of a petition in bankruptcy against the Issuer for the nonpayment of the fees or other amounts payable by the Issuer to the Collateral Manager under this Agreement until the payment in full of all Notes issued under the Indenture and the expiration of a period equal to one year and a day, or, if longer, the applicable preference period, following such payment. Nothing in this Section 22 shall preclude, or be deemed to stop, the Collateral Manager (x) from taking any action prior to the expiration of the aforementioned period in (A) any case or Proceeding voluntarily filed or commenced by the Issuer, or (B) any involuntary insolvency Proceeding filed or commenced by a Person other than the Collateral Manager, or (y) from commencing against the Issuer or any of its properties any legal action which is not a bankruptcy, reorganization,
+arrangement, insolvency, moratorium or liquidation proceeding. The provisions of this Section 22 shall survive the termination of this Agreement for any reason whatsoever.
 </t>
         </is>
       </c>
@@ -920,23 +1061,18 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
+          <t>23</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr"/>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Expenses</t>
+          <t>Governing Law</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t xml:space="preserve">(a) GS Inc. shall be responsible for all expenses of the members of the Shareholders' Committee incurred in the operation and administration of this Agreement, including expenses of proxy solicitation for and tabulation of the Preliminary Vote, expenses incurred in preparing appropriate filings and correspondence with the SEC, lawyers', accountants', agents', consultants', experts', investment banking and other professionals' fees, expenses incurred in enforcing the provisions of this Agreement, expenses incurred in maintaining any necessary or appropriate books and records relating to this Agreement and expenses incurred in the preparation of amendments to and waivers of provisions of this Agreement.
-(b) Each Covered Person shall be responsible for all expenses incurred by him in connection with compliance with his obligations under this Agreement, including expenses incurred by the Shareholders' Committee or GS Inc. in enforcing the provisions of this Agreement relating to such obligations.
+          <t xml:space="preserve">THIS AGREEMENT SHALL BE GOVERNED BY AND CONSTRUED IN ACCORDANCE WITH THE LAW OF THE STATE OF NEW YORK.
 </t>
         </is>
       </c>
@@ -947,24 +1083,18 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
+          <t>24</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr"/>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Filing of Schedule 13D or 13G</t>
+          <t>Indulgences Not Waivers</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t xml:space="preserve">(a) In the event that a Covered Person is required to file a report of beneficial ownership on Schedule 13D or 13G with respect to the shares of Common Stock beneficially owned by him (for this purpose as determined by Exchange Act Rule 13d-3 and Exchange Act Rule 13d-5), such Covered Person agrees that, unless otherwise directed by the Shareholders' Committee, he will not file a separate such report, but will file a report together with the other Covered Persons, containing the information required by the Exchange Act, and he understands and agrees that such report shall be filed on his behalf by the Shareholders' Committee, any member
-thereof or any person authorized thereby. Such Covered Person shall cooperate fully with the other Covered Persons and the Shareholders' Committee to achieve the timely filing of any such report and any amendments thereto as may be required, and such Covered Person agrees that any information concerning him which he furnishes in connection with the preparation and filing of such report will be complete and accurate.
-(b) By his signature hereto, each Covered Person appoints the Shareholders' Committee and each member thereof, with full power of substitution and resubstitution, his true and lawful attorney-in-fact to execute such reports and any and all amendments thereto and to file such reports with all exhibits thereto and other documents in connection therewith with the SEC, granting to such attorneys, and each of them, full power and authority to do and perform each and every act and thing whatsoever that such attorney or attorneys may deem necessary, advisable or appropriate to carry out fully the intent of this Section 6.3 as such Covered Person might or could do personally, hereby ratifying and confirming all acts and things that such attorney or attorneys may do or cause to be done by virtue of this power of attorney. Each Covered Person hereby further designates such attorneys as such Covered Person's agents authorized to receive notices and communications with respect to such reports and any amendments thereto. It is understood and agreed by each Covered Person that this appointment, empowerment and authorization may be exercised by the aforementioned persons for the period beginning on May 7, 1999 and ending on the date such Covered Person is no longer subject to the provisions of this Agreement (and shall extend thereafter for such time as is required to reflect, and only to reflect, that such Covered Person is no longer a party to this Agreement).
+          <t xml:space="preserve">Neither the failure nor any delay on the part of any party hereto to exercise any right, remedy, power or privilege under this Agreement shall operate as a waiver thereof, nor shall any single or partial exercise of any right, remedy, power or privilege preclude any other or further exercise of the same or of any other right, remedy, power or privilege, nor shall any waiver of any right, remedy, power or privilege with respect to any occurrence be construed as a waiver of such right, remedy, power or privilege with respect to any other occurrence. No waiver shall be effective unless it is in writing and is signed by the party asserted to have granted such waiver.
 </t>
         </is>
       </c>
@@ -975,22 +1105,18 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
+          <t>25</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr"/>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Representatives, Successors and Assigns</t>
+          <t>Costs and Expenses</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t xml:space="preserve"> This Agreement shall be binding upon and inure to the benefit of the respective legal representatives, successors and assigns of the Covered Persons; provided, however, that a Covered Person may not assign this Agreement or any of his rights or obligations hereunder without the prior written consent of GS Inc., and any assignment without such consent by a Covered Person shall be void; and provided further that no assignment of this Agreement by GS Inc. or to a successor of GS Inc. (by operation of law or otherwise) shall be valid unless such assignment is made to a person which succeeds to the business of GS Inc. substantially as an entirety.
+          <t xml:space="preserve">The reasonable costs and expenses (including the fees and disbursements of counsel and accountants) incurred by the Collateral Manager in connection with the negotiation and preparation of and the execution of this Agreement, and all matters incident thereto, shall be borne by the Issuer and, unless paid on the Closing Date or shortly thereafter by ORCC or from the proceeds of the offering of the Securities (to the extent permitted under the Indenture), shall be subject to the Priority of Payments.
 </t>
         </is>
       </c>
@@ -1001,22 +1127,18 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
+          <t>26</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr"/>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Further Assurances</t>
+          <t>Titles Not to Affect Interpretation</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Each Covered Person agrees to execute such additional documents and take such further action as may be reasonably necessary to effect the provisions of this Agreement.
+          <t xml:space="preserve">The titles of paragraphs and subparagraphs contained in this Agreement are for convenience only, and they neither form a part of this Agreement nor are they to be used in the construction or interpretation hereof.
 </t>
         </is>
       </c>
@@ -1025,10 +1147,23 @@
       <c r="A26" s="1" t="n">
         <v>24</v>
       </c>
-      <c r="B26" t="inlineStr"/>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>27</t>
+        </is>
+      </c>
       <c r="C26" t="inlineStr"/>
-      <c r="D26" t="inlineStr"/>
-      <c r="E26" t="inlineStr"/>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Execution in Counterparts</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t xml:space="preserve">This Agreement may be executed in any number of counterparts, which may be effectively delivered by facsimile or other electronic means or other written form of communication, each of which shall be deemed to be an original as against any party whose signature appears thereon, and all of which shall together constitute one and the same instrument. This Agreement shall become binding when one or more counterparts hereof, individually or taken together, shall bear the signatures of all of the parties reflected hereon as the signatories.
+</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
@@ -1036,19 +1171,19 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>VII</t>
+          <t>28</t>
         </is>
       </c>
       <c r="C27" t="inlineStr"/>
-      <c r="D27" t="inlineStr"/>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Provisions Separable</t>
+        </is>
+      </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t xml:space="preserve">ARTICLE VII
-MISCELLANEOUS
-Section 7.1 Term of the Agreement; Termination of Certain Provisions.
-(a) The term of this Agreement shall continue until the first to occur of January 1, 2050 and such time as this Agreement is terminated by the affirmative vote of not less than 66 2/3% of the outstanding Covered Shares.
-(b) Unless this Agreement is previously terminated pursuant to Section 7.1(a) hereof, any Covered Person who ceases to be a Covered Person for any reason other than death shall no longer be bound by the provisions of this Agreement (other than Sections 5.3, 6.2, 6.3, 6.5, 7.4, 7.5, 7.6, 7.8 and 7.10 (the "Continuing Provisions")), and such Covered Person's name shall be removed from Appendix A to this Agreement.
-(c) Unless this Agreement is theretofore terminated pursuant to Section 7.1(a) hereof, the estate of any Covered Person who ceases to be a Covered Person by reason of death shall from and after the date of such death be bound only by the Continuing Provisions, and such Covered Person's name shall be removed from Appendix A to this Agreement.
+          <t xml:space="preserve">In case any provision in this Agreement shall be invalid, illegal or unenforceable as written, such provision shall be construed in the manner most closely resembling the apparent intent of the parties with respect to such provision so as to be valid, legal and enforceable; provided, however, that if there is no basis for such a construction, such provision shall be ineffective only to the extent
+of such invalidity, illegality or unenforceability and, unless the ineffectiveness of such provision destroys the basis of the bargain for one of the parties to this Agreement, the validity, legality and enforceability of the remaining provisions hereof or thereof shall not in any way be affected or impaired thereby.
 </t>
         </is>
       </c>
@@ -1059,27 +1194,18 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>7</t>
-        </is>
-      </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
+          <t>29</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr"/>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Amendments</t>
+          <t>Number and Gender</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t xml:space="preserve">(a) Except as provided in this Section 7.2, provisions of this Agreement may be amended only by the affirmative vote of the holders of a majority of the outstanding Covered Shares.
-(b) This Section 7.2(b) and Section 7.1(a) may be amended only by the affirmative vote of the holders of 66 2/3% of the outstanding Covered Shares. Any amendment of any other provision of this Agreement that would have the effect, in connection with a tender or exchange offer by any person other than the Company as to which the Board of Directors of GS Inc. is recommending rejection, of permitting transfers which would not be permitted by the terms of this Agreement as then in effect shall also require the affirmative vote of the holders of 66 2/3% of the outstanding Covered Shares.
-(c) This Section 7.2(c), Article V and any other provision the amendment (or addition) of which has the effect of materially changing the rights or obligations of the Shareholders' Committee hereunder may be amended (or added) either (i) with the approval of the Shareholders' Committee and the affirmative vote of the holders of a majority of the Covered Shares or (ii) by the affirmative vote of the holders of 66 2/3% of the outstanding Covered Shares.
-(d) In addition to any other vote or approval that may be required under this Section 7.2, any amendment of this Agreement that has the effect of changing the obligations of GS Inc. hereunder to make such obligations materially more onerous to GS Inc. shall require the approval of GS Inc.
-(e) Each Covered Person understands that it is intended that each Participating Managing Director of the Company will be a Covered Person under this Agreement or will become a Covered Person upon his appointment to such position, and each Covered Person further understands that from time to time certain other persons may
-become Covered Persons and certain Covered Persons will cease to be bound by provisions of this Agreement pursuant to the terms hereof when they cease to be Participating Managing Directors. Accordingly, this Agreement may be amended by action of the Shareholders' Committee from time to time and without the approval of any other person, but solely for the purposes of (i) adding to Appendix A such persons as shall be made party to this Agreement pursuant to the terms hereof, such addition to be effective as of the time of such action or appointment, and (ii) removing from Appendix A such persons as shall cease to be bound by the provisions of this Agreement pursuant to Sections 7.1(b) or (c) hereof, which additions and removals shall be given effect from time to time by appropriate changes to Appendix A
+          <t xml:space="preserve">Words used herein, regardless of the number and gender specifically used, shall be deemed and construed to include any other number, singular or plural, and any other gender, masculine, feminine or neuter, as the context requires.
 </t>
         </is>
       </c>
@@ -1090,25 +1216,18 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>7</t>
-        </is>
-      </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
+          <t>30</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr"/>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Waivers</t>
+          <t>Jurisdiction and Venue</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t xml:space="preserve"> The provisions of this Agreement may be waived only as provided in this Section 7.3.
-(a) In all circumstances other than those set forth in Section 7.2, the provisions of this Agreement may be waived only by the affirmative vote of the holders of a majority of the outstanding Covered Shares.
-(b) In connection with any waiver granted under this Agreement, the Shareholders' Committee or the holders of the percentage of Covered Shares required for the waiver, as the case may be, may impose such conditions as they determine on the granting of such waivers.
-(c) The failure of the Company or the Shareholders' Committee at any time or times to require performance of any provision of this Agreement shall in no manner affect the rights at a later time to enforce the same. No waiver by the Company or the Shareholders' Committee of the breach of any term contained in this Agreement, whether by conduct or otherwise, in any one or more instances, shall be deemed to be or construed as a further or continuing waiver of any such breach or the breach of any other term of this Agreement.
+          <t xml:space="preserve">The parties to this Agreement irrevocably submit to the non-exclusive jurisdiction of any New York state or federal court sitting in the Borough of Manhattan in The City of New York in any action or proceeding arising out of or relating to this Agreement, the Securities or the Indenture, and the parties irrevocably agree that all claims in respect of such action or proceeding may be heard and determined in such New York state or federal court. The parties to this Agreement irrevocably waive, to the fullest extent they may legally do so, the defense of an inconvenient forum to the maintenance of such action or proceeding. The parties to this Agreement irrevocably consent to the service of any and all process in any action or proceeding by the mailing or delivery of copies of such process to it in accordance with Section 18. The parties agree that a final judgment in any such action or proceeding shall be conclusive and may be enforced in other jurisdictions by suit on the judgment or in any other manner provided by law.
 </t>
         </is>
       </c>
@@ -1119,22 +1238,18 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>7</t>
-        </is>
-      </c>
-      <c r="C30" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
+          <t>31</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr"/>
       <c r="D30" t="inlineStr">
         <is>
-          <t>GOVERNING LAW</t>
+          <t>Rule 17g-5 Compliance</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t xml:space="preserve"> THIS AGREEMENT SHALL BE GOVERNED BY AND CONSTRUED IN ACCORDANCE WITH THE LAWS OF THE STATE OF DELAWARE, WITHOUT REGARD TO PRINCIPLES OF CONFLICTS OF LAWS.
+          <t xml:space="preserve">The Collateral Manager agrees that any notice, report, request for satisfaction of the Global Rating Condition or other information provided by the Collateral Manager (or any of its respective representatives or advisors) to any Rating Agency hereunder or under the Indenture or the Collateral Administration Agreement for the purposes of undertaking credit rating surveillance of the Secured Notes shall be provided, substantially concurrently, by the Collateral Manager to the Information Agent for posting on a password-protected website in accordance with the procedures set forth in Section 2A of the Collateral Administration Agreement and Section 14.16 of the Indenture.
 </t>
         </is>
       </c>
@@ -1143,260 +1258,25 @@
       <c r="A31" s="1" t="n">
         <v>29</v>
       </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
+      <c r="B31" t="inlineStr"/>
+      <c r="C31" t="inlineStr"/>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Resolution of Disputes</t>
+          <t>IN WITNESS WHEREOF</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t xml:space="preserve">(a) The Shareholders' Committee shall have the sole and exclusive power to enforce the provisions of this Agreement. The Shareholders' Committee may in its sole discretion request GS Inc. to conduct such enforcement, and GS Inc. agrees to conduct such enforcement as requested and directed by the Shareholders' Committee.
-(b) Without diminishing the finality and conclusive effect of any determination by the Shareholders' Committee of any matter under this Agreement (and subject to the provisions of paragraphs (c) and (d) hereof), any dispute, controversy or claim arising out of or relating to or concerning the provisions of this Agreement shall be finally settled by arbitration in New York City before, and in accordance with the rules then obtaining of, the New York Stock Exchange, Inc. ("NYSE"), or if the NYSE declines to arbitrate the matter, the American Arbitration Association ("AAA") in accordance with the commercial arbitration rules of the AAA.
-(c) Notwithstanding the provisions of paragraph (b), and in addition to its right to submit any dispute or controversy to arbitration, the Shareholders' Committee may bring, or may cause GS Inc. to bring, on behalf of the Shareholders' Committee or on behalf of one or more Covered Persons, an action or special proceeding in a state or federal court of competent jurisdiction sitting in the State of Delaware, whether or not an arbitration proceeding has theretofore been or is ever initiated, for the purpose of temporarily, preliminarily or permanently enforcing the provisions of this Agreement and, for the purposes of this paragraph (c), each Covered Person (i) expressly consents to the application of paragraph (d) to any such action or proceeding, (ii) agrees that proof shall not be required that monetary damages for breach of the provisions of this Agreement would be difficult to calculate and that remedies at law would be inadequate and (iii) irrevocably appoints each General Counsel of GS Inc., c/o The Corporation Trust Company, Corporation Trust Center, 1209 Orange Street, Wilmington, Delaware 19801 as such Covered Person's agent for service of process in connection with any such action or proceeding, who shall promptly advise such Covered Person of any such service of process.
-(d) Each Covered Person hereby irrevocably submits to the exclusive jurisdiction of any state or federal court located in the State of Delaware over any suit, action or proceeding arising out of or relating to or concerning this Agreement that is not otherwise arbitrated according to the provisions of paragraph (b) hereof. This includes any suit, action or proceeding to compel arbitration or to enforce an arbitration award. The parties acknowledge that the forum designated by this paragraph (d) has a reasonable relation to this Agreement, and to the parties' relationship with one another. Notwithstanding the foregoing, nothing herein shall preclude the Shareholders' Committee or GS Inc. from bringing any action or proceeding in any other court for the purpose of enforcing the provisions of this Section 7.5.
-The agreement of the parties as to forum is independent of the law that may be applied in the action, and they each agree to such forum even if the forum may under applicable law choose to apply non-forum law. The parties hereby waive, to the fullest extent permitted by applicable law, any objection which they now or hereafter may have to personal jurisdiction or to the laying of venue of any such suit, action or proceeding brought in any court referred to in paragraph (d). The parties undertake not to commence any action arising out of or relating to or concerning this Agreement in any forum other than a forum described in paragraph (d). The parties agree that, to the fullest extent permitted by applicable law, a final and non-appealable judgment in any such suit, action or proceeding in any such court shall be conclusive and binding upon the parties.
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" s="1" t="n">
-        <v>30</v>
-      </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
-      <c r="C32" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="D32" t="inlineStr">
-        <is>
-          <t>Relationship of Parties</t>
-        </is>
-      </c>
-      <c r="E32" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> The terms of this Agreement are intended not to create a separate entity for United States federal income tax purposes, and nothing in this Agreement shall be read to create any partnership, joint venture or separate entity among the parties or to create any trust or other fiduciary relationship between them.
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" s="1" t="n">
-        <v>31</v>
-      </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
-      <c r="D33" t="inlineStr">
-        <is>
-          <t>Notices</t>
-        </is>
-      </c>
-      <c r="E33" t="inlineStr">
-        <is>
-          <t xml:space="preserve">(a) Any communication, demand or notice to be given hereunder will be duly given (and shall be deemed to be received) when delivered in writing by hand or first class mail or by telecopy to a party at its address as indicated below:
-If to a Covered Person,
-c/o The Goldman Sachs Group, Inc.
-200 West Street
-15th Floor
-New York, New York 10282-2198
-Fax: (212) 341-5638
-Attention: General Counsel;
-If to the Shareholders' Committee, at
-Shareholders' Committee under the Shareholders' Agreement,
-c/o The Goldman Sachs Group, Inc.
-200 West Street
-15th Floor
-New York, New York 10282-2198
-Fax: (212) 341-5638
-Attention: General Counsel;
-and
-If to GS Inc., at
-The Goldman Sachs Group, Inc.
-200 West Street
-15th Floor
-New York, New York 10282-2198
-Fax: (212) 341-5638
-Attention: General Counsel.
-GS Inc. shall be responsible for notifying each Covered Person of the receipt of a communication, demand or notice under this Agreement relevant to such Covered Person at the address of such Covered Person then in the records of GS Inc. (and each Covered Person shall notify GS Inc. of any change in such address for communications, demands and notices).
-(b) Unless otherwise provided to the contrary herein, any notice which is required to be given in writing pursuant to the terms of this Agreement may be given by telecopy.
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" s="1" t="n">
-        <v>32</v>
-      </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
-      <c r="C34" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
-      </c>
-      <c r="D34" t="inlineStr">
-        <is>
-          <t>Severability</t>
-        </is>
-      </c>
-      <c r="E34" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> If any provision of this Agreement is finally held to be invalid, illegal or unenforceable, (a) the remaining terms and provisions hereof shall be unimpaired and (b) the invalid or unenforceable term or provision shall be deemed replaced by a term or provision that is valid and enforceable and that comes closest to expressing the intention of the invalid or unenforceable term or provision.
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" s="1" t="n">
-        <v>33</v>
-      </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
-      <c r="C35" t="inlineStr">
-        <is>
-          <t>9</t>
-        </is>
-      </c>
-      <c r="D35" t="inlineStr">
-        <is>
-          <t>Right to Determine Tender Confidentially</t>
-        </is>
-      </c>
-      <c r="E35" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> In connection with any tender or exchange offer for all or any portion of the outstanding Common Stock, subject to compliance with all applicable restrictions on transfer in this Agreement or any other agreement with GS Inc., each Covered Person will have the right to determine confidentially whether such Covered Person's Covered Shares will be tendered in such tender or exchange offer.
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" s="1" t="n">
-        <v>34</v>
-      </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
-      <c r="C36" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-      <c r="D36" t="inlineStr">
-        <is>
-          <t>No Third-Party Rights</t>
-        </is>
-      </c>
-      <c r="E36" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Nothing expressed or referred to in this Agreement will be construed to give any person other than the parties to this Agreement any legal or equitable right, remedy, or claim under or with respect to this Agreement or any provision of this Agreement. This Agreement and all of its provisions and conditions are for the sole and exclusive benefit of the parties to this Agreement and their successors and assigns.
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" s="1" t="n">
-        <v>35</v>
-      </c>
-      <c r="B37" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
-      <c r="C37" t="inlineStr">
-        <is>
-          <t>11</t>
-        </is>
-      </c>
-      <c r="D37" t="inlineStr">
-        <is>
-          <t>Section Headings</t>
-        </is>
-      </c>
-      <c r="E37" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> The headings of sections in this Agreement are provided for convenience only and will not affect its construction or interpretation.
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" s="1" t="n">
-        <v>36</v>
-      </c>
-      <c r="B38" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
-      <c r="C38" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
-      </c>
-      <c r="D38" t="inlineStr">
-        <is>
-          <t>Execution in Counterparts</t>
-        </is>
-      </c>
-      <c r="E38" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> This Agreement may be executed in any number of counterparts, each of which shall be deemed an original, but all such counterparts shall together constitute but one and the same instrument.
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" s="1" t="n">
-        <v>37</v>
-      </c>
-      <c r="B39" t="inlineStr"/>
-      <c r="C39" t="inlineStr"/>
-      <c r="D39" t="inlineStr">
-        <is>
-          <t>IN WITNESS WHEREOF</t>
-        </is>
-      </c>
-      <c r="E39" t="inlineStr">
-        <is>
-          <t>, the parties hereto have duly executed or caused to be duly executed this Agreement.
-THE GOLDMAN SACHS GROUP, INC.
-By: /s/ Karen P. Seymour
-Name: Karen P. Seymour
-Title: Executive Vice President
-and General Counsel
-Dated: December 31, 2019
-17</t>
+          <t xml:space="preserve">, the parties hereto have executed this Agreement as of the date first written above.
+OWL ROCK TECHNOLOGY ADVISORS LLC
+By:
+Name
+Title:
+OWL ROCK TECHNOLOGY FINANCING 2020-1
+By:
+Name:
+Title:
+</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
moved norm to own folder
</commit_message>
<xml_diff>
--- a/tests/test.xlsx
+++ b/tests/test.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:E115"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -464,17 +464,18 @@
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr">
         <is>
-          <t xml:space="preserve">EX-10.14 4 orctf-ex1014_70.htm EX-10.14
-Exhibit 10.14
-COLLATERAL MANAGEMENT AGREEMENT
-This Agreement, dated as of December 16, 2020 (this "Agreement"), is entered into by and between Owl Rock Technology Financing 2020-1, an exempted company incorporated with limited liability under the laws of the Cayman Islands, with its registered office at the offices of Walkers Fiduciary Limited, Cayman Corporate Centre, 27 Hospital Road, George Town, Grand Cayman, KY1-9008, Cayman Islands (together with successors and assigns permitted hereunder, the "Issuer"), and Owl Rock Technology Advisors LLC ("Owl Rock Technology Advisors"), a Delaware limited liability company, with its principal offices located at 399 Park Avenue, 38th Floor, New York, NY 10022, as collateral manager (in such capacity, the "Collateral Manager"). Capitalized terms used and not otherwise defined herein have the meanings assigned to them in the Indenture.
-WITNESSETH:
-WHEREAS, the Issuer intends to issue Notes pursuant to an indenture dated as of December 16, 2020 (the "Indenture"), among the Issuer, Owl Rock Technology Financing 2020-1 LLC, as co-issuer of the Co-Issued Notes (the "Co-Issuer" and, together with the Issuer, the "Issuers"), and State Street Bank and Trust Company, as trustee (together with any successor trustee permitted under the Indenture, the "Trustee");
-WHEREAS, the Issuer intends to issue Preferred Shares pursuant to the Issuer's memorandum and articles of association and subject to the Fiscal Agency Agreement, dated as of the Closing Date (the "Fiscal Agency Agreement"), among the Fiscal Agent, the Share Registrar and the Issuer, as amended from time to time in accordance with the terms thereof; 
-WHEREAS, the Issuer intends to pledge certain Collateral Obligations, Eligible Investments and Cash (all as defined in the Indenture) and certain other assets (all as set forth in the Indenture) (collectively, the "Assets") to the Trustee as security for its obligations under the Indenture;
-WHEREAS, the Issuer wishes to enter into this Agreement, pursuant to which the Collateral Manager agrees to perform, on behalf of the Issuer, certain duties with respect to the Assets in the manner and on the terms set forth herein and to perform such additional duties as are consistent with the terms of this Agreement, the Indenture and the Collateral Administration Agreement; and
-WHEREAS, the Collateral Manager has the capacity to provide the services required hereby and is prepared to perform such services upon the terms and conditions set forth herein.
-NOW, THEREFORE, in consideration of the mutual agreements herein set forth, the parties hereto agree as follows:
+          <t xml:space="preserve">EX-10.11 8 usb-pfloatxsecuritiescusto.htm EX-10.11
+EXECUTION VERSION
+_____________________
+CUSTODY AGREEMENT
+_____________________
+dated as of September 21, 2023
+by and between
+PROSPECT FLOATING RATE AND ALTERNATIVE INCOME FUND, INC.
+("Company")
+and
+U.S. BANK TRUST COMPANY, NATIONAL ASSOCIATION
+("Custodian")
 </t>
         </is>
       </c>
@@ -483,30 +484,12 @@
       <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
+      <c r="B3" t="inlineStr"/>
       <c r="C3" t="inlineStr"/>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Definitions</t>
-        </is>
-      </c>
+      <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Terms used herein and not defined below or elsewhere herein shall have the meanings set forth in the Indenture.
-"Agreement" shall mean this Agreement, as amended from time to time.
-"Cause" shall have the meaning set forth in Section 14.
-"Collateral Manager Information" shall have the meaning ascribed to such term in the Offering Circular.
-"Collateral Manager Securities" shall mean any Securities owned by the Collateral Manager, an Affiliate thereof, or any account, fund, client or portfolio established and controlled by the Collateral Manager or an Affiliate thereof or for which the Collateral Manager or an Affiliate thereof acts as the investment adviser or with respect to which the Collateral Manager or an Affiliate thereof exercises discretionary control thereover.
-"Governing Instruments" shall mean the memorandum of association, articles of association and by-laws, if applicable, in the case of a corporation, the partnership agreement, in the case of a partnership, the limited liability company agreement and certificate of formation, in the case of a limited liability company or the trust agreement and (if applicable) certificate of trust, in the case of a trust.
-"Notice of Removal" shall have the meaning set forth in Section 14.
-"Offering Circular" shall mean the final Offering Circular with respect to the Notes.
-"Related Person" shall mean with respect to any Person, the owners of the equity interests therein, directors, officers, employees, managers, agents and professional advisors thereof.
-"Responsible Officer" shall mean, with respect to any Person, any duly authorized director, officer or manager of such Person with direct responsibility for the administration of the applicable agreement and also, with respect to a particular matter, any other duly authorized director, officer or manager of such Person to whom such matter is referred because of such director's, officer's or manager's knowledge of and familiarity with the particular subject. Each party may receive and accept a certification of the authority of any other party as conclusive evidence of the authority of any Person to act, and such certification may be considered as in full force and effect until receipt by such other party of written notice to the contrary.
-"Termination Notice" shall have the meaning set forth in Section 14.
+          <t xml:space="preserve">TABLE OF CONTENTS
 </t>
         </is>
       </c>
@@ -515,37 +498,14 @@
       <c r="A4" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
+      <c r="B4" t="inlineStr"/>
       <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr">
         <is>
-          <t>General Duties and Authorization of the Collateral Manager</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">The Collateral Manager shall provide services to the Issuer as follows:
-(a)Subject to and in accordance with the applicable terms of the Indenture and the terms of this Agreement, the Collateral Manager agrees to, and is appointed and authorized by
-the Issuer to (i) select the Assets to be acquired, sold, terminated, tendered or otherwise disposed of by the Issuer, (ii) invest and reinvest the Assets subject to the Investment Criteria and other conditions and restrictions set forth in the Indenture, (iii) instruct the Trustee with respect to any acquisition, disposition or tender of, or Offer with respect to, any Assets received in respect thereof in the open market or otherwise by the Issuer, and (iv) perform all other tasks and take all other actions that any of the Indenture, the Collateral Administration Agreement or this Agreement specify are to be taken by the Collateral Manager (provided that the Collateral Manager will not be bound to follow any amendment or supplement to the Indenture unless it has consented thereto in accordance with the Indenture); and the Collateral Manager may, in its sole discretion, take any other action not inconsistent with an action that such agreements specify may be taken by the Collateral Manager.
-(b)The Collateral Manager shall monitor the Assets on behalf of the Issuer on an ongoing basis and will further agree to provide or cause to be provided to the Issuer all reports, schedules and other data reasonably available to the Collateral Manager that the Issuer is required to prepare and deliver or cause to be prepared and delivered under the Indenture, in such forms and containing such information required thereby, in reasonably sufficient time for such required reports, schedules and data to be reviewed and delivered by or on behalf of the Issuer to the parties entitled thereto under the Indenture. The obligation of the Collateral Manager to furnish such reports, schedules and other data is subject to the Collateral Manager's timely receipt of necessary information, reports, schedules and other data from the Person responsible for the delivery or preparation thereof (including without limitation, Obligors of the Collateral Obligations, the Rating Agency, the Trustee and the Collateral Administrator) and to any confidentiality restrictions with respect thereto. 
-(c)Without limiting the foregoing, the Issuer authorizes the Collateral Manager to, at any time and subject to and in accordance with this Agreement, the Indenture and the Loan Sale Agreement: (i) direct the Trustee to dispose of any or all Assets in the open market or otherwise, (ii) direct the Trustee to acquire or retain, as security for the Secured Notes in substitution for or in addition to any Collateral Obligations, Eligible Investments or other Assets, one or more Collateral Obligations, Eligible Investments or other Assets, and (iii) as agent of the Issuer, direct the Trustee to take the following actions with respect to any Asset:
-(A)tender such Assets pursuant to an Offer;
-(B)consent or object to any proposed amendment, modification or waiver with respect to such Asset, including pursuant to an Offer;
-(C)retain or dispose of any securities or other property (if other than Cash) received pursuant to an Offer or with respect to any Asset;
-(D)waive any default with respect to any Asset;
-(E)vote to accelerate, or to rescind the acceleration of, the maturity of any Asset; or
-(F)exercise any other rights or remedies with respect to such Asset as provided in the related Underlying Document or take any other
-action consistent with the terms of the Indenture and the standard of care set forth in Section 2(f).
-(d)The Issuer hereby irrevocably (except as provided below) appoints the Collateral Manager as its true and lawful agent and attorney-in-fact (with full power of substitution) in its name, place and stead and at its expense, in connection with the performance of its duties provided for in this Agreement or in the Indenture. The Issuer hereby ratifies and confirms all that such attorney-in-fact (or any substitute) shall lawfully do hereunder and pursuant hereto and authorizes such attorney-in-fact to exercise full discretion and act for the Issuer in the same manner and with the same force and effect as the managers or officers of the Issuer might or could do in respect of the performance of such services, as well as in respect of all other things the Collateral Manager deems necessary or incidental to the furtherance or conduct of such services, subject in each case to the other terms of this Agreement. The Issuer hereby authorizes such attorney-in-fact, in its sole discretion (but subject to applicable law and the provisions of this Agreement and the Indenture), to take all actions that it considers reasonably necessary and appropriate in respect of the Assets, this Agreement, the Indenture and the other Transaction Documents. This grant of power of attorney is coupled with an interest, and it shall survive and not be affected by the subsequent dissolution or bankruptcy of the Issuer, except that, notwithstanding anything herein to the contrary, the appointment herein of the Collateral Manager as the Issuer's agent and attorney-in-fact shall automatically cease and terminate upon the effective date of any termination of this Agreement, the resignation of the Collateral Manager pursuant to Section 12 or any removal of the Collateral Manager pursuant to Section 14.
-(e)The Collateral Manager and the Issuer shall take such other action, and furnish such certificates, opinions and other documents, as may be reasonably requested by the other party hereto in order to effectuate the purposes of this Agreement and to facilitate compliance with applicable laws and regulations and the terms of this Agreement.
-(f)The Collateral Manager will perform its obligations under this Agreement, the Indenture and the Fiscal Agency Agreement with reasonable care and in good faith using a degree of skill and attention no less than that which the Collateral Manager exercises with respect to comparable assets that it may manage for itself and its other clients and which is consistent with what the Collateral Manager reasonably believes to be the customary and usual collateral management practices that a prudent collateral manager of national recognition in the United States would use to manage comparable assets for its own account and for the account of others, except as expressly provided otherwise in this Agreement, the Indenture and the Fiscal Agency Agreement or under applicable law; provided that the Collateral Manager shall not be liable for any losses or damages resulting from any failure to satisfy the foregoing standard of care except to the extent that such failure would result in liability pursuant to Section 10. Without prejudicing the preceding, the Collateral Manager shall follow its customary standards, policies and procedures in performing its duties under this Agreement, the Indenture and the Fiscal Agency Agreement.
-</t>
-        </is>
-      </c>
+          <t>Page</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -553,19 +513,18 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>1</t>
         </is>
       </c>
       <c r="C5" t="inlineStr"/>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Brokerage</t>
+          <t>DEFINITIONS</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t xml:space="preserve">If the Collateral Manager chooses to effect a transaction for the purchase or sale of an Asset through a broker-dealer, the Collateral Manager shall use commercially reasonable efforts to obtain the best execution for all orders placed with respect to the Assets, considering all
-circumstances (but, for the avoidance of doubt and without limiting the foregoing, with no obligation to obtain the lowest price) and in a manner permitted by law. Subject to the preceding sentence, the Collateral Manager may, in the allocation of business, take into consideration research and other brokerage services furnished to the Collateral Manager or its Affiliates by brokers and dealers which are not Affiliates of the Collateral Manager. Such services may be furnished to the Collateral Manager or its Affiliates in connection with its other advisory activities or investment operations. Transactions may be executed as part of concurrent authorizations to purchase or sell the same investment for other accounts served by the Collateral Manager or its Affiliates. When these concurrent transactions occur, the objective of the Collateral Manager (and any of its Affiliates involved in such transactions) shall be to allocate the executions among the accounts in an equitable manner. A more complete description of the Collateral Manager's policies with respect to the placement of orders is set forth in the Collateral Manager's most recent Form ADV, a copy of which has been made available to the Issuer and to the Trustee.
+          <t xml:space="preserve">1
 </t>
         </is>
       </c>
@@ -576,28 +535,18 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>2</t>
         </is>
       </c>
       <c r="C6" t="inlineStr"/>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Additional Activities of the Collateral Manager</t>
+          <t>APPOINTMENT OF CUSTODIAN</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t xml:space="preserve">Nothing herein shall prevent the Collateral Manager or any of its Affiliates from engaging in its customary businesses, or from rendering services of any kind to the Issuer and its Affiliates, the Trustee, the Holders or beneficial owners of the Securities or any other Person or entity to the extent permitted by applicable law and not expressly prohibited under the Indenture. Without prejudice to the generality of the foregoing, the Collateral Manager or any of its Affiliates and any directors, officers, partners, employees and agents of the Collateral Manager or its Affiliates may, among other things, and subject to any limits specified in the Indenture:
-(a)serve as directors (whether supervisory or managing), partners, officers, employees, agents, nominees or signatories for the Issuer, its Affiliates or any issuer of any obligations included in the Assets, to the extent permitted by their Governing Instruments, as from time to time amended, or by any resolutions duly adopted by the Issuer, its Affiliates or any issuer of any obligations included in the Assets, pursuant to their respective Governing Instruments;
-(b)receive fees for services of any nature rendered to the issuer of any obligations included in the Assets;
-(c)be retained to provide services to the Issuer or its Affiliates that are unrelated to this Agreement, and be paid therefor;
-(d)be a secured or unsecured creditor of, or hold an equity interest in, the Issuer, its Affiliates or any issuer of any obligation included in the Assets;
-(e)make a market in any Collateral Obligations or in any Notes; and
-(f)serve as a member of any "creditors' committee" or informal workout group with respect to any obligation included in the Assets which is, has become, or, in the Collateral Manager's opinion, may become a Defaulted Obligation.
-It is understood that the Collateral Manager and any of its Affiliates have engaged (and expect to continue to engage) in other business and have furnished (and expect to continue to furnish) investment management and advisory services to others, including Persons which may
-have investment policies similar to those followed by the Collateral Manager with respect to the Assets and which may own obligations or securities of the same class, or which are of the same type, as the Collateral Obligations or the Eligible Investments or other obligations or securities of the Obligors or issuers of the Collateral Obligations or the Eligible Investments. The Collateral Manager will be free, in its sole discretion, to make recommendations to others, or effect transactions on behalf of itself or for others, which may be the same as or different from those effected with respect to the Assets and the Issuer. Nothing in the Indenture or this Agreement shall prevent the Collateral Manager or any of its Affiliates, acting either as principal or agent on behalf of others, from buying or selling, or from recommending to or directing any other account to buy or sell, at any time, obligations or securities of the same kind or class, or obligations or securities of a different kind or class of the same Obligor or issuer, as those directed by the Collateral Manager to be purchased or sold on behalf of the Issuer.
-It is understood that, to the extent permitted by applicable law, the Collateral Manager, its Affiliates or their respective Related Persons or any member of their families or a Person advised by the Collateral Manager or its Affiliates may have an interest in a particular transaction or in obligations or securities of the same kind or class, or obligations or securities of a different kind or class of the same Obligor or issuer, as those whose purchase or sale the Collateral Manager may direct under this Agreement. If, in light of market conditions and investment objectives, the Collateral Manager determines that it would be advisable to purchase or sell the same Collateral Obligation both for the Issuer, and either the proprietary account of the Collateral Manager or any Affiliate of the Collateral Manager or another client of the Collateral Manager or any Affiliate, the Collateral Manager will allocate such investment opportunities across such Persons for which such opportunities are appropriate in a manner it deems fair and equitable over time in accordance with (i) its internal conflicts of interest and allocation policies (as such policies and procedures may change from time to time in the sole discretion of the Collateral Manager) and (ii) any applicable requirements of the Advisers Act. The Issuer agrees that, in the course of managing the Collateral Obligations held by the Issuer, the Collateral Manager may consider its relationships with other clients (including Obligors and issuers) and its Affiliates. The Collateral Manager may decline to make a particular investment for the Issuer in view of such relationships.
-Unless the Collateral Manager determines in its sole discretion that such purchase or sale may be appropriate, the Collateral Manager may refrain from directing the purchase or sale hereunder of securities or obligations of (i) Persons of which the Collateral Manager, its Affiliates or any of its or their officers, directors, partners or employees are directors or officers, (ii) Persons for which the Collateral Manager or any of its Affiliates acts as financial adviser or underwriter or (iii) Persons about which the Collateral Manager or any of its Affiliates has information which the Collateral Manager deems confidential or non-public or otherwise might prohibit it from trading such securities or obligations in accordance with applicable law. The Collateral Manager shall not be obligated to utilize with respect to the Assets any particular investment opportunity of which it becomes aware or to pursue any particular investment strategy.
+          <t xml:space="preserve">7
 </t>
         </is>
       </c>
@@ -608,19 +557,18 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>3</t>
         </is>
       </c>
       <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Acquisitions from or Dispositions to the Collateral Manager and Related Parties</t>
+          <t>DUTIES OF CUSTODIAN</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t xml:space="preserve">Subject to compliance with applicable laws and regulations and subject to this Agreement and the applicable provisions of the Loan Sale Agreement and the Indenture, the Collateral Manager may direct the Trustee to acquire a Collateral Obligation from, or sell a Collateral
-Obligation, Eligible Investment or Equity Security to, the Collateral Manager, any of its Affiliates or any client for whom the Collateral Manager or any of its Affiliates serve as investment advisor. Any such acquisition by the Issuer shall be for Fair Market Value or as otherwise specified in the Indenture.
+          <t xml:space="preserve">8
 </t>
         </is>
       </c>
@@ -631,20 +579,18 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>4</t>
         </is>
       </c>
       <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Records; Confidentiality</t>
+          <t>REPORTING</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t xml:space="preserve">(a)The Collateral Manager shall maintain appropriate books of account and records relating to services performed hereunder, and such books of account and records shall be accessible for inspection by a representative of the Issuer, the Trustee and the Independent accountants appointed by the Collateral Manager on behalf of the Issuer pursuant to Article X of the Indenture at any time during normal business hours and upon not less than three Business Days' prior notice. The Collateral Manager shall provide the Issuer with sufficient information and reports to maintain the books and records of the Issuer.
-(b)The Collateral Manager shall keep confidential any and all information obtained in connection with the services rendered hereunder and shall not disclose any such information to non-affiliated third parties except (i) with the prior written consent of the Issuer, (ii) such information as any Rating Agency shall reasonably request in connection with its rating of the Notes, (iii) in connection with establishing trading or investment accounts or otherwise in connection with effecting transactions on behalf of the Issuer, (iv) as required by law, regulation, court order or the rules or regulations of any self-regulating organization, regulatory authority, body or official having jurisdiction over the Collateral Manager, (v) to its professional advisers or (vi) such information as shall have been publicly disclosed other than in violation of this Agreement. Notwithstanding the foregoing, the Collateral Manager (a) may present summary data with respect to the performance of the Assets in conjunction with presentation of performance statistics of other funds managed or to be managed by the Collateral Manager or its Affiliates, and may aggregate data with respect to the performance of one or more categories of Assets with similar data of such other funds and (b) may disclose such other information about the Issuer, the Assets and the Securities as is customarily disclosed by managers of collateralized loan obligations. For purposes of this Section 6, the Holders and beneficial owners of the Securities shall in no event be considered "non-affiliated third parties."
-(c)Notwithstanding anything in this Agreement or any other Transaction Document to the contrary, the Collateral Manager, the Issuers, the Trustee and the Holders and beneficial owners of the Securities (and each of their respective employees, representatives or other agents) may disclose to any and all Persons, without limitation of any kind, the U.S. tax treatment and U.S. tax structure (in each case, under applicable federal, state or local law) of the transactions contemplated by this Agreement and all materials of any kind (including opinions or other tax analyses) that are provided to them relating to such U.S. tax treatment and U.S. tax structure; provided that such U.S. tax treatment and U.S. tax structure shall be kept confidential to the extent reasonably necessary to comply with applicable U.S. federal or state laws.
+          <t xml:space="preserve">17
 </t>
         </is>
       </c>
@@ -655,19 +601,19 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>5</t>
         </is>
       </c>
       <c r="C9" t="inlineStr"/>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Obligations of the Collateral Manager</t>
+          <t>DEPOSIT IN U</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t xml:space="preserve">Unless otherwise specifically required by any provision of this Agreement, any other Transaction Document or applicable law, the Collateral Manager shall use commercially
-reasonable efforts to ensure that no action is taken by it, and shall not intentionally or with reckless disregard take any action, which would (a) materially adversely affect the Issuer for purposes of Cayman Islands law, United States federal or state law or any other law known to the Collateral Manager to be applicable to the Issuer, (b) not be permitted under the Issuers' Governing Instruments, (c) violate in any material respect any law, rule or regulation of any governmental body or agency having jurisdiction over the Issuer, including, without limitation, any Cayman Islands or United States federal, state or other applicable securities law, (d) require registration of the Issuer or the pool of Assets as an "investment company" under the Investment Company Act or (e) result in the Issuer or the Co-Issuer violating the terms of the Indenture. In connection with the foregoing, but without prejudice to Section 2 hereof, the Collateral Manager will not be required to make any independent investigation of any facts or laws in connection with its obligations under this Agreement or the conduct of its business generally. If the Collateral Manager is ordered to take any such action by the Issuer, the Collateral Manager shall promptly notify the Issuer, the Trustee and the Rating Agency of the Collateral Manager's judgment that such action would, or would reasonably be expected to, have one or more of the consequences set forth above and need not take such action unless (i) the action would not have the consequences set forth in clause (c) above and (ii) the Issuer again requests the Collateral Manager to do so and a Majority of each Class of Notes have consented thereto in writing. Notwithstanding any such request, the Collateral Manager need not take such action unless arrangements satisfactory to it are made to insure or indemnify the Collateral Manager from any liability it may incur as a result of such action. The Collateral Manager, its partners, their respective partners, and the Collateral Manager's directors, officers, stockholders and employees shall not be liable to the Issuer, the Trustee, the Holders or any other Person, except as provided in Section 10 of this Agreement. Any indemnification or insurance pursuant to this Section 7 that is payable out of the Assets shall be payable only in accordance with the priorities set forth in Article XI of the Indenture.
+          <t xml:space="preserve">S. SECURITIES SYSTEMS
+17
 </t>
         </is>
       </c>
@@ -678,23 +624,18 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>6</t>
         </is>
       </c>
       <c r="C10" t="inlineStr"/>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Compensation</t>
+          <t>SECURITIES HELD OUTSIDE OF THE UNITED STATES</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t xml:space="preserve">(a)The Issuer shall pay to the Collateral Manager, for services rendered and performance of its obligations under this Agreement, a fee, payable in arrears on each Payment Date (including any Redemption Date, other than a Redemption Date in connection with a redemption of Secured Notes in part by Class not occurring on a regularly scheduled Payment Date) in accordance with the Priority of Payments that consists of (i) an amount equal to 0.15% per annum (calculated on the basis of a 360 day year and the actual number of days elapsed during the related Interest Accrual Period) of the Fee Basis Amount measured as of the first day of the Collection Period relating to such Payment Date (the "Base Management Fee") and (ii) an amount equal to 0.20% per annum (calculated on the basis of a 360 day year and the actual number of days elapsed during the related Interest Accrual Period) of the Fee Basis Amount measured as of the first day of the Collection Period relating to such Payment Date (the "Subordinated Management Fee" and, together with the Base Management Fee, the "Management Fees"). If any portion of any Management Fee payable on any Payment Date in accordance with the Priority of Payments is not paid in full for any reason, such portion shall be deferred and remain due and payable on subsequent Payment Dates.
-(b)The Collateral Manager may, in its sole discretion, waive its rights to receive any portion of the Management Fees payable on any Payment Date. The Collateral
-Manager hereby waives its rights to receive all Management Fees until such date as the Collateral Manager notifies the Issuer and the Trustee that it is revoking such waiver.
-(c)If this Agreement is terminated for any reason, or if the Collateral Manager resigns or is removed, the Base Management Fee and the Subordinated Management Fee will each be prorated for any partial period elapsing from the last Payment Date on which such Collateral Manager was entitled to receive the Base Management Fee and the Subordinated Management Fee to the effective date of such termination, resignation or removal and shall be immediately due and payable on each Payment Date following the effective date of such termination, resignation or removal in accordance with the Priority of Payments until paid in full. Otherwise, such Collateral Manager shall not be entitled to any further compensation for further services but shall be entitled to receive any expense reimbursement accrued to the effective date of termination, resignation or removal and any indemnity amounts owing (or that may become owing) under this Agreement. Any Management Fee, expense reimbursement and indemnities owed to such Collateral Manager or owed to any successor Collateral Manager on any Payment Date shall be paid pro rata based on the amount thereof then owing to each such Person, subject to the Priority of Payments.
-(d)The Collateral Manager shall be responsible for expenses incurred in the performance of its obligations under this Agreement; provided, however, the Issuer will pay or reimburse the Collateral Manager for expenses including fees and out-of-pocket expenses reasonably incurred by the Collateral Manager in connection with the services provided under this Agreement with respect to (i) the costs and expenses of the Collateral Manager incurred in connection with the negotiation, preparation and execution of this Agreement and all other agreements and matters related to the issuance of any Securities; (ii) any transfer fees necessary to register any Collateral Obligation in accordance with the Indenture; (iii) any fees and expenses in connection with the acquisition, management or disposition of Assets or otherwise in connection with the Securities or the Issuer (including (a) investment related travel, communications and related expenses, (b) loan processing fees, accounting and legal fees and expenses (including internally allocated expenses) and other expenses of professionals retained by the Collateral Manager on behalf of the Issuer and (c) amounts in connection with the termination, cancellation or abandonment of a potential acquisition or disposition of any Assets that is not consummated); (iv) any and all taxes, regulatory and governmental charges that may be incurred or payable by the Issuer; (v) any and all insurance premiums or expenses incurred in connection with the activities of the Issuer by the Collateral Manager; (vi) any and all costs, fees and expenses incurred in connection with the rating of the Secured Notes or obtaining ratings or credit estimates on Collateral Obligations, and communications with the Rating Agency; (vii) any and all costs, fees and expenses incurred in connection with the Collateral Manager's communications with the Holders (including charges related to annual meetings and for preparation of reports); (viii) costs, fees and expenses of one or more firms that provide software databases and applications for the purpose of modeling, evaluating and monitoring the Assets and the Securities pursuant to a licensing or other agreement; (ix) fees and expenses for services to the Issuer in respect of the Assets relating to asset pricing and rating services; (x) any and all expenses incurred to comply with any law or regulation related to the activities of the Issuer and, to the extent relating to the Issuer and the Assets, the Collateral Manager; (xi) the fees and expenses of any independent advisor employed to value or consider Collateral Obligations; (xii) any and all costs, fees and expenses incurred in connection with any amendment or supplemental indenture effected (or proposed to be effected) pursuant to the Indenture; (xiii) in the event the Issuer is included in the
-consolidated financial statements of the Collateral Manager or its Affiliates, costs and expenses associated with the preparation of such financial statements and other information by the Collateral Manager or its Affiliates to the extent related to the inclusion of the Issuer in such financial statements; (xiv) any and all costs, fees and expenses incurred in connection with the preparation and audit of the Issuer's financial statements; (xv) any out-of-pocket costs or expenses incurred by the Collateral Manager in connection with complying with applicable law; and (xvi) as otherwise agreed upon by the Issuer and the Collateral Manager, to be paid in accordance with the Indenture. In addition, the Issuer will pay or reimburse the costs and expenses (including fees and disbursements of counsel and accountants) of the Collateral Manager and the Issuer incurred in connection with or incidental to the entering into of this Agreement or any amendment hereto.
+          <t xml:space="preserve">18
 </t>
         </is>
       </c>
@@ -705,18 +646,18 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>7</t>
         </is>
       </c>
       <c r="C11" t="inlineStr"/>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Benefit of the Agreement</t>
+          <t>CERTAIN GENERAL TERMS</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t xml:space="preserve">The Collateral Manager shall perform its obligations hereunder in accordance with the terms of this Agreement and the terms of the Indenture applicable to it and shall use all reasonable endeavors, in the course of carrying out such obligations, to protect the interests of the Holders as a group. The Collateral Manager agrees that such obligations shall be enforceable at the instance of the Issuer, the Trustee, on behalf of the Holders, or the requisite percentage of Holders as provided in the Indenture.
+          <t xml:space="preserve">21
 </t>
         </is>
       </c>
@@ -727,36 +668,18 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>8</t>
         </is>
       </c>
       <c r="C12" t="inlineStr"/>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Limits of Collateral Manager Responsibility</t>
+          <t>COMPENSATION OF CUSTODIAN</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t xml:space="preserve">(a)The Collateral Manager assumes no responsibility under this Agreement other than to render the services called for hereunder and under the terms of the Indenture applicable to it in good faith and shall not be responsible for any action or inaction of the Issuer or the Trustee in following or declining to follow any advice, recommendation or direction of the Collateral Manager. The Collateral Manager, its Affiliates, and their respective Related Persons shall not be liable to the Issuers, the Trustee, any Holder of Securities, any holder of the Issuer's ordinary shares, the Initial Purchaser, any of their respective Affiliates or Related Persons or any other Person for any act, omission, error of judgment, mistake of law, or for any claim, loss, liability, damage, judgements, assessments, settlement cost, or other expense (including attorneys' fees and expenses and court costs) arising out of any investment, or for any other act or omission in the performance of the Collateral Manager's obligations under or in connection with this Agreement or the terms of any other Transaction Document applicable to the Collateral Manager, incurred as a result of actions taken or recommended or for any omissions of the Collateral Manager, or for any decrease in the value of the Assets, except the Collateral Manager will be liable (i) by reason of acts or omissions constituting bad faith, willful misconduct or gross negligence in the performance of its duties under this Agreement and under the terms of the Indenture or (ii) with respect to the Collateral Manager Information, as of the date made, containing any untrue statement of a material fact or omitting to state a material fact necessary in order to make the statements in the Offering Circular, in light of the circumstances under which they were made, not misleading (the preceding clauses (i) and (ii) collectively referred to as "Collateral Manager Breaches").
-(b)The Collateral Manager shall not be liable for any consequential, punitive, exemplary or special damages or lost profits under this Agreement or under the Indenture. Nothing
-contained in this Agreement shall be deemed to waive any liability which cannot be waived under applicable state or federal law or any rules or regulations thereunder.
-(c)Indemnity by the Issuer. The Issuer shall indemnify and hold harmless (the Issuer in such case, the "Indemnifying Party") the Collateral Manager, its Affiliates, and their respective Related Persons (such parties collectively in such case, the "Indemnified Parties") from and against any and all losses, claims, damages, judgments, assessments, costs or other liabilities (collectively, "Losses") (as Administrative Expenses) and will promptly reimburse each such Indemnified Party for all reasonable fees and expenses incurred by an Indemnified Party with respect thereto (including, without limitation, reasonable fees and expenses of counsel and costs of collection) (collectively, "Expenses") (as Administrative Expenses) arising out of or in connection with the issuance of the Securities (including, without limitation, any untrue statement of material fact or alleged untrue statement of material fact contained in the Offering Circular, or any omission or alleged omission to state in the Offering Circular a material fact necessary in order to make the statements therein, in the light of the circumstances under which they were made, not misleading, other than Collateral Manager Information), the transactions contemplated by the Offering Circular, the Indenture or this Agreement and any acts or omissions of any such Indemnified Party; provided that such Indemnified Party shall not be indemnified for any Losses or Expenses incurred as a result of any Collateral Manager Breach or any information contained under the headings "U.S. Credit Risk Retention" and "EU Risk Retention Requirements--The Retention Holder" in the Offering Circular as of the date made containing any untrue statement of a material fact or omitting to state a material fact necessary in order to make the statements in the Offering Circular, in light of the circumstances under which they were made, not misleading.
-(d)Notwithstanding anything contained herein to the contrary, the obligations of the Issuer under this Section 10 shall be limited-recourse obligations of the Issuer, payable solely out of the Assets in accordance with the priorities set forth in Article XI of the Indenture and shall be subject to the terms of Section 22 hereof. 
-(e)Notwithstanding anything to the contrary contained in this Agreement, the provisions of this Agreement shall not be construed so as to provide for the exculpation of the Collateral Manager or the indemnification of the Issuer or the Collateral Manager for any liability (including liability under U.S. federal securities laws), to the extent (but only to the extent) that such liability may not be waived, modified or limited under applicable law or such indemnification may not be demanded under applicable law, but shall otherwise be construed so as to effectuate the provisions of this Agreement to the fullest extent permitted by applicable law.
-(f)In providing services under this Agreement, the Collateral Manager may rely in good faith upon and will be fully protected and incur no liability for acting at the direction of the Issuer (where such direction has been given without direct advice from the Collateral Manager) or for relying upon advice of nationally recognized counsel, accountants or other advisers as the Collateral Manager determines, in its sole discretion, is reasonably appropriate in connection with the services provided by the Collateral Manager under this Agreement.
-(g)An Indemnified Party shall (or with respect to an Indemnified Party other than the Collateral Manager, the Collateral Manager shall cause such Indemnified Party to) promptly notify the Indemnifying Party if the Indemnified Party receives a complaint, claim,
-compulsory process or other notice of any loss, claim, damage or liability giving rise to a claim for indemnification under this Section 10 and give written notice to the Indemnifying Party of such claim within ten (10) days after such claim is made or threatened, which notice shall specify in reasonable detail the nature of the claim and the amount (or an estimate of the amount) of the claim but failure so to notify the Indemnifying Party (i) shall not relieve such Indemnifying Party from its obligations under paragraph (a) above unless and to the extent that it did not otherwise learn of such action or proceeding and to the extent such failure results in the forfeiture by the Indemnifying Party of substantial rights and defenses and (ii) shall not, in any event, relieve the Indemnifying Party for any obligations to any Person entitled to indemnity pursuant to paragraph (a) above other than the indemnification obligations provided for in paragraph (a) above.
-(h)With respect to any claim made or threatened against an Indemnified Party, or compulsory process or request served upon such Indemnified Party for which such Indemnified Party is or may be entitled to indemnification under this Section 10, such Indemnified Party shall (or with respect to an Indemnified Party other than the Collateral Manager, the Collateral Manager shall cause such Indemnified Party to), at the Indemnifying Party's expense:
-(i)provide the Indemnifying Party such information and cooperation with respect to such claim as the Indemnifying Party may reasonably require, including, but not limited to, making appropriate personnel available to the Indemnifying Party at such reasonable times as the Indemnifying Party may request;
-(ii)cooperate and take all such steps as the Indemnifying Party may reasonably request to preserve and protect any defense to such claim;
-(iii)in the event suit is brought with respect to such claim, upon reasonable prior notice, afford to the Indemnifying Party the right, which the Indemnifying Party may exercise in its sole discretion and at its expense, to participate in the investigation, defense and settlement of such claim;
-(iv)neither incur any material expense to defend against nor release or settle any such claim or make any admission with respect thereto (other than routine or incontestable admissions or factual admissions the failure to make which would expose such Indemnified Party to unindemnified liability) without the prior written consent of the Indemnifying Party; provided, that the Indemnifying Party shall have advised such Indemnified Party that such Indemnified Party is entitled to be indemnified hereunder with respect to such claim; and
-(v)upon reasonable prior notice, afford to the Indemnifying Party the right, in its sole discretion and at its sole expense, to assume the defense of such claim, including, but not limited to, the right to designate counsel and to control all negotiations, litigation, arbitration, settlements, compromises and appeals of such claim; provided, that if the Indemnifying Party assumes the defense of such claim, it shall not be liable for any fees and expenses of counsel for any Indemnified Party incurred thereafter in connection with such claim except that if such Indemnified Party reasonably determines that counsel designated by the Indemnifying Party has a conflict of interest, such Indemnifying Party shall pay the reasonable fees and disbursements of one counsel (in addition to any local
-counsel) separate from its own counsel for all Indemnified Parties in connection with any one action or separate but similar or related actions in the same jurisdiction arising out of the same general allegations or circumstances; and provided further, that prior to entering into any final settlement or compromise, such Indemnifying Party shall seek the consent of the Indemnified Party and use its best efforts in the light of the then prevailing circumstances (including, without limitation, any express or implied time constraint on any pending settlement offer) to obtain the consent of such Indemnified Party as to the terms of settlement or compromise. If an Indemnified Party does not consent to the settlement or compromise within a reasonable time under the circumstances, the Indemnifying Party shall not thereafter be obligated to indemnify the Indemnified Party for any amount in excess of such proposed settlement or compromise.
-(i)No Indemnified Party shall, without the prior written consent of the Indemnifying Party, which consent shall not be unreasonably withheld or delayed, settle or compromise any claim giving rise to a claim for indemnity hereunder, or permit a default or consent to the entry of any judgment in respect thereof, unless such settlement, compromise or consent includes, as an unconditional term thereof, the giving by the claimant to the Indemnifying Party of a release from liability substantially equivalent to the release given by the claimant to such Indemnified Party in respect of such claim.
-(j)In the event that any Indemnified Party waives its right to indemnification hereunder, the Indemnifying Party shall not be entitled to appoint counsel to represent such Indemnified Party nor shall the Indemnifying Party reimburse such Indemnified Party for any costs of counsel to such Indemnified Party.
-(k)Indemnity by Collateral Manager. The Collateral Manager shall indemnify, defend and hold harmless the Issuer and its Related Persons from and against any and all Losses and shall reimburse each such Person for all Expenses in investigating, preparing, pursuing or defending any claim, action, proceeding or investigation with respect to any pending or threatened litigation against the Issuer or any such Related Person (collectively, "Actions"), to the extent that such Action is caused by, or is a direct consequence of, any Collateral Manager Breach; provided that no such indemnity shall be paid to the extent that such Action was caused by, or arose out of or in connection with, bad faith, willful misconduct, gross negligence or reckless disregard of the Issuer or any Related Person.
+          <t xml:space="preserve">24
 </t>
         </is>
       </c>
@@ -767,31 +690,18 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>9</t>
         </is>
       </c>
       <c r="C13" t="inlineStr"/>
       <c r="D13" t="inlineStr">
         <is>
-          <t>No Partnership or Joint Venture</t>
+          <t>RESPONSIBILITY OF CUSTODIAN</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t xml:space="preserve">The Issuer and the Collateral Manager are not partners or joint venturers with each other and nothing herein shall be construed to make them such partners or joint venturers or impose any liability as such on either of them. The Collateral Manager's relation to the Issuer shall be deemed to be solely that of an independent contractor.
-12.Term; Termination.
-(a)This Agreement shall commence as of the date first set forth above and shall continue in force until the first of the following occurs: (i) the payment in full of the Notes and the termination of the Indenture in accordance with its terms; (ii) the liquidation of the Assets and the
-final distribution of the proceeds of such liquidation pursuant to the terms of the Indenture; or (iii) the termination of this Agreement in accordance with clause (b) or (c) of this Section 12 or Section 14 of this Agreement.
-(b)This Agreement may be terminated without cause by the Collateral Manager, and the Collateral Manager may resign upon 90 days' prior written notice (or such shorter notice as is acceptable to the Issuer) to the Issuer, the Trustee (who will forward such notice to each Holder), and the Rating Agency; provided, however, that the Collateral Manager shall have the right to resign immediately upon the effectiveness of any material change in applicable law or regulations which renders the performance by the Collateral Manager of its duties under the Collateral Management Agreement or under the Indenture to be a violation of such law or regulation. No such termination or resignation shall be effective until the date as of which a successor collateral manager shall have been appointed in accordance with this Agreement and delivered an instrument of acceptance to the Issuer and the resigned Collateral Manager and the successor collateral manager has effectively assumed all of the Collateral Manager's duties and obligations pursuant to this Agreement.
-(c)If this Agreement is terminated pursuant to this Section 12, such termination shall be without any further liability or obligation of either party to the other, except as provided in Sections 8(c), 10, 15 and 22 of this Agreement, which provisions shall survive the termination of this Agreement.
-(d)Promptly after notice of any removal for Cause pursuant to Section 14 hereof or resignation of the Collateral Manager pursuant to this Section 12 while any Securities are Outstanding, the Issuer shall:
-(i)transmit copies of such notice to the Trustee (who shall forward a copy of such notice to the Holders), the Fiscal Agent and the Rating Agency; and
-(ii)at the direction of a Majority of the Preferred Shares appoint as a successor collateral manager any institution that (A) has demonstrated an ability to professionally and competently perform duties similar to those imposed upon the Collateral Manager hereunder, (B) is legally qualified and has the capacity to assume all of the duties, responsibilities and obligations of the Collateral Manager hereunder and under the applicable terms of the Indenture, (C) does not cause the Issuer or the Co-Issuer or the pool of Assets to become required to register under the Investment Company Act, (D) has been approved by a Majority of the Controlling Class and a Majority of the Preferred Shares (provided, for the avoidance of doubt, that if a Majority of the Controlling Class or a Majority of the Preferred Shares has nominated such successor, it shall be deemed to have approved of such successor) and (E) does not by its appointment cause the Issuer or the Co-Issuer to be treated as a publicly traded partnership taxable as a corporation for U.S. federal income tax purposes or subject to U.S. federal, state or local income tax on a net income basis (including any tax liability imposed under Section 1446 of the Code).
-(e)If (i) a Majority of the Preferred Shares fails to nominate a successor within 30 days of initial notice of the resignation or removal of the Collateral Manager or (ii) a Majority of the Controlling Class does not approve the proposed successor nominated by the holders of the
-Preferred Shares within 10 days of the date of the notice of such nomination, then a Majority of the Controlling Class shall, within 60 days of the failure described in clause (i) or (ii) of this sentence, as the case may be, nominate a successor Collateral Manager that meets the criteria set forth in clause (d)(ii) above. If a Majority of the Preferred Shares approves such proposed successor nominated pursuant to the preceding sentence, such nominee shall become the Collateral Manager. If no successor Collateral Manager is appointed within 90 days (or, in the event of a change in applicable law or regulation which renders the performance by the resigning Collateral Manager of its duties under this Agreement or the Indenture to be a violation of such law or regulation, within 30 days) following the termination or resignation of the Collateral Manager, any of the Collateral Manager, a Majority of the Preferred Shares and the Majority of the Controlling Class shall have the right to petition a court of competent jurisdiction to appoint a successor Collateral Manager, in either such case whose appointment shall become effective after such successor has accepted its appointment and without the consent of any Holder of any Securities.
-(f)Any successor Collateral Manager shall be entitled to the Base Management Fee and the Subordinated Management Fee accruing from the effective date of its appointment. No compensation payable to such successor Collateral Manager shall be greater than such components of the Management Fee without the prior written consent of 100% of the Holders of each Class of Securities, including Collateral Manager Securities.
-(g)The Issuer, the Trustee and the successor collateral manager shall take such action (or cause the outgoing Collateral Manager to take such action) consistent with this Agreement and the terms of the Indenture applicable to the Collateral Manager, as shall be necessary to effectuate any such succession. Promptly following the appointment of a successor collateral manager in accordance with the foregoing, the Issuer shall provide written notice thereof to the Rating Agency.
-(h)In the event of removal of the Collateral Manager pursuant to this Agreement by the Issuer, the Issuer shall have all of the rights and remedies available with respect thereto at law or equity, and, without limiting the foregoing, the Issuer may by notice in writing to the Collateral Manager as provided under this Agreement terminate all the rights and obligations of the Collateral Manager under this Agreement (except those that survive termination pursuant to Section 12(c) above). Upon expiration of the applicable notice period with respect to termination specified in this Section 12 or Section 14 of this Agreement, as applicable, all authority and power of the Collateral Manager under this Agreement, whether with respect to the Assets or otherwise, shall automatically and without further action by any person or entity pass to and be vested in the successor collateral manager upon the appointment thereof. Nevertheless, the Collateral Manager shall take such steps as may be reasonably necessary to transfer such authority and power.
+          <t xml:space="preserve">24
 </t>
         </is>
       </c>
@@ -802,43 +712,18 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>10</t>
         </is>
       </c>
       <c r="C14" t="inlineStr"/>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Delegation; Assignments; Succession</t>
+          <t>SECURITY CODES</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t xml:space="preserve">(a)Except as provided in this Agreement, the Collateral Manager may not assign or delegate its rights or responsibilities under this Agreement without obtaining the consent of the Issuer and the consent of a Majority of the Controlling Class and a Majority of the Preferred Shares (voting separately).
-(b)The Collateral Manager may, without obtaining the consent of any Holder of Securities, but subject to any consent of the Issuer required for an assignment under the Advisers Act, assign any of its rights or obligations under this Agreement to an Affiliate of the Collateral Manager, to the surviving entity of a merger, consolidation or restructuring of the Collateral Manager, or to any other entity to which all or substantially all of the assets, or at the time of such transfer, the collateral management business, of the Collateral Manager has been transferred; provided that such Affiliate, successor or transferee (i) has demonstrated an ability to professionally and competently perform duties similar to those imposed upon the Collateral Manager pursuant to this Agreement, (ii) has the legal right and capacity to act as Collateral Manager under this Agreement, (iii) shall not cause any of the Issuer, the Co-Issuer or the pool of Assets to become required to register under the provisions of the 1940 Act and (iv) by its appointment will not cause the Issuer or Co-Issuer to be treated as a publicly traded partnership taxable as a corporation for U.S. federal income tax purposes or subject to U.S. federal, state or local income tax on a net income basis (including any tax liability imposed under Section 1446 of the Code). The Collateral Manager shall deliver prior notice to the Rating Agency of any such assignment or combination.
-(c)In addition, the Collateral Manager may, without the consent of any Person, delegate to third parties (including without limitation its Affiliates) the duties assigned to the Collateral Manager under this Agreement, and employ third parties (including without limitation its Affiliates) to render advice (including investment advice), to provide services to arrange for trade execution and otherwise provide assistance to the Issuer, and to perform any of the Collateral Manager's duties under this Agreement; provided that the Collateral Manager shall not (i) delegate investment advice responsibilities, including (without limitation) asset selection, credit review and the negotiation and determination of the acquisition price of a Collateral Obligation to non-affiliates; (ii) be relieved of any of its duties under this Agreement regardless of the performance of any services by third parties; or (iii) by its appointment cause the Issuer or the Co-Issuer to be treated as a publicly traded partnership taxable as a corporation for U.S. federal income tax purposes or subject to U.S. federal, state or local income tax on a net income basis (including any tax liability imposed under Section 1446 of the Code).
-(d)Any assignment by the Collateral Manager consented to by the Issuer and the required Holders shall bind the assignee hereunder in the same manner as the Collateral Manager is bound. In addition, the assignee shall execute and deliver to the Issuer and the Trustee an appropriate agreement naming such assignee as a Collateral Manager. Upon the execution and delivery of such a counterpart by the assignee, the Collateral Manager shall be released from further obligations pursuant to this Agreement, except with respect to its obligations under Section 10 of this Agreement arising prior to such assignment and except with respect to its obligations under Sections 15 and 22 hereof. 
-(e)This Agreement shall not be assigned by the Issuer without the prior written consent of the Collateral Manager, except that the Collateral Manager agrees and consents to the assignment by the Issuer of this Agreement pursuant to Section 15.1(f) of the Indenture.
-(f)In the event of any assignment by the Issuer, the Issuer shall (x) use its best efforts to cause its successor to execute and deliver to the Collateral Manager such documents as
-the Collateral Manager shall consider reasonably necessary to effect fully such assignment and (y) provide written notice thereof to the Issuer, each Holder, the Trustee and the Rating Agency.
-14.Termination by the Issuer for Cause.
-This Agreement may be terminated, and the Collateral Manager may be removed for Cause (as defined below) upon 30 Business Days' prior written notice by the Issuer (a "Termination Notice") at the direction of either (i) a Majority of the Controlling Class or (ii) a Majority of the Preferred Shares; provided that Collateral Manager Securities shall be disregarded and have no voting rights with respect to any vote in respect of removal of the Collateral Manager for Cause. Simultaneous with its direction to the Issuer to so remove the Collateral Manager, either (i) a Majority of the Controlling Class or (ii) a Majority of the Preferred Shares (as applicable) shall give to the Issuer a written statement setting forth the reason for such removal (a "Notice of Removal") and the Issuer shall deliver a copy of the Termination Notice and the Notice of Removal to the Trustee (who shall deliver a copy of such notice to the Holders) within five Business Days of receipt of such written notice. No such termination or removal pursuant to this Section 14 shall be effective (A) until the date as of which a successor collateral manager shall have been appointed in accordance with Section 12 and have delivered an instrument of acceptance to the Issuer and the removed Collateral Manager and the successor collateral manager has effectively assumed all of the Collateral Manager's duties and obligations under this Agreement and the Indenture and (B) unless the Notice of Removal shall have been delivered to the Issuer as set forth above.
-For purposes of determining "Cause" with respect to termination of this Agreement pursuant to this Section 14, such term shall mean any one of the following events:
-(a)the Collateral Manager willfully and intentionally violated or breached any material provision of this Agreement or the Indenture applicable to it (not including a willful and intentional breach that results from a good faith dispute regarding reasonable alternative courses of action or reasonable interpretation of instructions);
-(b)the Collateral Manager breached any provision of this Agreement or any terms of the Indenture applicable to it (other than as covered by clause (a) above and it being understood that failure to meet any Concentration Limitation, Collateral Quality Test or Coverage Test is not a breach for purposes of this clause (b)), which breach would reasonably be expected to have a material adverse effect on any Class of Secured Notes and shall not cure such breach (if capable of being cured) within 60 days after the earlier to occur of a Responsible Officer of the Collateral Manager receiving notice or having actual knowledge of such breach, unless, if such breach is remediable, the Collateral Manager has taken action commencing the cure thereof within such 60 day period that the Collateral Manager believes in good faith will remedy such breach within 90 days after the earlier to occur of a Responsible Officer receiving notice or having actual knowledge thereof;
-(c)the failure of any representation or warranty of the Collateral Manager in Section 16 hereof to be correct in any material respect when such representation or warranty is made, which failure (i) would reasonably be expected to have a material adverse effect on any Class of Secured Notes and (ii) if capable of being corrected, is not corrected by the Collateral Manager within 45 days of a Responsible Officer of the Collateral Manager receiving notice of
-such failure, unless if such failure is remediable, the Collateral Manager has taken action commencing the cure thereof within such 45-day period that the Collateral Manager believes in good faith will remedy such failure within 90 days after the earlier to occur of a Responsible Officer receiving notice thereof or having actual knowledge thereof;
-(d)(A) the Collateral Manager is wound up or dissolved; (B) there is appointed over the Collateral Manager or a substantial portion of its assets a receiver, administrator, administrative receiver, trustee or similar officer; or (C) the Collateral Manager (i) ceases to be able to, or admits in writing its inability to, pay its debts as they become due and payable, or makes a general assignment for the benefit of, or enters into any composition or arrangement with, its creditors generally; (ii) applies for or consents (by admission of material allegations of a petition or otherwise) to the appointment of a receiver, trustee, assignee, custodian, liquidator or sequestrator (or other similar official) of the Collateral Manager or of any substantial part of its properties or assets, or authorizes such an application or consent, or proceedings seeking such appointment are commenced without such authorization, consent or application against the Collateral Manager and continue undismissed for 60 days; (iii) authorizes or files a voluntary petition in bankruptcy, or applies for or consents (by admission of material allegations of a petition or otherwise) to the application of any bankruptcy, reorganization, arrangement, readjustment of debt, insolvency or dissolution, or authorizes such application or consent, or proceedings to such end are instituted against the Collateral Manager without such authorization, application or consent and are approved as properly instituted and remain undismissed for 60 days or result in adjudication of bankruptcy or insolvency; or (iv) permits or suffers all or any substantial part of its properties or assets to be sequestered or attached by court order and the order remains undismissed for 60 days;
-(e)the occurrence and continuation of an Event of Default specified under clause (a), (b) or (c) of the definition of such term that results primarily from any material breach by the Collateral Manager of its duties under this Agreement or under the Indenture which breach or default is not cured within any applicable cure period (excluding any such Event of Default relating to a good faith dispute with respect to reasonable alternative courses of action or the meaning of any relevant provision under the Transaction Documents or any matter that is in the process of being reconciled in accordance with the applicable Transaction Documents); or
-(f)(i) the occurrence of an act by the Collateral Manager that constitutes fraud or felony criminal activity in the performance of its obligations under this Agreement (as determined pursuant to a final adjudication by a court of competent jurisdiction) or the Collateral Manager being indicted for a felony criminal offense materially related to its business of providing asset management services or (ii) any Responsible Officer of the Collateral Manager primarily responsible for the performance by the Collateral Manager of its obligations under this Agreement (in the performance of his or her investment management duties) is indicted for a felony criminal offense materially related to the business of the Collateral Manager providing asset management services and continues to have responsibility for the performance by the Collateral Manager under this Agreement for a period of thirty (30) days after such indictment.
-Prior to the effective appointment of any successor collateral manager in accordance with this Agreement, the event or circumstance giving rise to the removal of the Collateral Manager for Cause described above (other than pursuant to clause (d) of the definition thereof) may be waived
-by a written approval of both a Majority of the Controlling Class and a Majority of the Preferred Shares (voting separately) as a basis for termination of this Agreement and removal of the Collateral Manager hereunder; provided that Collateral Manager Securities shall be disregarded and have no voting rights for purposes of this waiver, it being understood that if all of the Securities of either such Class are Collateral Manager Securities, the approval of a Majority of such Class shall not be required for such waiver.
-If any of the events specified in clauses (a) through (f) of this Section 14 shall occur, the Collateral Manager shall give prompt written notice thereof to the Issuer, the Trustee (who shall forward such notice to the Holders) and the Rating Agency; provided that if the events specified in clause (d) above shall occur, the Collateral Manager shall give written notice thereof to the Issuer, the Trustee (who will forward such notice to the holders of the Securities) and the Rating Agency immediately upon the Collateral Manager's becoming aware of the occurrence of such event. In no event will the Trustee be required to determine whether or not Cause exists to remove the Collateral Manager.
-15.Action Upon Termination.
-(a)From and after the effective date of termination of this Agreement, the Collateral Manager shall not be entitled to compensation for further services hereunder, but shall be paid all compensation to which it is entitled, and shall receive all other amounts for which it is entitled to reimbursement, all as provided in and subject to Section 8 hereof, and shall be entitled to receive any amounts owing under Sections 7 and 10 hereof. Upon such termination, the Collateral Manager shall as soon as practicable:
-(i)deliver to and at the direction of the Issuer all property and documents of the Trustee or the Issuer or otherwise relating to the Assets then in the custody of the Collateral Manager; and
-(ii)deliver to the Trustee an accounting with respect to the books and records delivered to the Trustee or the successor collateral manager appointed pursuant to Section 12(d) hereof.
-Notwithstanding such termination, the Collateral Manager shall remain liable for its acts or omissions hereunder as described in Section 10 arising prior to termination and for any expenses, losses, damages, liabilities, demands, charges and claims of any nature whatsoever (including reasonable attorneys' fees) in respect of or arising out of a breach of the representations and warranties made by the Collateral Manager in Section 16(b) hereof or from any failure of the Collateral Manager to comply in all material respects with the provisions of this Section 15.
-(b)The Collateral Manager agrees that, notwithstanding any termination, it shall reasonably cooperate in any Proceeding arising in connection with this Agreement, the Indenture or any of the Assets (excluding any such Proceeding in which claims are asserted against the Collateral Manager or any Affiliate of the Collateral Manager) upon receipt of appropriate indemnification and expense reimbursement.
+          <t xml:space="preserve">27
 </t>
         </is>
       </c>
@@ -849,34 +734,18 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>11</t>
         </is>
       </c>
       <c r="C15" t="inlineStr"/>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Representations and Warranties</t>
+          <t>TAX LAW</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t xml:space="preserve">(a)The Issuer hereby represents and warrants to the Collateral Manager as follows:
-(i)The Issuer has been duly incorporated and is validly existing under the laws of the Cayman Islands, has all requisite corporate power and authority to own its assets and the securities proposed to be owned by it and included in the Assets and to transact the business in which it is presently engaged and is duly qualified under the laws of each jurisdiction where its ownership or lease of property or the conduct of its business requires, or the performance of its obligations under this Agreement, the Indenture or the Securities would require, such qualification, except for failures to be so qualified, authorized or licensed that would not in the aggregate have a material adverse effect on the business, operations, assets or financial condition of the Issuer.
-(ii)The Issuer has all requisite corporate power and authority to execute, deliver and perform this Agreement, the Indenture and the Securities and all obligations required hereunder, under the Indenture and the Securities and has taken all necessary action to authorize the execution, delivery and performance of this Agreement, the Indenture and the Securities and the performance of all obligations imposed upon it hereunder and thereunder. No consent of any other Person including, without limitation, shareholders and creditors of the Issuer, and no license, permit, approval or authorization of, exemption by, notice or report to, or registration, filing or declaration with, any governmental authority, other than those that may be required under state securities or "blue sky" laws and those that have been or shall be obtained in connection with the Indenture and the issuance of the Securities, is required by the Issuer in connection with this Agreement, the Indenture or the Securities or the execution, delivery, performance, validity or enforceability of this Agreement, the Indenture or the Securities or the obligations imposed upon it hereunder or thereunder. This Agreement constitutes, and each instrument or document required hereunder, when executed and delivered hereunder, shall constitute, the legally valid and binding obligations of the Issuer enforceable against the Issuer in accordance with its terms, subject, as to enforcement, to (a) the effect of bankruptcy, insolvency or similar laws affecting generally the enforcement of creditors' rights, as such laws would apply in the event of any bankruptcy, receivership, insolvency or similar event applicable to the Issuer and (b) general equitable principles (whether enforceability of such principles is considered in a proceeding at law or in equity).
-(iii)The execution, delivery and performance of this Agreement and the documents and instruments required hereunder shall not violate any provision of any existing law or regulation binding on the Issuer, or any order, judgment, award or decree of any court, arbitrator or governmental authority binding on or applicable to the Issuer, or the Governing Instruments of, or any securities issued by, the Issuer or of any mortgage, indenture, lease, contract or other agreement, instrument or undertaking to which the Issuer is a party or by which the Issuer or any of its assets is or may be bound, the violation of which would have a material adverse effect on the business, operations, assets or financial condition of the Issuer, and shall not result in or require the creation or imposition of any lien on any of its property, assets or revenues pursuant to the provisions of any such mortgage, indenture, lease, contract or other agreement, instrument or undertaking (other than the lien of the Indenture).
-(iv)The Issuer is not in violation of its Governing Instruments or in breach or violation of or in default under the Indenture or any contract or agreement to which it is a party or by which it or any of its assets may be bound, or any applicable statute or any rule, regulation or order of any court, government agency or body having jurisdiction over the Issuer or its properties, the breach or violation of which or default under which would have a material adverse effect on the validity or enforceability of this Agreement or the performance by the Issuer of its duties hereunder.
-(v)True and complete copies of the Indenture and the Issuer's Governing Instruments have been or, no later than the Closing Date, will be delivered to the Collateral Manager. In addition, the Issuer acknowledges that it has received Part 2 of the Collateral Manager's Form ADV filed with the Securities and Exchange Commission, as required by Rule 204-3 under the Advisers Act, prior to or concurrently with the date of execution of this Agreement.
-The Issuer agrees to deliver a true and complete copy of each and every amendment to the documents referred to in Section 16(a)(v) above to the Collateral Manager as promptly as practicable after its adoption or execution.
-(b)The Collateral Manager hereby represents and warrants to the Issuer as follows:
-(i)The Collateral Manager is a limited liability company duly organized and validly existing and in good standing under the law of the State of Delaware and has full power and authority to own its assets and to transact the business in which it is currently engaged and is duly qualified as a limited liability company and is in good standing under the laws of each jurisdiction where its ownership or lease of property or the conduct of its business requires, or the performance of this Agreement would require such qualification, except for those jurisdictions in which the failure to be so qualified, authorized or licensed would not have a material adverse effect on the business, operations, assets or financial condition of the Collateral Manager or on the ability of the Collateral Manager to perform its obligations under, or on the validity or enforceability of, this Agreement and the provisions of the Indenture which are applicable to the Collateral Manager; the Collateral Manager is a registered investment adviser under the United States Investment Advisers Act of 1940, as amended (the "Advisers Act").
-(ii)The Collateral Manager has full power and authority to execute and deliver this Agreement and perform all obligations required hereunder and under the provisions of the Indenture which are applicable to the Collateral Manager, and the Collateral Manager has taken all necessary action to authorize this Agreement on the terms and conditions hereof and the execution, delivery and performance of this Agreement and all obligations required hereunder and under the terms of the Indenture which are applicable to the Collateral Manager. No consent of any other person, including, without limitation, creditors of the Collateral Manager, and no license, permit, approval or authorization of, exemption by, notice or report to, or registration, filing or declaration with, any governmental authority (other than those already obtained) is required by the Collateral Manager in connection with this Agreement or the execution, delivery,
-performance, validity or enforceability of this Agreement or the obligations required hereunder or under the terms of the Indenture which are applicable to the Collateral Manager. This Agreement has been, and each instrument and document required hereunder or under the terms of the Indenture shall be, executed and delivered by a duly authorized officer of the Collateral Manager, and this Agreement constitutes, and each instrument and document required hereunder or under the terms of the Indenture when executed and delivered by the Collateral Manager hereunder or under the terms of the Indenture shall constitute, the legally valid and binding obligations of the Collateral Manager enforceable against the Collateral Manager in accordance with their terms, subject, as to enforcement, to (a) the effect of bankruptcy, insolvency or similar laws affecting generally the enforcement of creditors' rights and (b) general equitable principles (whether considered in a proceeding at law or in equity).
-(iii)The execution, delivery and performance of this Agreement and the terms of the Indenture applicable to the Collateral Manager and the documents and instruments required hereunder or under the terms of the Indenture shall not violate any provision of any existing law or regulation binding on or applicable to the Collateral Manager, or any order, judgment, award or decree of any court, arbitrator or governmental authority binding on the Collateral Manager, or the Governing Instruments of, or any securities issued by the Collateral Manager or of any mortgage, indenture, lease, contract or other agreement, instrument or undertaking to which the Collateral Manager is a party or by which the Collateral Manager or any of its assets is or may be bound, the violation of which would have a material adverse effect on the business operations, assets or financial condition of the Collateral Manager or its ability to perform its obligations under this Agreement, and shall not result in or require the creation or imposition of any lien on any of its property, assets or revenues pursuant to the provisions of any such mortgage, indenture, lease, contract or other agreement, instrument or undertaking.
-(iv)There is no charge, investigation, action, suit or proceeding before or by any court pending or, to the knowledge of the Collateral Manager, threatened that, if determined adversely to the Collateral Manager, would have a material adverse effect upon the performance by the Collateral Manager of its duties under, or on the validity or enforceability of, this Agreement or the provisions of the Indenture applicable to the Collateral Manager hereunder.
-(v)The Collateral Manager is authorized to carry on its business in the United States.
-(vi)The Collateral Manager is not in violation of its Governing Instruments or in breach or violation of or in default under any contract or agreement to which it is a party or by which it or any of its property may be bound, or any applicable statute or any rule, regulation or order of any court, government agency or body having jurisdiction over the Collateral Manager or its properties, the breach or violation of which or default under which would have a material adverse effect on the validity or enforceability of this Agreement or the provisions of the Indenture applicable to the Collateral Manager hereunder, or the performance by the Collateral Manager of its duties hereunder or under the Indenture.
-(vii)The Collateral Manager Information contained in the Offering Circular, as the same may be thereafter amended or supplemented, as of the date thereof, as of the date of any such amendment or supplement, and as of the Closing Date, is true and correct in all material respects and does not omit to state any material fact necessary in order to make the statements therein, in the light of the circumstances under which they were made, not misleading.
-The Collateral Manager makes no representation, express or implied, with respect to the Issuer or the disclosure with respect to the Issuer.
+          <t xml:space="preserve">27
 </t>
         </is>
       </c>
@@ -887,18 +756,18 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>12</t>
         </is>
       </c>
       <c r="C16" t="inlineStr"/>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Observation Rights</t>
+          <t>EFFECTIVE PERIOD AND TERMINATION</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t xml:space="preserve">The Issuer covenants and agrees, if requested in writing by the Collateral Manager and to the extent practicable under the circumstances, to notify the Collateral Manager of each meeting of the Board of Directors of the Issuer following the receipt of such request by the Issuer and to use commercially reasonable efforts to provide any materials distributed to the Board of Directors in connection with any such meeting and to afford a representative of the Collateral Manager the opportunity to be present at each such meeting, in person or by telephone at the option of the Collateral Manager.
+          <t xml:space="preserve">28
 </t>
         </is>
       </c>
@@ -909,56 +778,18 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>13</t>
         </is>
       </c>
       <c r="C17" t="inlineStr"/>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Notices</t>
+          <t>REPRESENTATIONS AND WARRANTIES</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t xml:space="preserve">Unless expressly provided otherwise herein, all notices, requests, demands and other communications required or permitted under this Agreement shall be in writing (including by telecopy) and shall be deemed to have been duly given, made and received when delivered against receipt or upon actual receipt, by registered or certified mail, postage prepaid, return receipt requested, by hand delivery, or by courier service or, in the case of telecopy or email notice, when received in legible form, addressed as set forth below:
-(a)
-If to the Issuer:
-Owl Rock Technology Financing 2020-1
-c/o Walkers Fiduciary Limited
-Cayman Corporate Centre
-27 Hospital Road,
-George Town, Grand Cayman
-Attention: The Directors
-KY1-9008, Cayman Islands
-Telephone no. +1 (345) 814-7600
-Email: fiduciary@walkersglobal.com
-(b)
-If to the Collateral Manager:
-Owl Rock Technology Advisors LLC
-399 Park Avenue, Floor 38
-New York, NY 10022
-Attention: Alan Kirshenbaum
-E-mail Address: alan@owlrock.com with a copy to legal@owlrock.com
-(c)
-If to the Trustee:
-State Street Bank and Trust Company
-1776 Heritage Drive
-Mail Code: JAB0250
-North Quincy, Massachusetts 02171
-Attention: Structured Trust and Analytics
-Ref: Owl Rock Technology Financing 2020-1
-Facsimile: (617) 937-4358
-Telephone: (617) 662-9839
-(d)
-If to the Rating Agency:
-S&amp;P Global Rating
-55 Water Street, 41st Floor
-New York, New York 10041
-Attention: Structured Credit-CDO Surveillance
-(e)
-If to the Holders:
-At their respective addresses set forth on the Register.
-Any party may alter the address, email address or telecopy number to which communications or copies are to be sent by giving notice of such change of address in conformity with the provisions of this Section 18 for the giving of notice.
+          <t xml:space="preserve">29
 </t>
         </is>
       </c>
@@ -969,18 +800,18 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>19</t>
+          <t>14</t>
         </is>
       </c>
       <c r="C18" t="inlineStr"/>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Binding Nature of Agreement; Successors and Assigns</t>
+          <t>PARTIES IN INTEREST; NO THIRD PARTY BENEFIT</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t xml:space="preserve">This Agreement shall be binding upon and inure to the benefit of the parties hereto and their respective heirs, personal representatives, successors and assigns as provided herein. The Collateral Manager agrees that its obligations hereunder shall be enforceable, at the instance of the Issuer, on behalf of the Issuer by the Trustee under the Indenture, as provided in the Indenture (subject to the rights and defenses of the Collateral Manager and the provisions of Sections 10 and 15 hereunder). The Collateral Manager agrees and consents to the provisions contained in Article XV of the Indenture.
+          <t xml:space="preserve">30
 </t>
         </is>
       </c>
@@ -991,20 +822,18 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>15</t>
         </is>
       </c>
       <c r="C19" t="inlineStr"/>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Entire Agreement; Amendments</t>
+          <t>NOTICES</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t xml:space="preserve">This Agreement contains the entire agreement and understanding among the parties hereto with respect to the subject matter hereof and supersedes all prior and contemporaneous agreements, understandings, inducements and conditions, express or implied, oral or written, of any nature whatsoever with respect to the subject matter hereof. The parties hereto hereby acknowledge that any prior agreement concerning the subject matter hereof has been terminated as of the date hereof and is of no further force or effect (except for provisions in such agreement designated to survive termination). (For the avoidance of doubt, the parties acknowledge that this Agreement does not govern the relationship of Owl Rock Technology Advisors in its capacity as a Holder.) The express terms hereof control and supersede any course of performance and/or usage of the trade inconsistent with any of the terms hereof.
-This Agreement may be amended by the parties thereto to (i) correct inconsistencies, typographical or other errors, defects or ambiguities or (ii) conform the Collateral Management Agreement to the Offering Circular, the Collateral Administration Agreement or the Indenture (as it may be amended from time to time in accordance with the terms thereof), in each case without the consent of the holders of any Securities and without satisfaction of the S&amp;P Rating Condition. The Collateral Manager will provide notice to the Rating Agency of any such amendment.
-Any other amendment to this Agreement requires the consent of the parties hereto and the approval of a Majority of the Preferred Shares, with at least ten (10) days' prior written notice to the Trustee (who shall forward such notice to the Controlling Class), the Fiscal Agent and the Rating Agency; provided that any such amendment to this Agreement that would (i) modify the definition of the term Cause, (ii) modify the Base Management Fee, including any component of the Base Management Fee, the method for calculating any component of the Base Management Fee or any definition used in any component of the Base Management Fee or (iii) modify the Class or Classes or the percentage of the Aggregate Outstanding Amount of any Class that has the right to remove the Collateral Manager, consent to any assignment of this Agreement or nominate or approve any successor Collateral Manager shall, in each case, also require the approval of a Majority of the Controlling Class and satisfaction of the S&amp;P Rating Condition.
+          <t xml:space="preserve">30
 </t>
         </is>
       </c>
@@ -1015,18 +844,18 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>16</t>
         </is>
       </c>
       <c r="C20" t="inlineStr"/>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Conflict with the Indenture</t>
+          <t>CHOICE OF LAW AND JURISDICTION</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t xml:space="preserve">In the event that this Agreement requires any action to be taken with respect to any matter and the Indenture requires that a different action be taken with respect to such matter, and such actions are mutually exclusive, the provisions of the Indenture in respect thereof shall control.
+          <t xml:space="preserve">31
 </t>
         </is>
       </c>
@@ -1037,20 +866,18 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>17</t>
         </is>
       </c>
       <c r="C21" t="inlineStr"/>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Subordination; Limited Recourse; Non-Petition</t>
+          <t>ENTIRE AGREEMENT; COUNTERPARTS</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t xml:space="preserve">(a)The Collateral Manager agrees that the payment of all amounts to which it is entitled pursuant to this Agreement shall be subordinated to the extent set forth in the Indenture, including Article XI thereof.
-(b)Notwithstanding any other provision of this Agreement, the obligations of the Issuer hereunder are, from time to time and at any time, limited recourse obligations of the Issuer, payable solely from the Assets and only to the extent of funds available from time to time and in accordance with the Priority of Payments, and following exhaustion of the Assets, any claims of the Collateral Manager hereunder shall be extinguished and shall not thereafter revive. The Collateral Manager further agrees (i) not to take any action in respect of any claims hereunder against any officer, director, employee, shareholder, noteholder or administrator of the Issuer and (ii) not to cause the filing of a petition in bankruptcy against the Issuer for the nonpayment of the fees or other amounts payable by the Issuer to the Collateral Manager under this Agreement until the payment in full of all Notes issued under the Indenture and the expiration of a period equal to one year and a day, or, if longer, the applicable preference period, following such payment. Nothing in this Section 22 shall preclude, or be deemed to stop, the Collateral Manager (x) from taking any action prior to the expiration of the aforementioned period in (A) any case or Proceeding voluntarily filed or commenced by the Issuer, or (B) any involuntary insolvency Proceeding filed or commenced by a Person other than the Collateral Manager, or (y) from commencing against the Issuer or any of its properties any legal action which is not a bankruptcy, reorganization,
-arrangement, insolvency, moratorium or liquidation proceeding. The provisions of this Section 22 shall survive the termination of this Agreement for any reason whatsoever.
+          <t xml:space="preserve">31
 </t>
         </is>
       </c>
@@ -1061,18 +888,18 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>23</t>
+          <t>18</t>
         </is>
       </c>
       <c r="C22" t="inlineStr"/>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Governing Law</t>
+          <t>AMENDMENT; WAIVER</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t xml:space="preserve">THIS AGREEMENT SHALL BE GOVERNED BY AND CONSTRUED IN ACCORDANCE WITH THE LAW OF THE STATE OF NEW YORK.
+          <t xml:space="preserve">32
 </t>
         </is>
       </c>
@@ -1083,18 +910,18 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>24</t>
+          <t>19</t>
         </is>
       </c>
       <c r="C23" t="inlineStr"/>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Indulgences Not Waivers</t>
+          <t>SUCCESSOR AND ASSIGNS</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t xml:space="preserve">Neither the failure nor any delay on the part of any party hereto to exercise any right, remedy, power or privilege under this Agreement shall operate as a waiver thereof, nor shall any single or partial exercise of any right, remedy, power or privilege preclude any other or further exercise of the same or of any other right, remedy, power or privilege, nor shall any waiver of any right, remedy, power or privilege with respect to any occurrence be construed as a waiver of such right, remedy, power or privilege with respect to any other occurrence. No waiver shall be effective unless it is in writing and is signed by the party asserted to have granted such waiver.
+          <t xml:space="preserve">32
 </t>
         </is>
       </c>
@@ -1105,18 +932,18 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>25</t>
+          <t>20</t>
         </is>
       </c>
       <c r="C24" t="inlineStr"/>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Costs and Expenses</t>
+          <t>SEVERABILITY</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t xml:space="preserve">The reasonable costs and expenses (including the fees and disbursements of counsel and accountants) incurred by the Collateral Manager in connection with the negotiation and preparation of and the execution of this Agreement, and all matters incident thereto, shall be borne by the Issuer and, unless paid on the Closing Date or shortly thereafter by ORCC or from the proceeds of the offering of the Securities (to the extent permitted under the Indenture), shall be subject to the Priority of Payments.
+          <t xml:space="preserve">33
 </t>
         </is>
       </c>
@@ -1127,18 +954,18 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>26</t>
+          <t>21</t>
         </is>
       </c>
       <c r="C25" t="inlineStr"/>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Titles Not to Affect Interpretation</t>
+          <t>REQUEST FOR INSTRUCTIONS</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t xml:space="preserve">The titles of paragraphs and subparagraphs contained in this Agreement are for convenience only, and they neither form a part of this Agreement nor are they to be used in the construction or interpretation hereof.
+          <t xml:space="preserve">33
 </t>
         </is>
       </c>
@@ -1149,18 +976,18 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>27</t>
+          <t>22</t>
         </is>
       </c>
       <c r="C26" t="inlineStr"/>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Execution in Counterparts</t>
+          <t>OTHER BUSINESS</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t xml:space="preserve">This Agreement may be executed in any number of counterparts, which may be effectively delivered by facsimile or other electronic means or other written form of communication, each of which shall be deemed to be an original as against any party whose signature appears thereon, and all of which shall together constitute one and the same instrument. This Agreement shall become binding when one or more counterparts hereof, individually or taken together, shall bear the signatures of all of the parties reflected hereon as the signatories.
+          <t xml:space="preserve">33
 </t>
         </is>
       </c>
@@ -1171,19 +998,18 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>28</t>
+          <t>23</t>
         </is>
       </c>
       <c r="C27" t="inlineStr"/>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Provisions Separable</t>
+          <t>REPRODUCTION OF DOCUMENTS</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t xml:space="preserve">In case any provision in this Agreement shall be invalid, illegal or unenforceable as written, such provision shall be construed in the manner most closely resembling the apparent intent of the parties with respect to such provision so as to be valid, legal and enforceable; provided, however, that if there is no basis for such a construction, such provision shall be ineffective only to the extent
-of such invalidity, illegality or unenforceability and, unless the ineffectiveness of such provision destroys the basis of the bargain for one of the parties to this Agreement, the validity, legality and enforceability of the remaining provisions hereof or thereof shall not in any way be affected or impaired thereby.
+          <t xml:space="preserve">33
 </t>
         </is>
       </c>
@@ -1194,18 +1020,28 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>29</t>
+          <t>24</t>
         </is>
       </c>
       <c r="C28" t="inlineStr"/>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Number and Gender</t>
+          <t>MISCELLANEOUS</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t xml:space="preserve">Words used herein, regardless of the number and gender specifically used, shall be deemed and construed to include any other number, singular or plural, and any other gender, masculine, feminine or neuter, as the context requires.
+          <t xml:space="preserve">33
+SCHEDULES
+SCHEDULE A - Initial Authorized Persons
+i
+ACTIVE\1602581275.4
+THIS CUSTODY AGREEMENT (this "Agreement") is dated as of September 21, 2023 and is by and between PROSPECT FLOATING RATE AND ALTERNATIVE INCOME FUND, INC. (and any successor or permitted assign, the "Company"), a Maryland corporation and U.S. BANK TRUST COMPANY, NATIONAL ASSOCIATION (or any successor or permitted assign acting as custodian hereunder, the "Custodian"), a national banking association.
+RECITALS
+WHEREAS, the Company is a closed-end management investment company, which, prior to the commencement of its investment operations, has elected to be regulated as a business development company under the Investment Company Act of 1940, as amended (the "1940 Act");
+WHEREAS, the Company desires to retain U.S. Bank Trust Company, National Association to act as custodian for the Company and each Subsidiary hereafter identified to the Custodian;
+WHEREAS, the Company desires that certain of the Company's Securities (as defined below) and cash be held and administered by the Custodian pursuant to this Agreement in compliance with Section 17(f) of the 1940 Act;
+NOW THEREFORE, in consideration of the mutual covenants and agreements contained herein, the parties hereto agree as follows:
 </t>
         </is>
       </c>
@@ -1216,18 +1052,77 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>30</t>
+          <t>1</t>
         </is>
       </c>
       <c r="C29" t="inlineStr"/>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Jurisdiction and Venue</t>
+          <t>DEFINITIONS</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t xml:space="preserve">The parties to this Agreement irrevocably submit to the non-exclusive jurisdiction of any New York state or federal court sitting in the Borough of Manhattan in The City of New York in any action or proceeding arising out of or relating to this Agreement, the Securities or the Indenture, and the parties irrevocably agree that all claims in respect of such action or proceeding may be heard and determined in such New York state or federal court. The parties to this Agreement irrevocably waive, to the fullest extent they may legally do so, the defense of an inconvenient forum to the maintenance of such action or proceeding. The parties to this Agreement irrevocably consent to the service of any and all process in any action or proceeding by the mailing or delivery of copies of such process to it in accordance with Section 18. The parties agree that a final judgment in any such action or proceeding shall be conclusive and may be enforced in other jurisdictions by suit on the judgment or in any other manner provided by law.
+          <t xml:space="preserve">1.1 Defined Terms. In addition to terms expressly defined elsewhere herein, the following words shall have the following meanings as used in this Agreement:
+"Account" or "Accounts" means the Securities Account(s) and any Subsidiary Securities Account(s), collectively.
+"Agreement" means this Custody Agreement (as the same may be amended from time to time in accordance with the terms hereof).
+"Authorized Person" has the meaning set forth in Section 7.4(a).
+"Business Day" means any day that is not Saturday or Sunday and is not a legal holiday or a day in which banking institutions generally are authorized or obligated by law or regulation to remain closed in New York, New York, or the city in which the Custodian (pursuant to Section 15) or any Sub-Custodian is located.
+"Company" has the meaning set forth in the first paragraph of this Agreement.
+"Confidential Information" has the meaning set forth in Section 24.
+"Custodian" has the meaning set forth in the first paragraph of this Agreement.
+"Disclosing Party" has the meaning set forth in Section 24.
+"Document Custody Agreement" means the Document Custody Agreement dated as of even date between the Document Custodian and the Company.
+ACTIVE\1602581275.4
+"Document Custodian" means U.S. Bank National Association in its capacity as document custodian under that certain Document Custody Agreement.
+"Eligible Foreign Custodian" has the meaning set forth in Rule 17 f-5(a)(1), including a majority-owned or indirect subsidiary of a U.S. Bank (as defined in Rule 17 f-5), a bank holding company meeting the requirements of an Eligible Foreign Custodian (as set forth in Rule 17 f-5 or by other appropriate action of the SEC), or a foreign branch of a Bank (as defined in Section 2(a)(5) of the 1940 Act) meeting the requirements of a custodian under Section 17(f) of the 1940 Act; the term does not include any Eligible Securities Depository.
+"Eligible Investment" means any investment that at the time of its acquisition is one or more of the following:
+(a) United States government and agency obligations;
+(b) commercial paper having a rating assigned to such commercial paper by Standard &amp; Poor's Rating Services or Moody's Investor Service, Inc. (or, if neither such organization shall rate such commercial paper at such time, by any nationally recognized rating organization in the United States of America) equal to one of the two highest ratings assigned by such organization, it being understood that as of the date hereof such ratings by Standard &amp; Poor's Rating Services are "A1+" and "A1" and such ratings by Moody's Investor Service, Inc. are "P1" and "P2";
+(c) interest bearing deposits in United States dollars in United States banks with an unrestricted surplus of at least U.S. $250,000,000, maturing within one year; and
+(d) money market funds (including funds of the bank serving as Custodian or its affiliates) or United States government securities funds designed to maintain a fixed share price and high liquidity.
+"Eligible Securities Depository" has the meaning set forth in Section (b)(1) of Rule 17 f-7 under the 1940 Act.
+"ERISA" has the meaning set forth in Section 13.1(c).
+"Federal Reserve Bank Book-Entry System" means a depository and securities transfer system operated by the Federal Reserve Bank of the United States on which are eligible to be held all United States Government direct obligation bills, notes and bonds.
+"Financing Documents" means any Loan Assignment Agreement, Participation Agreement, and any related instrument, security, credit agreement, assignment agreement and/or other agreements or documents, if any, that may be delivered to the Custodian pursuant to this Agreement.
+"Foreign Sub-custodian" means and includes any sub-custodian appointed to administer any of the Company's Foreign Securities, pursuant to Section 6.
+"Foreign Securities" means Securities for which the primary market is outside the United States.
+"Investment Adviser" means Prospect Capital Management L.P.
+2
+"Loan" means any U.S. dollar denominated commercial loan, or Participation therein, whether made by a bank or other financial institution and/or made in a direct lending capacity to the borrower thereunder or otherwise that by its terms provides for payments of principal and/or interest, including discount obligations and payment-in-kind obligations, acquired by the Company from time to time.
+"Loan Assignment Agreement" has the meaning set forth in Section 3.3(b)(ii).
+"Participation" means an interest in a Loan that is acquired indirectly by way of a participation from a selling institution.
+"Participation Agreement" has the meaning set forth in Section 3.3(b)(ii).
+"Person" means any individual, corporation, partnership, limited liability company, joint venture, association, joint stock company, trust (including any beneficiary thereof) unincorporated organization, or any government or agency or political subdivision thereof.
+"Plan-assets Vehicle" has the meaning set forth in Section 13.1(c).
+"Proceeds" means, collectively, (i) the net cash proceeds to the Company of any offering by the Company of any class of securities issued by the Company, (ii) all cash distributions, earnings, dividends, fees and other cash payments paid on the Securities (or, as applicable, Subsidiary Securities) by or on behalf of the issuer or obligor thereof, or applicable paying agent or administrative agent, (iii) the net cash proceeds of the sale or other disposition of the Securities (or, as applicable, Subsidiary Securities) pursuant to the terms of this Agreement (and any Reinvestment Earnings from investment of the foregoing) and (iv) the net cash proceeds to the Company of any borrowing or other financing by the Company, as delivered to and received by the Custodian from time to time.
+"Proper Instructions" means instructions (including Trade Confirmations) received by the Custodian in form acceptable to it, from the Company or any Person duly authorized by the Company in any of the following forms acceptable to the Custodian:
+(a) in writing signed by an Authorized Person (and delivered by hand, by mail, by electronic mail, by overnight courier or by facsimile);
+(b) by electronic mail (or other electronic transmission) from an Authorized Person;
+(c) in a communication utilizing access codes effected between electro mechanical or electronic devices; or
+(d) such other means as may be agreed upon from time to time by the Custodian and the party giving such instructions, including oral instructions and any SWIFT Transmissions (as defined herein).
+"Receiving Party" has the meaning set forth in Section 24.
+"Reinvestment Earnings" has the meaning set forth in Section 3.6(b).
+3
+"Securities" means, collectively, (i) the investments, including Loans and Uncertificated Securities, acquired by the Company and delivered to the Custodian by the Company from time to time during the term of, and pursuant to the terms of, this Agreement and (ii) all dividends in kind (e.g., non-cash dividends) from the investments described in clause (i). For avoidance of doubt, the term "securities" includes stocks, shares, bonds, debentures, notes, mortgages or other obligations and any certificates, receipts, warrants or other instruments representing rights to receive, purchase, or subscribe for the same, or evidencing or representing any other rights or interests therein, or in any property or assets.
+"Securities Account(s)" means collectively the segregated accounts to be established by the Custodian at U.S. Bank National Association or any affiliate to which the Custodian shall deposit or credit and hold the Securities (other than Loans or Uncertificated Securities) and any cash Proceeds from time to time from or with respect to the Securities or the sale of the Securities of the Company, as applicable and in each case received by the Custodian pursuant to this Agreement, which account shall be in the name of the Company. The initial Securities Accounts are listed in Exhibit A.
+"Securities Depository" means The Depository Trust Company and any other clearing agency registered with the Securities and Exchange Commission under Section 17 A of the Securities Exchange Act of 1934, as amended (the "1934 Act"), which acts as a system for the central handling of Securities where all Securities of any particular class or series of an issuer deposited within the system are treated as fungible and may be transferred or pledged by bookkeeping entry without physical delivery of the Securities.
+"Securities System" means the Federal Reserve Book-Entry System, a clearing agency which acts as a Securities Depository, or another book entry system for the central handling of securities (including an Eligible Securities Depository).
+"Shares" means the shares of common stock, par value $0.01 per share, of the Company.
+"Street Delivery Custom" means a custom of the United States securities market to deliver securities which are being sold to the buying broker for examination to determine that the securities are in proper form.
+"Street Name" means the form of registration in which the securities are held by a broker who is delivering the securities to another broker for the purposes of sale, it being an accepted custom in the United States securities industry that a security in Street Name is in proper form for delivery to a buyer and that a security may be re-registered by a buyer in the ordinary course.
+"Sub-Custodian" shall mean and include (i) any branch of a "U.S. bank," as that term is defined in Rule 17 f-5 under the 1940 Act, and (ii) any "Eligible Foreign Custodian", as that term is defined in Rule 17 f-5 under the 1940 Act, having a contract with the Custodian which the Custodian has determined will provide reasonable care of assets of the Company based on the standards specified in Section 3.14. Such contract shall be in writing and shall include provisions that provide: (i) for indemnification or insurance arrangements (or any combination of the foregoing) such that the Company will be adequately protected against the risk of loss of assets held in accordance with such contract; (ii) that the Foreign Securities will not be subject to any right, charge, security interest, lien or claim of any kind in favor of the Sub-Custodian or its creditors except a claim of payment for their safe custody or administration, in the case of cash deposits, liens or rights in favor of creditors of the Sub-Custodian arising under bankruptcy,
+4
+insolvency, or similar laws; (iii) that beneficial ownership for the Foreign Securities will be freely transferable without the payment of money or value other than for safe custody or administration; (iv) that adequate records will be maintained identifying the assets as belonging to the Company or as being held by a third party for the benefit of the Company; (v) that the Company's independent public accountants will be given access to those records or confirmation of the contents of those records; and (vi) that the Company will receive periodic reports with respect to the safekeeping of the Company's assets, including, but not limited to, notification of any transfer to or from the Company's account or a third party account containing assets held for the benefit of the Company. Such contract may contain, in lieu of any or all of the provisions specified in (i)-(vi) above, such other provisions that the Custodian determines will provide, in their entirety, the same or a greater level of care and protection for Company assets as the specified provisions.
+"Subsidiary" means, collectively, any wholly owned subsidiary of any Company identified to the Custodian by the Company.
+"Subsidiary Securities" means, collectively, (i) the investments, including Loans, acquired by a Subsidiary and delivered to the Custodian by such Subsidiary from time to time during the term of, and pursuant to the terms of, this Agreement and (ii) all dividends in kind (e.g., non-cash dividends) from the investments described in clause (i).
+"Subsidiary Securities Account(s)" shall have the meaning set forth in Section 3.13(a).
+"Trade Confirmation" means a trade ticket or confirmation to the Custodian from the Company of the Company's acquisition of a Loan, and setting forth applicable information with respect to such Loan, in such form as may be acceptable to the Custodian.
+"Uncertificated Security" means a Security that is not represented by a physical certificate.
+"Underlying Loan Agreement" means, with respect to any Loan, the document or documents evidencing the commercial loan agreement or facility pursuant to which such Loan is made.
+"Underlying Loan Documents" means, with respect to any Loan, the related Underlying Loan Agreement together with any agreements and instruments (including any Underlying Note) executed or delivered in connection therewith.
+"Underlying Note" means the one or more promissory notes executed by an obligor evidencing a Loan.
+"UCC" means the Uniform Commercial Code as in effect from time to time in the State of New York.
 </t>
         </is>
       </c>
@@ -1238,18 +1133,32 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>31</t>
-        </is>
-      </c>
-      <c r="C30" t="inlineStr"/>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Rule 17g-5 Compliance</t>
+          <t>Construction</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t xml:space="preserve">The Collateral Manager agrees that any notice, report, request for satisfaction of the Global Rating Condition or other information provided by the Collateral Manager (or any of its respective representatives or advisors) to any Rating Agency hereunder or under the Indenture or the Collateral Administration Agreement for the purposes of undertaking credit rating surveillance of the Secured Notes shall be provided, substantially concurrently, by the Collateral Manager to the Information Agent for posting on a password-protected website in accordance with the procedures set forth in Section 2A of the Collateral Administration Agreement and Section 14.16 of the Indenture.
+          <t xml:space="preserve"> In this Agreement unless the contrary intention appears:
+(a)any reference to this Agreement or another agreement or instrument refers to such agreement or instrument as the same may be amended, modified or otherwise rewritten from time to time;
+5
+(b)a reference to a statute, ordinance, code or other law includes regulations and other instruments under it and consolidations, amendments, re-enactments or replacements of any of them;
+(c)any term defined in the singular form may be used in, and shall include, the plural with the same meaning, and vice versa;
+(d)a reference to a Person includes a reference to the Person's executors, custodians, successors and permitted assigns;
+(e)an agreement, representation or warranty in favor of two or more Persons is for the benefit of them jointly and severally;
+(f)an agreement, representation or warranty on the part of two or more Persons binds them jointly and severally;
+(g)a reference to the term "including" means "including, without limitation,";
+(h)a reference to any accounting term is to be interpreted in accordance with generally accepted principles and practices in the United States, consistently applied, unless otherwise instructed by the Company; and
+(i)any reference to "execute", "executed", "sign", "signed", "signature" or any other like term hereunder shall include execution by electronic signature (including, without limitation, any .pdf file, .jpeg file, or any other electronic or image file, or any "electronic signature" as defined under the U.S. Electronic Signatures in Global and National Commerce Act ("E-SIGN") or the New York Electronic Signatures and Records Act ("ESRA"), which includes any electronic signature provided using Orbit, Adobe Sign, DocuSign, or any other similar platform identified by the Company and reasonably available at no undue burden or expense to the Custodian), except to the extent the Custodian requests otherwise. Any such electronic signatures shall be valid, effective and legally binding as if such electronic signatures were handwritten signatures and shall be deemed to have been duly and validly delivered for all purposes hereunder.
 </t>
         </is>
       </c>
@@ -1258,25 +1167,2160 @@
       <c r="A31" s="1" t="n">
         <v>29</v>
       </c>
-      <c r="B31" t="inlineStr"/>
-      <c r="C31" t="inlineStr"/>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
       <c r="D31" t="inlineStr">
         <is>
+          <t>Headings</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Headings are inserted for convenience and do not affect the interpretation of this Agreement.
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr"/>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>APPOINTMENT OF CUSTODIAN</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr"/>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>Appointment and Acceptance</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> (a) The Company hereby appoints the Custodian as custodian of all Securities and Proceeds owned by the Company and the Subsidiaries (as applicable) and delivered to and received by the Custodian from time to time during the period of this Agreement, on the terms and conditions set forth in this Agreement (which shall include any addendum hereto which is hereby incorporated herein and made a part of this Agreement), and the Custodian hereby accepts such appointment and agrees to perform the services and duties set forth in this Agreement with respect to it and subject to and in accordance with the provisions hereof. Any Account may contain any number of accounts for the convenience of the Custodian or as required by the Company or the Subsidiaries (as applicable) for convenience in administering such accounts.
+6
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>Instructions</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> The Company agrees that it shall from time to time provide, or cause to be provided, to the Custodian all necessary instructions and information, and shall respond promptly to all inquiries and requests of the Custodian, as may reasonably be necessary to enable the Custodian to perform its duties hereunder.
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>Company Responsible For Directions</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> The Company is solely responsible for directing the Custodian with respect to deposits to, withdrawals from and transfers to or from the Accounts. Without limiting the generality of the foregoing, the Custodian has no responsibility for the Company's legal and regulatory compliance (including the 1940 Act), any of its obligations to third-parties in respect of the Accounts, and the Custodian shall have no liability for the application of any funds made with Proper Instructions of the Company. The Company shall be solely responsible for properly instructing all applicable payors to make all appropriate payments to the Custodian for deposit to the Accounts, and for properly instructing the Custodian with respect to the allocation or application of all such deposits.
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr"/>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>DUTIES OF CUSTODIAN</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr"/>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>Segregation</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> All Securities, Subsidiary Securities and non-cash property held by the Custodian, as applicable, for the account of the Company or Subsidiary, respectively (other than Securities and Subsidiary Securities maintained in a Securities Depository or Securities System), shall be physically segregated from other Securities and non-cash property in the possession of the Custodian (including the Securities and non-cash property of the other series of the Company, if applicable) and shall be identified as subject to this Agreement.
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>Securities Custody Account</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> The Custodian shall open and maintain at U.S. Bank National Association or any affiliate a segregated account in the name of the Company, subject only to order of the Custodian, in which the Custodian shall enter and carry, subject to Section 3.3(b), all Securities (other than Loans and Uncertificated Securities), cash and other investment assets of the Company which are delivered to it in accordance with this Agreement. For the avoidance of doubt, the Custodian shall not be required to credit or deposit Loans or Uncertificated Securities in the Securities Account but shall instead maintain a register of such Loans or Uncertificated Securities, containing such information as the Company and the Custodian may reasonably agree and marked so as to clearly identify them as the property of the Company.
+The Custodian shall have no power or authority to assign, hypothecate, pledge or otherwise dispose of any such Securities and investments except pursuant to the direction of the Company under the terms of this Agreement.
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="n">
+        <v>37</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>Delivery of Cash and Securities to Custodian</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t xml:space="preserve">(a)The Company shall deliver, or cause to be delivered, to the Custodian certain of the Company's Securities, cash and other investment assets, including (a) payments of income, payments of principal and capital distributions received by the Company with respect to such Securities, cash or other assets owned by the Company at any time during the period of this Agreement and (b) all cash received by the Company for the issuance, at any time during such period, of Shares or other securities or in connection with a borrowing by the Company. With respect to assets other than Loans, such assets shall be delivered to the Custodian in its role as, and (where relevant) at the address identified for, the Custodian. Except to the extent otherwise expressly provided herein, delivery of
+7
+Securities to the Custodian shall be in Street Name or other good delivery form. The Custodian shall not be responsible for such Securities, cash or other assets until actually delivered to, and received by it. With respect to Securities (other than Loan Assets, Uncertificated Securities and assets in the nature of "general intangibles" (as hereinafter defined)) held by the Custodian in its capacity as a "securities intermediary" (as defined in Section 8-102 of the Uniform Commercial Code as in effect in the State of New York (the "UCC")), the Custodian shall be obligated to exercise due care in accordance with reasonable commercial standards in discharging the duties as a securities intermediary to hold such Securities. A Security will be deemed to be "delivered" to the Custodian when the Company delivers such Security in the following manner: (i) if such Security is a Certificated Security or an instrument (other than a Security held in a Securities System), then in physical certificated form in the name of the Company or its nominee, (ii) if such Security is an Uncertificated Security or in the form of uncertificated share(s) or other interest (other than a Security held in a Securities System), then delivery of confirmation statements which identify such shares or interests as being recorded in the name of the Company or its nominee, (iii) if such Security is held in a Securities System or maintained in one or more omnibus accounts at the Custodian, its agents or sub-custodians, then delivery of confirmation that such Security is held in the Securities System or maintained through one or more omnibus accounts in the name of the Custodian (or its nominee) who shall identify the same on its books and records as held for the account of the Company, or (iv) in such other good delivery form that may be agreed to by the Custodian from time to time.
+(b)(i) In connection with its acquisition of a Loan, an Uncertificated Security or other delivery of a Security constituting a Loan, the Company shall deliver or cause to be delivered to the Custodian a properly completed Trade Confirmation containing such information in respect of such Loan or Uncertificated Security as the Custodian may reasonably require in order to enable the Custodian to perform its duties hereunder in respect of such Loan or Uncertificated Security on which the Custodian may conclusively rely without further inquiry or investigation, in such form and format as the Custodian reasonably may require.
+(ii) Notwithstanding any term hereof or elsewhere to the contrary, (a) it is hereby expressly acknowledged that (i) interests in Loans or Uncertificated Securities may be acquired by the Company from time to time which are not evidenced by, or accompanied by delivery of, a Security or an instrument, as that term is defined in Section 9-102(a)(4 a) of the UCC, and may be evidenced solely by delivery to the Custodian of (x) a facsimile or electronic copy of an assignment agreement ("Loan Assignment Agreement") in favor of the Company as assignee or, in respect of any Loan acquired by participation interest, a participation agreement (a "Participation Agreement") in favor of the Company as participant or (y) a copy of the register of the underlying issuer of such interest evidencing registration of such equity interest on the books and records of the applicable issuer to the name of the Company (or its nominee) and (ii) any such Loan Assignment Agreement or Participation Agreement (and the registration of the related Loan on the books and records of the applicable obligor or bank agent) shall be registered in the name of the Company (or its nominee), and (b) nothing herein shall require the Custodian to credit to the Securities Account or to treat as a financial asset (within the meaning of Section 8-102(a)(9) of the UCC) any such Loan or other asset in the nature of a general intangible (as defined in Section 9-102(a)(42) of the UCC) or to "maintain" a sufficient quantity thereof. The
+8
+Custodian is not under a duty to examine any such Financing Documents, or any underlying credit agreements or loan documents for such Loan to determine the validity, sufficiency, marketability or enforceability of any Loan Assignment Agreement, Participation Agreement or other Financing Document (and shall have no responsibility for the genuineness or completeness thereof), or for the Company's title to any related Loan.
+(iii) The Custodian may assume the genuineness of any such Financing Document it may receive and the genuineness and due authority of any signatures appearing thereon, and shall be entitled to assume that each such Financing Document it may receive is what it purports to be. If an original "security" or "instrument" as defined in Section 8-102 and Section 9-102(a)(47) of the UCC, respectively, is or shall be or becomes available with respect to any Loan to be held by the Custodian under this Agreement, it shall be the sole responsibility of the Company to make or cause delivery thereof to the Document Custodian under the Document Custody Agreement and the Custodian, and the Custodian shall not be under any obligation at any time to determine whether any such original security or instrument has been or is required to be issued or made available in respect of any Loan or to compel or cause delivery thereof to the Custodian.
+(iv) Contemporaneously with the acquisition of any Loan, the Company shall (a) cause any appropriate Financing Documents evidencing such Loan to be delivered to the Custodian; (b) if requested by the Custodian, provide to the Custodian an amortization schedule of principal payments and a schedule of the interest payable date(s) identifying the amount and due dates of all scheduled principal and interest payments for such Loan and (c) provide to the Custodian a properly completed Trade Confirmation containing such information in respect of such Loan as the Custodian may reasonably require in order to enable the Custodian to perform its duties hereunder in respect of such Loan on which the Custodian may conclusively rely without further inquiry or investigation, in such form and format as the Custodian reasonably may require; (d) take all actions necessary for the Company to acquire good title to such Loan; and (e) take all actions as may be necessary (including appropriate payment notices and instructions to bank agents or other applicable paying agents or administrative agents) to cause (A) all payments in respect of the Loan to be made to the Custodian and (B) all notices, solicitations and other communications in respect of such Loan to be directed to the Company. The Custodian shall have no liability for any delay or failure on the part of the Company to provide necessary information to the Custodian, or for any inaccuracy therein or incompleteness thereof, or for any delay or failure on the part of the Company to give such effective payment instruction to bank agents and other paying agents or administrative agents, in respect of the Loans. With respect to each such Loan, the Custodian shall be entitled to rely on any information and notices it may receive from time to time from the related bank agent, obligor, participating bank, nationally recognized pricing service or vendor, reputable financial information reporting source or similar party with respect to the related Loan, and shall be entitled to update its records (as it may deem necessary or appropriate), or from the Company, on the basis of such information or notices received, without any obligation on its part independently to verify, investigate or recalculate such information.
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>Release of Securities</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t xml:space="preserve">9
+(a)The Custodian shall release and if applicable, ship for delivery, or direct its agents or Sub-Custodian to release and if applicable, ship for delivery, as the case may be, Securities of the Company held by the Custodian, its agents or its Sub-Custodian from time to time upon receipt of Proper Instructions (which shall, among other things, specify the Securities to be released, with such delivery and other information as may be necessary to enable the Custodian to perform), which may be standing instructions (in form acceptable to the Custodian) in the following cases:
+(i)upon sale of such Securities by or on behalf of the Company and, such sale may, unless and except to the extent otherwise directed by Proper Instructions, be carried out by the Custodian:
+(A) in accordance with the customary or established practices and procedures in the jurisdiction or market where the transactions occur, including delivery to the purchaser thereof or to a dealer therefor (or an agent of such purchaser or dealer) against expectation of receiving later payment; or
+(B) in the case of a sale effected through a Securities System, in accordance with the rules governing the operations of the Securities System;
+(ii)upon the receipt of payment in connection with any repurchase agreement related to such Securities;
+(iii)to a depositary agent in connection with tender or other similar offers for such Securities;
+(iv)to the issuer thereof or its agent when such Securities are called, redeemed, retired or otherwise become payable (unless otherwise directed by Proper Instructions, the cash or other consideration is to be delivered to the Custodian, its agents or its Sub-Custodian);
+(v)to an issuer thereof, or its agent, for transfer into the name of the Custodian or of any nominee of the Custodian or into the name of any of its agents or Sub-Custodian or their nominees or for exchange for a different number of bonds, certificates or other evidence representing the same aggregate face amount or number of units;
+(vi)to brokers clearing banks or other clearing agents for examination in accordance with the Street Delivery Custom;
+(vii) for exchange or conversion pursuant to any plan of merger, consolidation, recapitalization, reorganization or readjustment of the Securities of the issuer of such Securities, or pursuant to any deposit agreement (unless otherwise directed by Proper Instructions, the new securities and cash, if any, are to be delivered to the Custodian, its agents or its Sub-Custodian);
+(viii) in the case of warrants, rights or similar securities, the surrender thereof in the exercise of such warrants, rights or similar securities or the surrender of interim receipts or temporary securities for definitive securities (unless otherwise directed by Proper Instructions, the new
+10
+securities and cash, if any, are to be delivered to the Custodian, its agents or its Sub-Custodian); and/or
+(ix)for any other purpose, but only upon receipt of Proper Instructions.
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>Registration of Securities</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Securities held by the Custodian, its agents or its Sub-Custodian (other than bearer securities or securities held in a Securities System) shall be registered in the name of the Company or its nominee; or, at the option of the Custodian, in the name of the Custodian or in the name of any nominee of the Custodian, or in the name of its agents or its Sub-Custodian or their nominees; or if directed by the Company by Proper Instruction, may be maintained in Street Name. The Custodian, its agents and its Sub-Custodian shall not be obligated to accept Securities on behalf of the Company under the terms of this Agreement unless such Securities (other than Loans) are in Street Name or other good deliverable form.
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>Bank Accounts and Management of Cash</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t xml:space="preserve">(a)Proceeds and other cash received by the Custodian from time to time shall be deposited into or credited to the respective Securities Account as designated by the Company. All amounts deposited into or credited to the designated Securities Account shall be subject to clearance and receipt of final payment by the Custodian.
+(b)Amounts held in each respective Securities Account from time to time may be invested in Eligible Investments pursuant to specific written Proper Instructions (which may be standing instructions) received by the Custodian from an Authorized Person acting on behalf of the Company. Such investments shall be subject to availability and the Custodian's then applicable transaction charges (which shall be at the Company's expense). The Custodian shall have no liability for any loss incurred on any such investment. Absent receipt of such written instruction from the Company, the Custodian shall have no obligation to invest (or otherwise pay interest on) amounts on deposit in each respective Securities Account. In no instance will the Custodian have any obligation to provide investment advice to the Company. Any earnings from such investment of amounts held in the Securities Accounts from time to time (collectively, "Reinvestment Earnings") shall be redeposited in the respective Securities Account (and may be reinvested at the written direction of the Company). The Custodian shall have no liability for any losses on any investments made as described herein.
+(c)In the event that the Company shall at any time request a withdrawal of amounts from any of the Securities Accounts, the Custodian shall be entitled to liquidate, and shall have no liability for any loss incurred as a result of the liquidation of, any investment of the funds credited to such account as needed to provide necessary liquidity. Investment instructions may be in the form of standing instructions (in the form of Proper Instructions acceptable to Custodian).
+(d)The Company acknowledges that cash deposited or invested with any bank (including the bank acting as Custodian) may make a margin or generate banking income for which such bank shall not be required to account to the Company.
+11
+(e)The Custodian shall be authorized to open such additional accounts as may be necessary or convenient for administration of its duties hereunder with notice to be provided to the Company.
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="n">
+        <v>41</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>Foreign Exchange</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t xml:space="preserve">(a)Upon the receipt of Proper Instructions, the Custodian, its agents or its Sub-Custodian may (but shall not be obligated to) enter into all types of contracts for foreign exchange on behalf of the Company, upon terms acceptable to the Custodian and the Company (in each case at the Company's expense), including transactions entered into with the Custodian, its Sub-Custodian or any affiliates of the Custodian or the Sub-Custodian. The Custodian shall have no liability for any losses incurred in or resulting from the rates obtained in such foreign exchange transactions; and absent specific and acceptable Proper Instructions, the Custodian shall not be deemed to have any duty to carry out any foreign exchange on behalf of the Company. The Custodian shall be entitled at all times to comply with any legal or regulatory requirements applicable to currency or foreign exchange transactions.
+(b)The Company acknowledges that the Custodian, any Sub-Custodian or any affiliates of the Custodian or any Sub-Custodian, involved in any such foreign exchange transactions may make a margin or generate banking income from foreign exchange transactions entered into pursuant to this section for which they shall not be required to account to the Company.
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>Collection of Income</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Subject to Section 7.8, the Custodian, its agents or its Sub-Custodian shall use reasonable efforts to collect on a timely basis all income and other payments with respect to the Securities held hereunder to which the Company shall be entitled, to the extent consistent with usual custom in the securities custodian business in the United States. Such efforts shall include collection of interest income, dividends and other payments with respect to registered domestic securities if on the record date with respect to the date of payment by the issuer the Security is registered in the name of the Custodian or its nominee (or in the name of its agent or Sub-Custodian, or their nominee); and interest income, dividends and other payments with respect to bearer domestic securities if, on the date of payment by the issuer such securities are held by the Custodian or its Sub-Custodian or agent; provided, however, that in the case of Securities held in Street Name, the Custodian shall use commercially reasonable efforts only to timely collect income. In no event shall the Custodian's agreement herein to collect income be construed to obligate the Custodian to commence, undertake or prosecute any legal proceedings.
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="n">
+        <v>43</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>Payment of Moneys</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t xml:space="preserve">(a)Upon receipt of Proper Instructions, which may be standing instructions, the Custodian shall pay out from the respective Securities Account designated by the Company (or remit to its agents or its Sub-Custodian, and direct them to pay out) moneys of the Company on deposit therein in the following cases:
+(i)upon the purchase of Securities for the Company pursuant to such Proper Instructions; and such purchase may, unless and except to the extent otherwise directed by Proper Instructions, be carried out by the Custodian:
+12
+(A) in accordance with the customary or established practices and procedures in the jurisdiction or market where the transactions occur, including delivering money to the seller thereof or to a dealer therefor (or any agent for such seller or dealer) against expectation of receiving later delivery of such securities; or
+(B) in the case of a purchase effected through a Securities System, in accordance with the rules governing the operation of such Securities System;
+(ii)for the purchase or sale of foreign exchange or foreign exchange agreements for the account of the Company, including transactions executed with or through the Custodian, its agents or its Sub-Custodian, as contemplated by Section 3.7; and
+(iii)for any other purpose directed by the Company, but only upon receipt of Proper Instructions specifying the amount of such payment, and naming the Person or Persons to whom such payment is to be made.
+(b)At any time or times, the Custodian shall be entitled to pay (i) itself from any of the Securities Accounts, whether or not in receipt of express direction or instruction from the Company, any amounts due and payable to it pursuant to Section 8, and (ii) as otherwise permitted by Section 7.5, Section 9.4 or Section 12.5, provided, however, that in each case (i) the Custodian shall have first invoiced or billed the Company for such amounts and the Company shall have failed to pay such amounts within sixty (60) days after the date of such invoice or bill, and (ii) all such payments shall be accounted for to the Company.
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="n">
+        <v>44</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>Proxies</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> The Custodian will, with respect to the Securities held hereunder, use reasonable efforts to cause to be promptly executed by the registered holder of such Securities proxies received by the Custodian from its agents or its Sub-Custodian or from issuers of the Securities being held for the Company, without indication of the manner in which such proxies are to be voted, and upon receipt of Proper Instructions shall promptly deliver to the applicable issuer such proxies, proxy soliciting materials and notices relating to such Securities. In the absence of such Proper Instructions, or in the event that such Proper Instructions are not received in a timely fashion, the Custodian shall be under no duty to act with regard to such proxies. Notwithstanding the above, neither Custodian nor any nominee of the Custodian shall vote any of the Securities held hereunder by or for the account of the Company, except in accordance with Proper Instructions.
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>Communications Relating to Securities</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> The Custodian shall transmit promptly to the Company all written information (including proxies, proxy soliciting materials, notices, pendency of calls and maturities of Securities and expirations of rights in connection therewith) received by the Custodian, from its agents or its Sub-Custodian or from issuers of the Securities being held for the Company. The Custodian shall have no obligation or duty to exercise any right or power, or otherwise to preserve rights, in or under any Securities unless and except to the extent it has received timely Proper Instruction from the Company in accordance with the next sentence. The Custodian will not be liable for any untimely exercise of any right or power in connection with Securities at any time held by the Custodian, its agents or Sub-Custodian unless:
+13
+(i)the Custodian has received Proper Instructions with regard to the exercise of any such right or power; and
+(ii)the Custodian, or its agents or Sub-Custodian are in actual possession of such Securities,
+in each case, at least three (3) Business Days prior to the date on which such right or power is to be exercised. It will be the responsibility of the Company to notify the Custodian of the Person to whom such communications must be forwarded under this Section.
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="1" t="n">
+        <v>46</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>Records</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> The Custodian shall create and maintain complete and accurate records relating to its activities under this Agreement with respect to the Securities, cash or other property held for the Company under this Agreement. To the extent that the Custodian, in its sole opinion, is able to do so, the Custodian shall provide assistance to the Company (at the Company's reasonable request made from time to time) by providing sub-certifications regarding certain of its services performed hereunder to the Company in connection with the Company's certification requirements pursuant to applicable law, including the Sarbanes-Oxley Act of 2002, as amended. All such records shall be the property of the Company and shall at all times during the regular business hours of the Custodian be open for inspection by duly authorized officers, employees or agents of the Company, upon reasonable request with at least five (5) Business Days' prior written notice and at the Company's expense. The Custodian shall, at the Company's request, supply the Company with a tabulation of securities owned by the Company and held by the Custodian and shall, when requested to do so by the Company and for such compensation as shall be agreed upon between the Company and the Custodian, include, to the extent applicable, the certificate numbers in such tabulations, to the extent such information is available to the Custodian.
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>Custody of Subsidiary Securities</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t xml:space="preserve">(a)At the request of the Company, with respect to each Subsidiary identified to the Custodian by the Company, there shall be established by the Custodian at U.S. Bank National Association or its affiliate a segregated account to which the Custodian shall deposit and hold any Subsidiary Securities (other than Loans) (and any Proceeds received by it in the form of dividends in kind) and any cash Proceeds received by it from time to time from or with respect to Subsidiary Securities received by it pursuant to this Agreement, which account shall be in the name of the Subsidiary (the "Subsidiary Securities Accounts") and the initial Subsidiary Securities Accounts are listed on Exhibit A.
+(b) To the maximum extent possible, the provisions of this Agreement regarding Securities of the Company, the Securities Account shall be applicable to any Subsidiary Securities, cash and other investment assets, Subsidiary Securities Account. The parties hereto agree that the Company shall notify the Custodian in writing as to the establishment of any Subsidiary as to which the Custodian is to serve as custodian pursuant to the terms of this Agreement; and identify in writing any accounts the Custodian shall be required to establish for such Subsidiary as herein provided. The Company hereby notifies the Custodian that, as of the date of this Agreement, Prospect Flexible Funding, LLC is a Subsidiary for purposes of this Agreement and the Accounts listed on Exhibit A.
+14
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="1" t="n">
+        <v>48</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>Responsibility for Property Held by Sub-Custodians</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> The Custodian may appoint one or more Sub-Custodians to establish and maintain arrangements with (i) Eligible Securities Depositories or (ii) Eligible Foreign Custodians. The Custodian's responsibility with respect to the selection or appointment of a Sub-Custodian (other than an affiliate of the Custodian) shall be limited to a duty to exercise reasonable care and good faith in the selection of such Sub-Custodian in light of prevailing settlement and securities handling practices, procedures and controls in the relevant market. To the extent permitted by applicable law, the Custodian shall request each Sub-Custodian to identify on its own books and records that any assets held at such Sub-Custodian by Custodian on behalf of its customers belong to customers of the Custodian, such that it is readily apparent that such assets do not belong to the Custodian or such Sub-Custodian. With respect to any costs, expenses, damages, liabilities, or claims (including attorneys' and accountants' fees) incurred as a result of the acts or the failure to act by any Sub-Custodian (other than an affiliate of the Custodian), the Custodian shall take reasonable action to recover such costs, expenses, damages, liabilities, or claims from such Sub-Custodian; provided that the Custodian's sole liability in that regard shall be limited to amounts actually received by it from such Sub-Custodian (exclusive of related costs and expenses incurred by the Custodian).
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="1" t="n">
+        <v>49</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr"/>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>REPORTING</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t xml:space="preserve">4.1 If requested by the Company, the Custodian shall render to the Company a monthly report of (i) all deposits to and withdrawals from the Securities Account during the month, and the outstanding balance (as of the last day of the preceding monthly report and as of the last day of the subject month), (ii) an itemized statement of the Securities held pursuant to this Agreement as of the end of each month, all transactions in the Securities during the month, as well as a list of all Securities transactions that remain unsettled at that time, and (iii) such other matters as the parties may agree from time to time.
+4.2 For each Business Day, the Custodian shall render to the Company a daily report of (i) all deposits to and withdrawals from the Securities Account for such Business Day and the outstanding balance as of the end of such Business Day, (ii) a report of settled trades of Securities for such Business Day, (iii) all holdings as of such Business Day and (iv) any cash or Securities expected to have been received in the Securities Account that were not received.
+4.3 The Custodian shall have no duty or obligation to undertake any market valuation of the Securities under any circumstance.
+4.4 The Custodian shall provide the Company, promptly upon request, with such reports as are reasonably available to it and as the Company may reasonably request from time to time, on the internal accounting controls and procedures for safeguarding securities, which are employed by the Custodian.
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>In accordance with Section 3</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t xml:space="preserve">12, at the reasonable request of, and at the expense of, the Company, the Custodian agrees to reasonably cooperate with the Company's independent public accountants and shall provide requested information to the extent such information is reasonably available to the Custodian.
+15
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="1" t="n">
+        <v>51</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr"/>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>DEPOSIT IN U</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t xml:space="preserve">S. SECURITIES SYSTEMS
+The Custodian may deposit and/or maintain Securities in a Securities System within the United States ("U.S. Securities System") in accordance with applicable Federal Reserve Board and Securities and Exchange Commission rules and regulations, including Rule 17 f-4 under the 1940 Act, and subject to the following provisions:
+(a)The Custodian may keep domestic Securities in a U.S. Securities System provided that such Securities are represented in an account of the Custodian in the U.S. Securities System which shall not include any assets of the Custodian other than assets held by it as a fiduciary, custodian or otherwise for customers;
+(b)The records of the Custodian with respect to Securities which are maintained in a U.S. Securities System shall identify by book-entry those Securities belonging to the Company;
+(c)If requested by the Company, the Custodian shall provide to the Company copies of all notices received from the U.S. Securities System of transfers of Securities for the account of the Company; and
+(d)Anything to the contrary in this Agreement notwithstanding, the Custodian shall not be liable to the Company for any direct loss, damage, cost, expense, liability or claim to the Company resulting from use of any Securities System (other than to the extent resulting from the gross negligence, willful misconduct or bad faith of the Custodian itself or from failure of the Custodian to enforce effectively such rights as it may have against the U.S. Securities System).
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="1" t="n">
+        <v>52</v>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr"/>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>SECURITIES HELD OUTSIDE OF THE UNITED STATES</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr"/>
+    </row>
+    <row r="55">
+      <c r="A55" s="1" t="n">
+        <v>53</v>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>Appointment of Foreign Sub-custodian</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> The Company hereby authorizes and instructs the Custodian in its sole discretion to employ one or more Foreign Sub-custodians to act as Eligible Securities Depositories or as sub-custodian to hold the Securities and other assets of the Company maintained outside the United States, subject to the Company's approval in accordance with this Section. If the Custodian wishes to appoint a Foreign Sub-custodian to hold property of the Company subject to this Agreement, it will so notify the Company and provide it with information reasonably necessary to determine any such new Foreign Sub-custodian's eligibility under Rule 17 f-5 under the 1940 Act, including a copy of the proposed agreement with such Foreign Sub-custodian. The Company shall at the meeting of its Board of Directors next following receipt of such notice and information give a written approval or disapproval of the proposed action.
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="1" t="n">
+        <v>54</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>Assets to be Held</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> The Custodian shall limit the Securities and other assets maintained in the custody of the Foreign Sub-custodian to: (a) Foreign Securities and (b) cash and cash equivalents in such amounts as the Company (through Proper Instructions) may determine to be reasonably necessary to effect the Company's transactions in such investments.
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="1" t="n">
+        <v>55</v>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>Omnibus Accounts</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> The Custodian may hold Foreign Securities and related Proceeds with one or more Foreign Sub-custodians in each case in a single account with such Foreign Sub-custodian that is identified as belonging to the Custodian for the benefit of its customers; provided however, that the records of the Custodian with respect to
+16
+Securities and related Proceeds that are property of the Company maintained in such account(s) shall identify by book-entry those Securities and other property as belonging to the Company.
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="1" t="n">
+        <v>56</v>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>Reports Concerning Foreign Sub-custodian</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> The Custodian will supply to the Company, upon request from time to time, statements in respect of the Securities held by Foreign Sub-custodians or Eligible Securities Depositories, including an identification of the Foreign Sub-custodians and Eligible Securities Depositories having physical possession of the Foreign Securities.
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="1" t="n">
+        <v>57</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>Transactions in Foreign Custody Account</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Notwithstanding any provision of this Agreement to the contrary, settlement and payment for Securities received by a Foreign Sub-custodian for the account of the Company may be effected in accordance with the customary established securities trading or securities processing practices and procedures in the jurisdiction or market in which the transaction occurs, including delivering securities to the purchaser thereof or to a dealer therefor (or an agent for such purchaser or dealer) against a receipt with the expectation of receiving later payment for such securities from such purchaser or dealer.
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="1" t="n">
+        <v>58</v>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>Foreign Sub-custodian</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Each contract or agreement pursuant to which the Custodian employs a Foreign Sub-custodian shall include provisions that provide: (i) for indemnification or insurance arrangements (or any combination of the foregoing) such that the Company will be adequately protected against the risk of loss of assets held in accordance with such contract; (ii) that the Company's assets will not be subject to any right, charge, security interest, lien or claim of any kind in favor of the Sub-custodian or its creditors (except a claim of payment for their safe custody or administration) or, in the case of cash deposits, liens or rights in favor of creditors of the Sub-custodian arising under bankruptcy, insolvency, or similar laws; (iii) that beneficial ownership for the Company's assets will be freely transferable without the payment of money or value other than for safe custody or administration; (iv) that adequate records will be maintained identifying the assets as belonging to the Company or as being held by a third party for the benefit of the Company; (v) that the Company's independent public accountants will be given access to those records or confirmation of the contents of those records; and (vi) that the Company will receive periodic reports with respect to the safekeeping of the Company's assets, including notification of any transfer to or from a Company's account or a third party account containing assets held for the benefit of the Company. Such contract may contain, in lieu of any or all of the provisions specified above, such other provisions that the Custodian determines will provide, in their entirety, the same or a greater level of care and protection for Company assets as the specified provisions, in their entirety.
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="1" t="n">
+        <v>59</v>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>Custodian's Responsibility for Foreign Sub-custodian</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t xml:space="preserve">(a)With respect to its responsibilities under this Section 6, the Custodian agrees to exercise reasonable care, prudence and diligence such as a person having responsibility for the safekeeping of property of the Company would exercise. The Custodian further agrees that the Foreign Securities will be subject to reasonable care, based on the standards applicable to the Custodian in the relevant market, if maintained with each Foreign Sub-custodian, after considering all factors relevant to the safekeeping of such assets, including: (i) the Foreign Sub-custodian's practices, procedures, and internal controls, including the physical protections available for certificated securities (if applicable), the method of keeping custodial records, and the security and data protection practices;
+17
+(ii) whether the Foreign Sub-custodian has the requisite financial strength to provide reasonable care for Company assets; (iii) the Foreign Sub-custodian's general reputation and standing and, in the case of Eligible Securities Depository, the Eligible Securities Depository's operating history and number of participants; and (iv) whether the Company will have jurisdiction over and be able to enforce judgments against the Foreign Sub-custodian, such as by virtue of the existence of any offices of the Foreign Sub-custodian in the United States or the Sub-custodian's consent to service of process in the United States.
+(b)At the end of each calendar quarter, or at such other times as the Company's board of directors deems reasonable and appropriate based on the circumstances of the Company's foreign custody arrangements, the Custodian shall provide written reports notifying the board of directors of the Company as to the placement of the Foreign Securities and cash of the Company with a particular Foreign Sub-custodian and of any material changes in the Company's foreign custody arrangements. The Custodian shall promptly take such steps as may be required to withdraw assets of the Company from any Foreign Sub-custodian that has ceased to meet the requirements of this Section.
+(c)The Custodian shall establish a system to monitor the appropriateness of maintaining the Company's assets with a particular Foreign Sub-custodian and the performance of the contract governing the Company's arrangements with such Foreign Sub-custodian. To the extent the Custodian holds Foreign Securities and related Proceeds with one or more Eligible Securities Depositories, the Custodian shall provide the Company with an analysis of the custody risks associated with maintaining assets with such Eligible Securities Depository and shall monitor such custody risks on a continuing basis and promptly notify the Company of any material change in these risks. The Custodian agrees to exercise reasonable care, prudence and diligence in performing its obligations under this clause (c). If the Custodian determines that a custody arrangement with an Eligible Securities Depository no longer meets the requirements of this Section, the Company's Foreign Securities must be withdrawn from such depository as soon as reasonably practicable.
+(d)The Custodian's responsibility with respect to the selection or appointment of a Foreign Sub-custodian shall be limited to a duty to exercise reasonable care in the selection or retention of such Foreign Sub-custodian in light of prevailing settlement and securities handling practices, procedures and controls in the relevant market. With respect to any costs, expenses, damages, liabilities, or claims (including attorneys' and accountants' fees) incurred as a result of the acts or the failure to act by any Foreign Sub-custodian, the Custodian shall take reasonable action to recover such costs, expenses, damages, liabilities, or claims from such Foreign Sub-custodian; provided that the Custodian's sole liability in that regard shall be limited to amounts actually received by it from such Foreign Sub-custodian (exclusive of related costs and expenses incurred by the Custodian). The Custodian shall have no responsibility for any act or omission (or the insolvency of) any Securities System (including an Eligible Securities Depository).
+18
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="1" t="n">
+        <v>60</v>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr"/>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>CERTAIN GENERAL TERMS</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr"/>
+    </row>
+    <row r="63">
+      <c r="A63" s="1" t="n">
+        <v>61</v>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>No Duty to Examine Financing Documents</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Nothing herein shall obligate the Custodian to review or examine the terms of any Financing Document, underlying instrument, certificate, credit agreement, indenture, loan agreement, promissory note, or other financing document evidencing or governing any Security to determine the validity, sufficiency, marketability or enforceability of any Security (and shall have no responsibility for the genuineness or completeness thereof), or otherwise.
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="1" t="n">
+        <v>62</v>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>Resolution of Discrepancies</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> In the event of any discrepancy between the information set forth in any report provided by the Custodian to the Company and any information contained in the books or records of the Company, the Company shall promptly notify the Custodian thereof and the parties shall cooperate to diligently resolve the discrepancy.
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="1" t="n">
+        <v>63</v>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>Improper Instructions</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Notwithstanding anything herein to the contrary, the Custodian shall not be obligated to take any action (or forebear from taking any action), which it reasonably determines (at its sole option) to be contrary to the terms of this Agreement or applicable law. In no instance shall the Custodian be obligated to provide services on any day that is not a Business Day.
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="1" t="n">
+        <v>64</v>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>Proper Instructions</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t xml:space="preserve">(a)The Company will give written notice to the Custodian, in form acceptable to the Custodian, specifying the names and specimen signatures (whether manual, facsimile, pdf or other electronic signature) of persons authorized to give Proper Instructions (collectively, "Authorized Persons" and each is an "Authorized Person") which notice shall be signed (whether manual, facsimile, pdf or other electronic signature) by an Authorized Person previously certified to the Custodian. The Custodian shall be entitled to rely upon the identity and authority of such persons until it receives written notice from an Authorized Person of the Company to the contrary. The initial Authorized Persons are set forth on Schedule A attached hereto and made a part hereof (as such Schedule A may be modified from time to time by written notice from the Company to the Custodian). The Custodian shall be entitled to accept and act upon Proper Instructions sent by unsecured email, facsimile transmission or other similar unsecured electronic methods. If such person on behalf of the Company elects to give the Custodian email or facsimile instructions (or instructions by a similar electronic method) and the Custodian in its discretion elects to act upon such instructions, the Custodian's reasonable understanding of such instructions shall be deemed controlling. The Custodian shall not be liable for any losses, costs or expenses arising directly or indirectly from the Custodian's reliance upon and compliance with such instructions notwithstanding such instructions conflicting with or being inconsistent with a subsequent written instruction. The Company agrees to assume all risks arising out of the use of such electronic methods to submit instructions and directions to the Custodian, including without limitation the risk of the Custodian acting on unauthorized instructions, and the risk of interception and misuse by third parties and acknowledges and agrees that there may be more secure methods of transmitting such instructions than the method(s) selected by it and agrees that the security procedures (if any) to be followed in connection with its transmission of such instructions provide to it a commercially reasonable degree of protection in light of its particular needs and circumstances. The Company hereby authorizes and directs the Custodian to accept, rely and act
+19
+upon instruction from the Investment Manager, acting on behalf and in the name of the Company for all purposes hereunder, and the Custodian is authorized to recognize and act upon the instruction of the Investment Adviser, acting alone, on behalf and in the stead of the Company for all purposes hereunder; provided that such authorization and direction may be revoked at any time by an Authorized Person who is an officer of the Company (and each reference in this Agreement to the Company shall be deemed to include and apply to the Investment Adviser).
+(b)The Custodian shall have no responsibility or liability to the Company (or any other person or entity), and shall be indemnified and held harmless by the Company, in the event that a subsequent written confirmation of an oral instruction fails to conform to the oral instructions received by the Custodian. The Custodian shall not have an obligation to act in accordance with purported instructions to the extent that they conflict with applicable law or regulations, local market practice or the Custodian's operating policies and practices. The Custodian shall not be liable for any loss resulting from a delay while it obtains clarification of any Proper Instructions.
+(c)Reserved.
+(d)The Company hereby agrees that directions given by it pursuant to secure financial messaging services provided by SWIFT ("SWIFT Transmissions") are deemed to Proper Instructions for all purposes hereunder. The Company instructs the Custodian to accept and record SWIFT Transmissions initiated by the Company (or the Advisor on its behalf) to the same extent that written wire transfer instructions are accepted and processed by the Custodian. The Custodian may conclusively rely on SWIFT Transmissions and the Custodian shall be entitled to and the Company agrees to provide any verification of information as requested by the Custodian, including the call back process to an individual designated by the Company as authorized to provide such verification. The Custodian may also request, and the Company will provide, an additional signed direction (whether by manual, facsimile, .pdf or other electronic signature) in connection with any SWIFT Transmission. For purposes of compliance with any incumbency certificate of the Company, all instructions received by the Custodian through the methodology described herein shall be deemed in compliance with the procedures outlined therein (to the extent applicable).
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="1" t="n">
+        <v>65</v>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>Actions Permitted Without Express Authority</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> The Custodian may, at its discretion, without express authority from the Company:
+(a)make payments to itself as described in or pursuant to Section 3.9(b), or to make payments to itself or others for expenses of handling securities or other similar items relating to its duties under this Agreement, provided that (i) the Custodian shall have first invoiced or billed the Company for such amounts and the Company shall have failed to pay such amounts within thirty (30) days after the date of such invoice or bill, and (ii) all such payments shall be accounted for to the Company;
+(b)surrender Securities in temporary form for Securities in definitive form;
+(c)endorse for collection cheques, drafts and other negotiable instruments; and
+20
+(d)in general, attend to all nondiscretionary details in connection with the sale, exchange, substitution, purchase, transfer and other dealings with the securities and property of the Company.
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="1" t="n">
+        <v>66</v>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>Evidence of Authority</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> The Custodian shall be protected in acting upon any instructions, notice, request, consent, certificate instrument or paper reasonably believed by it to be genuine and to have been properly executed (whether manual, facsimile, pdf or other electronic signature) or otherwise given by or on behalf of the Company by an Authorized Person. The Custodian may receive and accept a certificate signed (whether manual, facsimile, pdf or other electronic signature) by any Authorized Person as conclusive evidence of:
+(a)the authority of any person to act in accordance with such certificate; or
+(b)any determination or of any action by the Company as described in such certificate,
+and such certificate may be considered as in full force and effect until receipt by the Custodian of written notice to the contrary from an Authorized Person of the Company.
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="1" t="n">
+        <v>67</v>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>Receipt of Communications</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Any communication received by the Custodian on a day which is not a Business Day or after 3:30 p.m., Eastern time (or such other time as is agreed by the Company and the Custodian from time to time), on a Business Day will be deemed to have been received on the next Business Day (but in the case of communications so received after 3:30 p.m., Eastern time, on a Business Day, the Custodian will use reasonable efforts to process such communications as soon as possible after receipt).
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="1" t="n">
+        <v>68</v>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>Actions on the Loans</t>
+        </is>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> The Custodian shall have no duty or obligation hereunder to take any action on behalf of the Company, to communicate on behalf of the Company, to collect amounts or proceeds in respect of, or otherwise to interact or exercise rights or remedies on behalf of the Company, with respect to any of the Loans. All such actions and communications are the responsibility of the Company.
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="1" t="n">
+        <v>69</v>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr"/>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>COMPENSATION OF CUSTODIAN</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr"/>
+    </row>
+    <row r="72">
+      <c r="A72" s="1" t="n">
+        <v>70</v>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>Fees</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> The Custodian shall be entitled to compensation for its services in accordance with the terms of that certain fee letter between the Company and the Custodian.
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="1" t="n">
+        <v>71</v>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>Expenses</t>
+        </is>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> The Company agrees to pay or reimburse to the Custodian upon its request from time to time all reasonable, out-of-pocket costs, disbursements, advances, expenses and indemnification amounts (including reasonable and documented out-of-pocket fees and expenses of legal counsel) incurred, and any disbursements and advances made (including any account overdraft resulting from any settlement or assumed settlement, provisional credit, chargeback, returned deposit item, reclaimed payment or claw-back, or the like), in connection with the preparation, execution or enforcement of this Agreement, or in connection with the transactions contemplated hereby or the administration of this Agreement or performance by the Custodian of its duties and services under this Agreement, from time to time (including costs and expenses of any action deemed necessary by the Custodian to collect any amounts owing to it under this Agreement).
+21
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="1" t="n">
+        <v>72</v>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr"/>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>RESPONSIBILITY OF CUSTODIAN</t>
+        </is>
+      </c>
+      <c r="E74" t="inlineStr"/>
+    </row>
+    <row r="75">
+      <c r="A75" s="1" t="n">
+        <v>73</v>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>General Duties</t>
+        </is>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> The Custodian shall have no duties, obligations or responsibilities under this Agreement or with respect to the Securities or Proceeds except for such duties as are expressly and specifically set forth in this Agreement, and the duties and obligations of the Custodian shall be determined solely by the express provisions of this Agreement. No implied duties, obligations or responsibilities shall be read into this Agreement against, or on the part of, the Custodian.
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="1" t="n">
+        <v>74</v>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>Instructions</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t xml:space="preserve">(a)The Custodian shall be entitled to refrain from taking any action unless it has such instruction (in the form of Proper Instructions) from the Company as it reasonably deems necessary, and shall be entitled to require, upon notice to the Company, that Proper Instructions to it be in writing. The Custodian shall have no liability for any action (or forbearance from action) taken pursuant to the Proper Instruction of the Company.
+(b)Whenever the Custodian is entitled or required to receive or obtain any communications or information pursuant to or as contemplated by this Agreement, it shall be entitled to receive the same in writing, in form, content and medium reasonably acceptable to it and otherwise in accordance with any applicable terms of this Agreement; and whenever any report or other information is required to be produced or distributed by the Custodian, it shall be in form, content and medium reasonably acceptable to it and the Company, and otherwise in accordance with any applicable terms of this Agreement.
+9.3 General Standards of Care. Notwithstanding any terms herein contained to the contrary, the acceptance by the Custodian of its appointments hereunder is expressly subject to the following terms, which shall govern and apply to each of the terms and provisions of this Agreement (whether or not so stated therein): 
+(a)The Custodian may rely on and shall be protected in acting or refraining from acting in reliance upon any written notice, instruction, statement, certificate, request, waiver, consent, opinion, report, receipt or other paper, electronic communication or document furnished to it (including any of the foregoing provided to it by facsimile or electronic means), not only as to its due execution and validity, but also as to the truth and accuracy of any information therein contained, which it in good faith believes to be genuine and signed (whether manual, facsimile, pdf or other electronic signature), sent or presented by the proper person (which in the case of any instruction from or on behalf of the Company shall be an Authorized Person); and the Custodian shall be entitled to presume the genuineness and due authority of any signature (whether manual, facsimile, pdf or other electronic signature) appearing thereon. The Custodian shall not be bound to make any independent investigation into the facts or matters stated in any such notice, instruction, statement, certificate, request, waiver, consent, opinion, report, receipt, electronic communication or other paper or document.
+(b)Neither the Custodian nor any of its directors, officers or employees shall be liable to anyone for any error of judgment, or for any act done or step taken or
+22
+omitted to be taken by it (or any of its directors, officers or employees), or for any mistake of fact or law, or for anything which it may do or refrain from doing in connection herewith, unless such action or inaction constitutes gross negligence, willful misconduct or fraud on its part and in breach of the terms of this Agreement. The Custodian shall not be liable for any action taken by it in good faith and reasonably believed by it to be within powers conferred upon it, or taken by it pursuant to any direction or instruction by which it is governed hereunder, or omitted to be taken by it by reason of the lack of direction or instruction required hereby for such action. The Custodian shall not be under any obligation at any time to ascertain whether the Company is in compliance with (i) the 1940 Act, the regulations thereunder, or the Company's investment objectives and policies then in effect or (ii) any restrictions, covenants, limitations or obligations to which the Company may be subject. For avoidance of doubt, the Custodian shall not be under any obligation to determine whether any investment constitutes an Eligible Investment under this Agreement.
+(c)In no event shall the Custodian be liable for any indirect, incidental, special, punitive or consequential damages (including lost profits or diminution of value), whether or not it has been advised of the likelihood of such damages.
+(d)The Custodian may consult with, and obtain advice from, legal counsel selected in good faith with respect to any question as to any of the provisions hereof or its duties hereunder, or any matter relating hereto, and the written opinion or advice of such counsel shall be full and complete authorization and protection in respect of any action taken, suffered or omitted by the Custodian in good faith in accordance with the opinion and directions of such counsel; the reasonable cost of such services shall be reimbursed pursuant to Section 8.2.
+(e)The Custodian shall not be deemed to have notice of any fact, claim or demand with respect hereto unless actually known by an officer working in its Global Corporate Trust group and charged with responsibility for administering this Agreement or unless (and then only to the extent received) in writing by the Custodian at the applicable address(es) as set forth in Section 15 and specifically referencing this Agreement.
+(f)No provision of this Agreement shall require the Custodian to expend or risk its own funds, or to take any action (or forbear from action) hereunder which might in its judgment involve any expense or any financial or other liability unless it shall be furnished with acceptable indemnification. Nothing herein shall obligate the Custodian to commence, prosecute or defend legal proceedings in any instance, whether on behalf of the Company or on its own behalf or otherwise, with respect to any matter arising hereunder, or relating to this Agreement or the services contemplated hereby.
+(g)The permissive right of the Custodian to take any action hereunder shall not be construed as a duty.
+(h)The Custodian may act or exercise its duties or powers hereunder through agents, Sub-Custodians or attorneys, and the Custodian shall not be liable or responsible for the actions or omissions of any such agent, Sub-Custodian or attorney appointed with due care.
+23
+(i)All indemnifications contained in this Agreement in favor of the Custodian shall survive the termination of this Agreement or the earlier resignation or removal of the Custodian.
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>Indemnification; Custodian's Lien</t>
+        </is>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t xml:space="preserve">(a)The Company shall and does hereby indemnify and hold harmless the Custodian, any Foreign Sub-custodian and each of its officers, directors, employees, attorneys, agents, advisors, successors and assigns (collectively, the "Indemnified Persons" and each an "Indemnified Person") for and from any and all costs and expenses (including reasonable and documented attorney's fees and expenses), and any and all losses, damages, claims (whether brought by or involving the Company or any third party) and liabilities, that may arise, be brought against or incurred by an Indemnified Person whether brought by or involving any third party or the Company and whether direct, indirect or consequential, as a result of or arising from or in any way relating to any claim, demand, suit, action or proceeding (including any inquiry or investigation) by any person, including without limitation the Company or any Subsidiary, and any advances or disbursements made by the Custodian (including in respect of any Account overdraft, returned deposit item, chargeback, provisional credit, settlement or assumed settlement, reclaimed payment, claw-back or the like), as a result of, relating to, or arising out of this Agreement, or the administration or performance of the Custodian's duties hereunder, the enforcement of any provision of this Agreement or the relationship between the Company (including, for the avoidance of doubt, any Subsidiary) and the Custodian created hereby, other than such liabilities, losses, damages, claims, costs and expenses as are directly caused by the Custodian's action or inaction constituting gross negligence, bad faith, fraud or willful misconduct.
+(b)The Custodian shall have and is hereby granted a continuing lien upon and security interest in, and right of set-off against, the Account, and any funds (and investments in which such funds may be invested) held therein or credited thereto from time to time, whether now held or hereafter required, and all proceeds thereof, to secure the payment of any amounts that may be owing to the Custodian under or pursuant to the terms of this Agreement, whether now existing or hereafter arising.
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="1" t="n">
+        <v>76</v>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>Force Majeure</t>
+        </is>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Without prejudice to the generality of the foregoing, the Custodian shall be without liability to the Company for any damage or loss resulting from or caused by events or circumstances beyond the Custodian's reasonable control including nationalization, expropriation, currency restrictions, the interruption, disruption or suspension of the normal procedures and practices of any securities market, power, mechanical, communications or other technological failures or interruptions, computer viruses or the like, fires, floods, earthquakes or other natural disasters, civil and military disturbance, acts of war or terrorism, riots, revolution, acts of God, work stoppages, strikes, national disasters of any kind, or other similar events or acts; errors by the Company (including any Authorized Person) in its instructions to the Custodian; or changes in applicable law, regulation or orders.
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="1" t="n">
+        <v>77</v>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr"/>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>SECURITY CODES</t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t xml:space="preserve">If the Custodian issues to the Company security codes, passwords or test keys in order that it may verify that certain transmissions of information, including Proper Instructions, have been
+24
+originated by the Company, the Company shall take all commercially reasonable steps to safeguard any security codes, passwords, test keys or other security devices which the Custodian shall make available.
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="1" t="n">
+        <v>78</v>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr"/>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>TAX LAW</t>
+        </is>
+      </c>
+      <c r="E80" t="inlineStr"/>
+    </row>
+    <row r="81">
+      <c r="A81" s="1" t="n">
+        <v>79</v>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>Domestic Tax Law</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> The Custodian shall have no responsibility or liability for any obligations now or hereafter imposed on the Company or the Custodian as custodian of the Securities or the Proceeds, by the tax law of the United States or any state or political subdivision thereof. The Custodian shall be kept indemnified by and be without liability to the Company for such obligations including taxes, (but excluding any income taxes assessable in respect of compensation paid to the Custodian pursuant to this Agreement) withholding, certification and reporting requirements, claims for exemption or refund, additions for late payment interest, penalties and other expenses (including legal expenses) that may be assessed against the Company, or the Custodian as custodian of the Securities or Proceeds.
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="1" t="n">
+        <v>80</v>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>Foreign Tax Law</t>
+        </is>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> It shall be the responsibility of the Company to notify the Custodian of the obligations imposed on the Company, or the Custodian as custodian of any foreign securities or related Proceeds, by the tax law of foreign (e.g., non-U.S.) jurisdictions, including responsibility for withholding and other taxes, assessments or other government charges, certifications and government reporting. The sole responsibility of the Custodian with regard to such tax law shall be to use reasonable efforts to cooperate with the Company with respect to any claims for exemption or refund under the tax law of the jurisdictions for which the Company has provided such information.
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="1" t="n">
+        <v>81</v>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr"/>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>EFFECTIVE PERIOD AND TERMINATION</t>
+        </is>
+      </c>
+      <c r="E83" t="inlineStr"/>
+    </row>
+    <row r="84">
+      <c r="A84" s="1" t="n">
+        <v>82</v>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>Effective Date</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> This Agreement shall become effective as of its due execution (whether manual, facsimile, pdf or other electronic signature) and delivery by each of the parties. This Agreement shall continue in full force and effect until terminated as hereinafter provided. This Agreement may only be amended by mutual written agreement of the parties hereto. This Agreement may be terminated by the Custodian or the Company pursuant to Section 12.2.
+12.2 Termination. This Agreement shall terminate upon the earliest of (a) occurrence of the effective date of termination specified in any written notice of termination given by either party to the other not later than sixty (60) days prior to the effective date of termination specified therein, and (b) such other date of termination as may be mutually agreed upon by the parties in writing.
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="1" t="n">
+        <v>83</v>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>Resignation</t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> The Custodian may at any time resign under this Agreement by giving not less than sixty (60) days advance written notice thereof to the Company. The Company may at any time remove the Custodian under this Agreement by giving not less than sixty (60) days advance written notice to the Custodian.
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="1" t="n">
+        <v>84</v>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>Successor</t>
+        </is>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Prior to the effective date of termination of this Agreement, or the effective date of the resignation or removal of the Custodian, as the case may be, the Company shall give Proper Instruction to the Custodian designating a successor Custodian, if applicable. The Custodian shall, upon receipt of Proper Instruction from the Company (i) deliver directly to the successor Custodian all Securities (other than Securities held in a Book-Entry System or Securities Depository) and cash then owned by
+25
+the Company and held by the Custodian as custodian, and (ii) transfer any Securities held in a Book-Entry System or Securities Depository to an account of or for the benefit of the Company at the successor Custodian, provided that the Company shall have paid to the Custodian all fees, expenses and other amounts to the payment or reimbursement of which it shall then be entitled. In addition, the Custodian shall, at the expense of the Company, transfer to each successor all relevant books, records, correspondence, and other data established or maintained by the Custodian under the Agreement (if such form differs from the form in which the Custodian has maintained the same, the Company shall pay any reasonable and documented expenses associated with transferring the data to such form) and will cooperate in the transfer of such duties and responsibilities. Upon such delivery and transfer, the Custodian shall be relieved of all obligations under this Agreement.
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="1" t="n">
+        <v>85</v>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>Payment of Fees, etc</t>
+        </is>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Upon termination of this Agreement or resignation of the Custodian, the Company shall pay to the Custodian such compensation, and shall likewise reimburse the Custodian for its costs, expenses and disbursements, as may be due as of the date of such termination or resignation (or removal, as the case may be). All indemnifications in favor of the Custodian under this Agreement shall survive the termination of this Agreement, or any resignation or removal of the Custodian.
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="1" t="n">
+        <v>86</v>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>Final Report</t>
+        </is>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> In the event of any resignation or removal of the Custodian, the Custodian shall provide to the Company a complete final report or data file transfer of any Confidential Information as of the date of such resignation or removal.
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="1" t="n">
+        <v>87</v>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr"/>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>REPRESENTATIONS AND WARRANTIES</t>
+        </is>
+      </c>
+      <c r="E89" t="inlineStr"/>
+    </row>
+    <row r="90">
+      <c r="A90" s="1" t="n">
+        <v>88</v>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>Representations of the Company</t>
+        </is>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> The Company represents and warrants to the Custodian that:
+(a)it has the power and authority to enter into and perform its obligations under this Agreement, and it has duly authorized, executed and delivered this Agreement so as to constitute its valid and binding obligation;
+(b)in giving any instructions which purport to be "Proper Instructions" under this Agreement, the Company will act in accordance with the provisions of its governing documents and any applicable laws and regulations.
+(c)the Company is not a Plan-Assets Vehicle (as defined below); (ii) the Company is not subject to the Employee Retirement Income Security Act of 1974, as amended ("ERISA"), (iii) the aggregate interest in any class of equity interests by any benefit plan investors (as such term is interpreted under ERISA) for whose benefit or account the Accounts for such Company is held does not equal or exceed 25% of the outstanding interests; and neither the portfolio of the Securities or the Accounts for such Company is deemed to be assets of an employee benefit plan which is subject to ERISA. If for any reason the Company breaches or otherwise fails to comply with any of the foregoing representations, warranties, or covenants, then (i) the Custodian's duties hereunder with respect to such Company terminates immediately upon such breach, regardless of whether the Custodian received notice of such breach or provided notice of termination and promptly thereafter, the Company and the Custodian shall negotiate in good faith to enter into a separate ERISA fund custody agreement, (ii) the Company will promptly notify the Custodian of such breach, (iii) the Company acknowledges
+26
+that the Custodian does not act as investment manager of the Securities or the Accounts and (iv) the Company acknowledges that the Custodian does not provide any services as a "fiduciary" with respect to the Company within the meaning of ERISA SS3(21). For purposes herein, "Plan-assets Vehicle" means an investment contract, product, or entity that holds plan assets (as determined pursuant to ERISA SSSS3(42) and 401 and 29 CFR SS2510.3-101.
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="1" t="n">
+        <v>89</v>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>Representations of the Custodian</t>
+        </is>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> The Custodian hereby represents and warrants to the Company that:
+(a)it has the power and authority to enter into and perform its obligations under this Agreement;
+(b)it has duly authorized, executed and delivered this Agreement so as to constitute its valid and binding obligations;
+(c) it is qualified to act as a custodian pursuant to Section 26(a)(1) of the 1940 Act; and
+(d)that it maintains business continuity policies and standards.
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="1" t="n">
+        <v>90</v>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr"/>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>PARTIES IN INTEREST; NO THIRD PARTY BENEFIT</t>
+        </is>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t xml:space="preserve">This Agreement is not intended for, and shall not be construed to be intended for, the benefit of any third parties and may not be relied upon or enforced by any third parties (other than successors and permitted assigns pursuant to Section 19).
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="1" t="n">
+        <v>91</v>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr"/>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>NOTICES</t>
+        </is>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Any Proper Instructions shall be given to the following address (or such other address as either party may designate by written notice to the other party), and otherwise any notices, approvals and other communications hereunder shall be sufficient if made in writing and given to the parties at the following address (or such other address as either of them may subsequently designate by notice to the other), given by (i) certified or registered mail, postage prepaid, (ii) recognized courier or delivery service, (iii) electronic mail or (iv) confirmed facsimile, with a duplicate sent on the same day by first class mail, postage prepaid:
+(a)if to the Company or any Subsidiary, to
+Prospect Floating Rate and Alternative Income Fund, Inc.
+10 East 40 th Street, 42 nd Floor
+New York, New York 10016
+Attention: Jonathan Tepper
+Facsimile: 212-448-9652
+Email: jtepper@prospectcap.com
+lharrison@prospectcap.com
+pfloat@prospectcap.com
+pacctflex@prospectcap.com
+pl@prospectcap.com
+fax@prospectcap.com
+(b)if to the Custodian, to
+27
+U.S. Bank Trust Company, National Association
+1 Federal Street, 3 rd Floor
+Boston, MA 02110
+Attention: Roni Richman Lally
+Reference: Prospect Flexible Funding, LLC
+Email: roni.richmanlally@usbank.com
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="1" t="n">
+        <v>92</v>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr"/>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>CHOICE OF LAW AND JURISDICTION</t>
+        </is>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t xml:space="preserve">This Agreement shall be construed, and the provisions thereof interpreted under and in accordance with and governed by the laws of the State of New York for all purposes (without regard to its choice of law provisions) except to the extent such laws are inconsistent with the federal securities laws, including the 1940 Act, in which case such federal securities laws shall govern. All actions and proceedings relating to or arising from, directly or indirectly, this Agreement may be brought in New York State or U.S. federal courts located within the City of New York, State of New York and the Company and the Custodian hereby submit to personal jurisdiction of such courts for such actions or proceedings. The Company and the Custodian each hereby waives, to the fullest extent permitted by applicable law, any right it may have to a trial by jury and any objection to laying of venue in such courts on grounds of forum nonconveniens in respect of any claim based upon, arising out of or in connection with this Agreement. No actions or proceedings relating to or arising from, directly or indirectly, this Agreement shall be brought in a forum outside of the United States of America.
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="1" t="n">
+        <v>93</v>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>17</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr"/>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>ENTIRE AGREEMENT; COUNTERPARTS</t>
+        </is>
+      </c>
+      <c r="E95" t="inlineStr"/>
+    </row>
+    <row r="96">
+      <c r="A96" s="1" t="n">
+        <v>94</v>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>17</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>Complete Agreement</t>
+        </is>
+      </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> This Agreement constitutes the complete and exclusive agreement of the parties with regard to the matters addressed herein and supersedes and terminates as of the date hereof, all prior agreements, acknowledgements or understandings, oral or written between the parties to this Agreement relating to such matters.
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="1" t="n">
+        <v>95</v>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>17</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>Counterparts</t>
+        </is>
+      </c>
+      <c r="E97" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> This Agreement may be executed (whether manual, facsimile, pdf or other electronic signature) in any number of counterparts and all counterparts taken together shall constitute one and the same instrument.
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="1" t="n">
+        <v>96</v>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>17</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t>Facsimile and Electronic Signatures</t>
+        </is>
+      </c>
+      <c r="E98" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> The exchange of copies of this Agreement and of signature pages by facsimile, pdf or other electronic transmission shall constitute effective execution and delivery of this Agreement as to the parties and may be used in lieu of the original Agreement for all purposes. Signatures of the parties transmitted by facsimile or pdf shall be deemed to be their original signatures for all purposes. By executing this Agreement, the Company hereby acknowledges and agrees, and directs the Custodian to acknowledge and agree and the Custodian does hereby acknowledge and agree, that execution of this Agreement, any Proper Instructions and any other notice, form or other document executed by the Company or the Custodian in connection with this Agreement, by electronic signature (including, without limitation, any .pdf file, .jpeg file or any other electronic or image file, or any other "electronic signature" as defined under E-SIGN or ESRA, including Orbit, Adobe Sign, DocuSign, or any other similar platform identified by the Company and reasonably available at no undue burden or expense to the Custodian) shall be permitted hereunder notwithstanding anything to the contrary herein and such electronic signatures shall be legally binding as if such electronic signatures were handwritten signatures. Any electronically signed document delivered via email from a person purporting to be an Authorized Person shall be
+28
+considered signed or executed by such Authorized Person on behalf of the Company. The Company also hereby acknowledges that the Custodian shall have no duty to inquire into or investigate the authenticity or authorization of any such electronic signature and shall be entitled to conclusively rely on any such electronic signature without any liability with respect thereto.
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="1" t="n">
+        <v>97</v>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr"/>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t>AMENDMENT; WAIVER</t>
+        </is>
+      </c>
+      <c r="E99" t="inlineStr"/>
+    </row>
+    <row r="100">
+      <c r="A100" s="1" t="n">
+        <v>98</v>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D100" t="inlineStr">
+        <is>
+          <t>Amendment</t>
+        </is>
+      </c>
+      <c r="E100" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> This Agreement may not be amended except by an express written instrument duly executed by each of the Company and the Custodian.
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" s="1" t="n">
+        <v>99</v>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D101" t="inlineStr">
+        <is>
+          <t>Waiver</t>
+        </is>
+      </c>
+      <c r="E101" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> In no instance shall any delay or failure to act be deemed to be or effective as a waiver of any right, power or term hereunder, unless and except to the extent such waiver is set forth in an express written instrument signed by the party against whom it is to be charged.
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>19</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr"/>
+      <c r="D102" t="inlineStr">
+        <is>
+          <t>SUCCESSOR AND ASSIGNS</t>
+        </is>
+      </c>
+      <c r="E102" t="inlineStr"/>
+    </row>
+    <row r="103">
+      <c r="A103" s="1" t="n">
+        <v>101</v>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>19</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D103" t="inlineStr">
+        <is>
+          <t>Successors Bound</t>
+        </is>
+      </c>
+      <c r="E103" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> The covenants and agreements set forth herein shall be binding upon and inure to the benefit of each of the parties and their respective successors and permitted assigns. Neither party shall be permitted to assign their rights under this Agreement without the written consent of the other party; provided, however, that the foregoing shall not limit the ability of the Custodian to delegate certain duties or services to or perform them through agents or attorneys appointed with due care as expressly provided in this Agreement.
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" s="1" t="n">
+        <v>102</v>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>19</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D104" t="inlineStr">
+        <is>
+          <t>Merger and Consolidation</t>
+        </is>
+      </c>
+      <c r="E104" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Any corporation or association into which the Custodian may be merged or converted or with which it may be consolidated, or any corporation or association resulting from any merger, conversion or consolidation to which the Custodian shall be a party, or any corporation or association to which the Custodian transfers all or substantially all of its corporate trust business shall be the successor of the Custodian hereunder, and shall succeed to all of the rights, powers and duties of the Custodian hereunder, without the execution or filing of any paper or any further act on the part of any of the parties hereto, subject in all cases to all representations, warranties, covenants and obligations made by the Custodian hereunder. For the avoidance of doubt, no corporation or association (as described above) shall succeed to the rights, powers and duties of the Custodian hereunder unless it is a qualified custodian pursuant to Section 17(f) and Section 26(a)(1) of the 1940 Act .
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" s="1" t="n">
+        <v>103</v>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr"/>
+      <c r="D105" t="inlineStr">
+        <is>
+          <t>SEVERABILITY</t>
+        </is>
+      </c>
+      <c r="E105" t="inlineStr">
+        <is>
+          <t xml:space="preserve">The terms of this Agreement are hereby declared to be severable, such that if any term hereof is determined to be invalid or unenforceable, such determination shall not affect the remaining terms.
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" s="1" t="n">
+        <v>104</v>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr"/>
+      <c r="D106" t="inlineStr">
+        <is>
+          <t>REQUEST FOR INSTRUCTIONS</t>
+        </is>
+      </c>
+      <c r="E106" t="inlineStr">
+        <is>
+          <t xml:space="preserve">If, in performing its duties under this Agreement, the Custodian is required to decide between alternative courses of action, the Custodian may (but shall not be obliged to) request written instructions from the Company as to the course of action desired by it. If the Custodian does not receive such instructions within two (2) Business Days after it has requested them, the Custodian
+29
+may, but shall be under no duty to, take or refrain from taking any such courses of action. The Custodian shall act in accordance with instructions received from the Company in response to such request after such two (2) Business Day period except to the extent it has already taken, or committed itself to take, action inconsistent with such instructions.
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" s="1" t="n">
+        <v>105</v>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr"/>
+      <c r="D107" t="inlineStr">
+        <is>
+          <t>OTHER BUSINESS</t>
+        </is>
+      </c>
+      <c r="E107" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nothing herein shall prevent the Custodian or any of its affiliates from engaging in other business, or from entering into any other transaction or financial or other relationship with, or receiving fees from or from rendering services of any kind to the Company or any other Person. Nothing contained in this Agreement shall constitute the Company and/or the Custodian (and/or any other Person) as members of any partnership, joint venture, association, syndicate, unincorporated business or similar assignment as a result of or by virtue of the engagement or relationship established by this Agreement.
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" s="1" t="n">
+        <v>106</v>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr"/>
+      <c r="D108" t="inlineStr">
+        <is>
+          <t>REPRODUCTION OF DOCUMENTS</t>
+        </is>
+      </c>
+      <c r="E108" t="inlineStr">
+        <is>
+          <t xml:space="preserve">This Agreement and all schedules, exhibits, attachments and amendments hereto may be reproduced by any photographic, photostatic, microfilm, micro-card, miniature photographic or other similar process. The parties hereto each agree that any such reproduction shall be admissible in evidence as the original itself in any judicial or administrative proceeding, whether or not the original is in existence and whether or not such reproduction was made by a party in the regular course of business, and that any enlargement, facsimile or further production shall likewise be admissible in evidence.
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" s="1" t="n">
+        <v>107</v>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>24</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr"/>
+      <c r="D109" t="inlineStr">
+        <is>
+          <t>CONFIDENTIAL INFORMATION</t>
+        </is>
+      </c>
+      <c r="E109" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Each party (in such capacity, the "Receiving Party") shall keep confidential any non-public information relating to the other party's business disclosed by or on behalf of such other party (in such capacity, the "Disclosing Party", and all such information collectively, "Confidential Information"), and shall use any such Confidential Information only in furtherance of its performance hereunder. Confidential Information may include: (i) any data or information that is competitively sensitive material, and not generally known to the public, including, but not limited to, information about product plans, marketing strategies, finances, operations, customer relationships, customer profiles, customer lists, sales estimates, business plans, and internal performance results relation to the past, present or future business activities of the Disclosing Party, its respective subsidiaries and affiliated companies; (ii) any scientific or technical information, design, process, procedure, formula, or improvement that is commercially valuable and secret in the sense that its confidentiality affords the Disclosing Party a competitive advantage of its competitors; (iii) all confidential or proprietary concepts, documentation, reports, data, specifications, computer software, source code, object code, flow charts, databases, documentation, reports, data, specifications, computer software, source code, object code, flow charts, databases, inventions, know-how, and trade secrets, whether or not patentable or copyrightable; and (iv) anything designated as confidential. Confidential Information shall not include information which (i) is disclosed in a publication available to the public, is otherwise in the public domain at the time of disclosure, or becomes publicly known through no breach of the terms hereof by the Receiving Party, (ii) is obtained by the Receiving Party in good faith from a third party source having the right to disclose such information, or (iii) was known by the Receiving Party, without any obligation of confidentiality, prior to the disclosure of such information. Notwithstanding anything to the contrary herein, the Receiving Party may disclose Confidential Information to its affiliates and its and their directors, officers, employees,
+30
+attorneys, accountants, agents or advisors who have a need to know such information in the course of the performance of its duties hereunder and are required to comply with the confidentiality obligations under this Section 24, provided, however, that the Receiving Party shall be responsible for the Compliance by the Receiving Party with such obligations. The Receiving Party may disclose Confidential Information to the extent and as required by applicable law or regulation in connection with oral questions, interrogatories, requests for information or documents, subpoena, civil investigative demand, any informal or formal investigation by any regulatory authority to whose jurisdiction Receiving Party is subject, or pursuant to a judicial, administrative or legal proceeding in which either party is involved.
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" s="1" t="n">
+        <v>108</v>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr"/>
+      <c r="D110" t="inlineStr">
+        <is>
+          <t>MISCELLANEOUS</t>
+        </is>
+      </c>
+      <c r="E110" t="inlineStr">
+        <is>
+          <t xml:space="preserve">The Company acknowledges receipt of the following notice:
+" IMPORTANT INFORMATION ABOUT PROCEDURES FOR OPENING A NEW ACCOUNT.
+To help the government fight the funding of terrorism and money laundering activities, Federal law requires all financial institutions to obtain, verify and record information that identifies each person who opens an account. For a non-individual person such as a business entity, a charity, a trust or other legal entity the Custodian will ask for documentation to verify its formation and existence as a legal entity. The Custodian may also ask to see financial statements, licenses, identification and authorization documents from individuals claiming authority to represent the entity or other relevant documentation."
+[PAGE INTENTIONALLY ENDS HERE. SIGNATURE PAGE FOLLOWS.]
+31
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" s="1" t="n">
+        <v>109</v>
+      </c>
+      <c r="B111" t="inlineStr"/>
+      <c r="C111" t="inlineStr"/>
+      <c r="D111" t="inlineStr">
+        <is>
           <t>IN WITNESS WHEREOF</t>
         </is>
       </c>
-      <c r="E31" t="inlineStr">
-        <is>
-          <t xml:space="preserve">, the parties hereto have executed this Agreement as of the date first written above.
-OWL ROCK TECHNOLOGY ADVISORS LLC
-By:
-Name
-Title:
-OWL ROCK TECHNOLOGY FINANCING 2020-1
-By:
+      <c r="E111" t="inlineStr">
+        <is>
+          <t xml:space="preserve">, each of the parties has caused this Agreement to be executed and delivered by a duly authorized officer, intending the same to take effect as of the date first written above.
+PROSPECT FLOATING RATE AND ALTERNATIVE INCOME FUND, INC., as Company
+By: 
 Name:
 Title:
-</t>
+U.S. BANK TRUST COMPANY, NATIONAL ASSOCIATION, as Custodian
+By: 
+Name:
+Title:
+Signature Page to Custody Agreement
+ACTIVE\1602581275.4
+SCHEDULE A
+Any of the following persons (each acting singly) shall be an Authorized Person (as this list may subsequently be modified by the Company from time to time by written notice to the Custodian):
+NAME TITLE SPECIMEN SIGNATURE EMAIL TELEPHONE
+ACTIVE\1602581275.4
+EXHIBIT A
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" s="1" t="n">
+        <v>110</v>
+      </c>
+      <c r="B112" t="inlineStr"/>
+      <c r="C112" t="inlineStr"/>
+      <c r="D112" t="inlineStr">
+        <is>
+          <t>Securities Accounts</t>
+        </is>
+      </c>
+      <c r="E112" t="inlineStr"/>
+    </row>
+    <row r="113">
+      <c r="A113" s="1" t="n">
+        <v>111</v>
+      </c>
+      <c r="B113" t="inlineStr"/>
+      <c r="C113" t="inlineStr"/>
+      <c r="D113" t="inlineStr">
+        <is>
+          <t>Name Number</t>
+        </is>
+      </c>
+      <c r="E113" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Prospect Flt Rate Inc Fund Payment/Custody 224808-200
+Prospect Flt Rate Inc Fund Int Collection 224808-201
+Prospect Flt Rate Inc Fund Prin Collection 224808-202
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" s="1" t="n">
+        <v>112</v>
+      </c>
+      <c r="B114" t="inlineStr"/>
+      <c r="C114" t="inlineStr"/>
+      <c r="D114" t="inlineStr">
+        <is>
+          <t>Subsidiary Accounts</t>
+        </is>
+      </c>
+      <c r="E114" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Prospect Flexible Funding, LLC
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" s="1" t="n">
+        <v>113</v>
+      </c>
+      <c r="B115" t="inlineStr"/>
+      <c r="C115" t="inlineStr"/>
+      <c r="D115" t="inlineStr">
+        <is>
+          <t>Name Number</t>
+        </is>
+      </c>
+      <c r="E115" t="inlineStr">
+        <is>
+          <t>PROSPECT FLEXIBLE FUNDING COLLECTION 191994-200
+PROSPECT FLEXIBLE FUNDING INT CLCTN 191994-201
+PROSPECT FLEXIBLE FUNDING PRN CLCTN 191994-202
+ACTIVE\1602581275.4</t>
         </is>
       </c>
     </row>

</xml_diff>